<commit_message>
feat：update stage excel change
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Stage_关卡表.xlsx
+++ b/nevergiveup/Excel/Stage_关卡表.xlsx
@@ -796,7 +796,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="bottomLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.46484375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1044,7 +1044,9 @@
       <c r="B6" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="D6" s="4" t="s">
         <v>41</v>
       </c>
@@ -1095,7 +1097,9 @@
       <c r="B7" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="D7" s="4" t="s">
         <v>41</v>
       </c>
@@ -1146,7 +1150,9 @@
       <c r="B8" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="D8" s="4" t="s">
         <v>41</v>
       </c>
@@ -1197,7 +1203,9 @@
       <c r="B9" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="D9" s="4" t="s">
         <v>67</v>
       </c>
@@ -1248,7 +1256,9 @@
       <c r="B10" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="D10" s="4" t="s">
         <v>67</v>
       </c>
@@ -1299,7 +1309,9 @@
       <c r="B11" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="D11" s="4" t="s">
         <v>67</v>
       </c>
@@ -1350,6 +1362,9 @@
       <c r="B12" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="C12" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>86</v>
       </c>
@@ -1400,6 +1415,9 @@
       <c r="B13" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="C13" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>86</v>
       </c>
@@ -1450,6 +1468,9 @@
       <c r="B14" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="C14" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>86</v>
       </c>
@@ -1500,6 +1521,9 @@
       <c r="B15" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="C15" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>105</v>
       </c>
@@ -1550,6 +1574,9 @@
       <c r="B16" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="C16" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>105</v>
       </c>
@@ -1600,6 +1627,9 @@
       <c r="B17" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="C17" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>105</v>
       </c>
@@ -1650,6 +1680,9 @@
       <c r="B18" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="C18" s="1" t="n">
+        <v>4</v>
+      </c>
       <c r="D18" s="1" t="s">
         <v>113</v>
       </c>
@@ -1700,6 +1733,9 @@
       <c r="B19" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="C19" s="1" t="n">
+        <v>4</v>
+      </c>
       <c r="D19" s="1" t="s">
         <v>113</v>
       </c>
@@ -1750,6 +1786,9 @@
       <c r="B20" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="C20" s="1" t="n">
+        <v>4</v>
+      </c>
       <c r="D20" s="1" t="s">
         <v>113</v>
       </c>
@@ -1800,7 +1839,9 @@
       <c r="B21" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="C21" s="6"/>
+      <c r="C21" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="D21" s="4" t="s">
         <v>41</v>
       </c>
@@ -1851,7 +1892,9 @@
       <c r="B22" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="C22" s="6"/>
+      <c r="C22" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="D22" s="4" t="s">
         <v>41</v>
       </c>
@@ -1902,7 +1945,9 @@
       <c r="B23" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="D23" s="4" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
feat：update stage excel and ertinity level
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Stage_关卡表.xlsx
+++ b/nevergiveup/Excel/Stage_关卡表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1894" uniqueCount="229">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -695,6 +695,18 @@
   </si>
   <si>
     <t xml:space="preserve">0|0|35.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36DE41A64E48B8A609CB8D836F967CBE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300740.56|101293.78|333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0|0|171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">无尽关卡</t>
   </si>
 </sst>
 </file>
@@ -828,7 +840,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -889,10 +901,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -901,19 +909,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1166,12 +1174,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S170"/>
+  <dimension ref="A1:S171"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E172" activeCellId="0" sqref="E172"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="T174" activeCellId="0" sqref="T174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2325,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" s="14" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="n">
         <v>1004</v>
       </c>
@@ -2875,7 +2883,7 @@
       <c r="F30" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G30" s="16" t="s">
+      <c r="G30" s="15" t="s">
         <v>134</v>
       </c>
       <c r="H30" s="7" t="s">
@@ -2934,7 +2942,7 @@
       <c r="F31" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G31" s="16" t="s">
+      <c r="G31" s="15" t="s">
         <v>134</v>
       </c>
       <c r="H31" s="7" t="s">
@@ -2993,7 +3001,7 @@
       <c r="F32" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="G32" s="15" t="s">
         <v>134</v>
       </c>
       <c r="H32" s="7" t="s">
@@ -3052,7 +3060,7 @@
       <c r="F33" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G33" s="16" t="s">
+      <c r="G33" s="15" t="s">
         <v>136</v>
       </c>
       <c r="H33" s="7" t="s">
@@ -3111,7 +3119,7 @@
       <c r="F34" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G34" s="16" t="s">
+      <c r="G34" s="15" t="s">
         <v>136</v>
       </c>
       <c r="H34" s="7" t="s">
@@ -3170,7 +3178,7 @@
       <c r="F35" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G35" s="16" t="s">
+      <c r="G35" s="15" t="s">
         <v>136</v>
       </c>
       <c r="H35" s="7" t="s">
@@ -3229,7 +3237,7 @@
       <c r="F36" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G36" s="16" t="s">
+      <c r="G36" s="15" t="s">
         <v>138</v>
       </c>
       <c r="H36" s="7" t="s">
@@ -3288,7 +3296,7 @@
       <c r="F37" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G37" s="16" t="s">
+      <c r="G37" s="15" t="s">
         <v>138</v>
       </c>
       <c r="H37" s="7" t="s">
@@ -3347,7 +3355,7 @@
       <c r="F38" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G38" s="16" t="s">
+      <c r="G38" s="15" t="s">
         <v>138</v>
       </c>
       <c r="H38" s="7" t="s">
@@ -3406,7 +3414,7 @@
       <c r="F39" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="G39" s="16" t="s">
+      <c r="G39" s="15" t="s">
         <v>140</v>
       </c>
       <c r="H39" s="7" t="s">
@@ -3465,7 +3473,7 @@
       <c r="F40" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="G40" s="16" t="s">
+      <c r="G40" s="15" t="s">
         <v>140</v>
       </c>
       <c r="H40" s="7" t="s">
@@ -3524,7 +3532,7 @@
       <c r="F41" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="G41" s="16" t="s">
+      <c r="G41" s="15" t="s">
         <v>140</v>
       </c>
       <c r="H41" s="7" t="s">
@@ -3583,7 +3591,7 @@
       <c r="F42" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G42" s="16" t="s">
+      <c r="G42" s="15" t="s">
         <v>142</v>
       </c>
       <c r="H42" s="7" t="s">
@@ -3642,7 +3650,7 @@
       <c r="F43" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G43" s="16" t="s">
+      <c r="G43" s="15" t="s">
         <v>142</v>
       </c>
       <c r="H43" s="7" t="s">
@@ -3701,7 +3709,7 @@
       <c r="F44" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G44" s="16" t="s">
+      <c r="G44" s="15" t="s">
         <v>142</v>
       </c>
       <c r="H44" s="7" t="s">
@@ -3760,7 +3768,7 @@
       <c r="F45" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G45" s="16" t="s">
+      <c r="G45" s="15" t="s">
         <v>144</v>
       </c>
       <c r="H45" s="7" t="s">
@@ -3819,7 +3827,7 @@
       <c r="F46" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G46" s="16" t="s">
+      <c r="G46" s="15" t="s">
         <v>144</v>
       </c>
       <c r="H46" s="7" t="s">
@@ -3878,7 +3886,7 @@
       <c r="F47" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G47" s="16" t="s">
+      <c r="G47" s="15" t="s">
         <v>144</v>
       </c>
       <c r="H47" s="7" t="s">
@@ -3937,7 +3945,7 @@
       <c r="F48" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="G48" s="16" t="s">
+      <c r="G48" s="15" t="s">
         <v>146</v>
       </c>
       <c r="H48" s="7" t="s">
@@ -3996,7 +4004,7 @@
       <c r="F49" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="G49" s="16" t="s">
+      <c r="G49" s="15" t="s">
         <v>146</v>
       </c>
       <c r="H49" s="7" t="s">
@@ -4036,7 +4044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="n">
         <v>1033</v>
       </c>
@@ -4055,7 +4063,7 @@
       <c r="F50" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="G50" s="17" t="s">
+      <c r="G50" s="16" t="s">
         <v>146</v>
       </c>
       <c r="H50" s="12" t="s">
@@ -4111,10 +4119,10 @@
       <c r="E51" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F51" s="18" t="s">
+      <c r="F51" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="G51" s="19" t="s">
+      <c r="G51" s="18" t="s">
         <v>148</v>
       </c>
       <c r="H51" s="7" t="s">
@@ -4151,7 +4159,7 @@
         <v>81</v>
       </c>
       <c r="S51" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4170,10 +4178,10 @@
       <c r="E52" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F52" s="18" t="s">
+      <c r="F52" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="G52" s="19" t="s">
+      <c r="G52" s="18" t="s">
         <v>148</v>
       </c>
       <c r="H52" s="7" t="s">
@@ -4210,7 +4218,7 @@
         <v>86</v>
       </c>
       <c r="S52" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4229,10 +4237,10 @@
       <c r="E53" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="18" t="s">
+      <c r="F53" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="G53" s="19" t="s">
+      <c r="G53" s="18" t="s">
         <v>148</v>
       </c>
       <c r="H53" s="7" t="s">
@@ -4269,7 +4277,7 @@
         <v>91</v>
       </c>
       <c r="S53" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4288,10 +4296,10 @@
       <c r="E54" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F54" s="18" t="s">
+      <c r="F54" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="G54" s="19" t="s">
+      <c r="G54" s="18" t="s">
         <v>150</v>
       </c>
       <c r="H54" s="7" t="s">
@@ -4328,7 +4336,7 @@
         <v>81</v>
       </c>
       <c r="S54" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4347,10 +4355,10 @@
       <c r="E55" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F55" s="18" t="s">
+      <c r="F55" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="G55" s="19" t="s">
+      <c r="G55" s="18" t="s">
         <v>150</v>
       </c>
       <c r="H55" s="7" t="s">
@@ -4387,7 +4395,7 @@
         <v>86</v>
       </c>
       <c r="S55" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4406,10 +4414,10 @@
       <c r="E56" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F56" s="18" t="s">
+      <c r="F56" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="G56" s="19" t="s">
+      <c r="G56" s="18" t="s">
         <v>150</v>
       </c>
       <c r="H56" s="7" t="s">
@@ -4446,7 +4454,7 @@
         <v>91</v>
       </c>
       <c r="S56" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4465,10 +4473,10 @@
       <c r="E57" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F57" s="18" t="s">
+      <c r="F57" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="G57" s="19" t="s">
+      <c r="G57" s="18" t="s">
         <v>152</v>
       </c>
       <c r="H57" s="7" t="s">
@@ -4505,7 +4513,7 @@
         <v>81</v>
       </c>
       <c r="S57" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4524,10 +4532,10 @@
       <c r="E58" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F58" s="18" t="s">
+      <c r="F58" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="G58" s="19" t="s">
+      <c r="G58" s="18" t="s">
         <v>152</v>
       </c>
       <c r="H58" s="7" t="s">
@@ -4564,7 +4572,7 @@
         <v>86</v>
       </c>
       <c r="S58" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4583,10 +4591,10 @@
       <c r="E59" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F59" s="18" t="s">
+      <c r="F59" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="G59" s="19" t="s">
+      <c r="G59" s="18" t="s">
         <v>152</v>
       </c>
       <c r="H59" s="7" t="s">
@@ -4623,7 +4631,7 @@
         <v>91</v>
       </c>
       <c r="S59" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4642,10 +4650,10 @@
       <c r="E60" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F60" s="18" t="s">
+      <c r="F60" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="G60" s="19" t="s">
+      <c r="G60" s="18" t="s">
         <v>154</v>
       </c>
       <c r="H60" s="7" t="s">
@@ -4682,7 +4690,7 @@
         <v>81</v>
       </c>
       <c r="S60" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4701,10 +4709,10 @@
       <c r="E61" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F61" s="18" t="s">
+      <c r="F61" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="G61" s="19" t="s">
+      <c r="G61" s="18" t="s">
         <v>154</v>
       </c>
       <c r="H61" s="7" t="s">
@@ -4741,7 +4749,7 @@
         <v>86</v>
       </c>
       <c r="S61" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4760,10 +4768,10 @@
       <c r="E62" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F62" s="18" t="s">
+      <c r="F62" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="G62" s="19" t="s">
+      <c r="G62" s="18" t="s">
         <v>154</v>
       </c>
       <c r="H62" s="7" t="s">
@@ -4800,7 +4808,7 @@
         <v>91</v>
       </c>
       <c r="S62" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4819,10 +4827,10 @@
       <c r="E63" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F63" s="18" t="s">
+      <c r="F63" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="G63" s="19" t="s">
+      <c r="G63" s="18" t="s">
         <v>156</v>
       </c>
       <c r="H63" s="7" t="s">
@@ -4859,7 +4867,7 @@
         <v>81</v>
       </c>
       <c r="S63" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4878,10 +4886,10 @@
       <c r="E64" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F64" s="18" t="s">
+      <c r="F64" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="G64" s="19" t="s">
+      <c r="G64" s="18" t="s">
         <v>156</v>
       </c>
       <c r="H64" s="7" t="s">
@@ -4918,7 +4926,7 @@
         <v>86</v>
       </c>
       <c r="S64" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4937,10 +4945,10 @@
       <c r="E65" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F65" s="18" t="s">
+      <c r="F65" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="G65" s="19" t="s">
+      <c r="G65" s="18" t="s">
         <v>156</v>
       </c>
       <c r="H65" s="7" t="s">
@@ -4977,7 +4985,7 @@
         <v>91</v>
       </c>
       <c r="S65" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4996,10 +5004,10 @@
       <c r="E66" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F66" s="18" t="s">
+      <c r="F66" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="G66" s="19" t="s">
+      <c r="G66" s="18" t="s">
         <v>158</v>
       </c>
       <c r="H66" s="7" t="s">
@@ -5036,7 +5044,7 @@
         <v>81</v>
       </c>
       <c r="S66" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5055,10 +5063,10 @@
       <c r="E67" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F67" s="18" t="s">
+      <c r="F67" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="G67" s="19" t="s">
+      <c r="G67" s="18" t="s">
         <v>158</v>
       </c>
       <c r="H67" s="7" t="s">
@@ -5095,7 +5103,7 @@
         <v>86</v>
       </c>
       <c r="S67" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5114,10 +5122,10 @@
       <c r="E68" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F68" s="18" t="s">
+      <c r="F68" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="G68" s="19" t="s">
+      <c r="G68" s="18" t="s">
         <v>158</v>
       </c>
       <c r="H68" s="7" t="s">
@@ -5154,7 +5162,7 @@
         <v>91</v>
       </c>
       <c r="S68" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5173,10 +5181,10 @@
       <c r="E69" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F69" s="18" t="s">
+      <c r="F69" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="G69" s="19" t="s">
+      <c r="G69" s="18" t="s">
         <v>160</v>
       </c>
       <c r="H69" s="7" t="s">
@@ -5213,7 +5221,7 @@
         <v>81</v>
       </c>
       <c r="S69" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5232,10 +5240,10 @@
       <c r="E70" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F70" s="18" t="s">
+      <c r="F70" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="G70" s="19" t="s">
+      <c r="G70" s="18" t="s">
         <v>160</v>
       </c>
       <c r="H70" s="7" t="s">
@@ -5272,7 +5280,7 @@
         <v>86</v>
       </c>
       <c r="S70" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5291,10 +5299,10 @@
       <c r="E71" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F71" s="18" t="s">
+      <c r="F71" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="G71" s="19" t="s">
+      <c r="G71" s="18" t="s">
         <v>160</v>
       </c>
       <c r="H71" s="7" t="s">
@@ -5331,7 +5339,7 @@
         <v>91</v>
       </c>
       <c r="S71" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5350,10 +5358,10 @@
       <c r="E72" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F72" s="18" t="s">
+      <c r="F72" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="G72" s="19" t="s">
+      <c r="G72" s="18" t="s">
         <v>162</v>
       </c>
       <c r="H72" s="7" t="s">
@@ -5390,7 +5398,7 @@
         <v>81</v>
       </c>
       <c r="S72" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5409,10 +5417,10 @@
       <c r="E73" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F73" s="18" t="s">
+      <c r="F73" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="G73" s="19" t="s">
+      <c r="G73" s="18" t="s">
         <v>162</v>
       </c>
       <c r="H73" s="7" t="s">
@@ -5449,7 +5457,7 @@
         <v>86</v>
       </c>
       <c r="S73" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5468,10 +5476,10 @@
       <c r="E74" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F74" s="18" t="s">
+      <c r="F74" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="G74" s="19" t="s">
+      <c r="G74" s="18" t="s">
         <v>162</v>
       </c>
       <c r="H74" s="7" t="s">
@@ -5508,7 +5516,7 @@
         <v>91</v>
       </c>
       <c r="S74" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5527,10 +5535,10 @@
       <c r="E75" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F75" s="18" t="s">
+      <c r="F75" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="G75" s="19" t="s">
+      <c r="G75" s="18" t="s">
         <v>164</v>
       </c>
       <c r="H75" s="7" t="s">
@@ -5567,7 +5575,7 @@
         <v>81</v>
       </c>
       <c r="S75" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5586,10 +5594,10 @@
       <c r="E76" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F76" s="18" t="s">
+      <c r="F76" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="G76" s="19" t="s">
+      <c r="G76" s="18" t="s">
         <v>164</v>
       </c>
       <c r="H76" s="7" t="s">
@@ -5626,7 +5634,7 @@
         <v>86</v>
       </c>
       <c r="S76" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5645,10 +5653,10 @@
       <c r="E77" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F77" s="18" t="s">
+      <c r="F77" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="G77" s="19" t="s">
+      <c r="G77" s="18" t="s">
         <v>164</v>
       </c>
       <c r="H77" s="7" t="s">
@@ -5685,7 +5693,7 @@
         <v>91</v>
       </c>
       <c r="S77" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5704,10 +5712,10 @@
       <c r="E78" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F78" s="18" t="s">
+      <c r="F78" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="G78" s="19" t="s">
+      <c r="G78" s="18" t="s">
         <v>65</v>
       </c>
       <c r="H78" s="7" t="s">
@@ -5744,7 +5752,7 @@
         <v>81</v>
       </c>
       <c r="S78" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5763,10 +5771,10 @@
       <c r="E79" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F79" s="18" t="s">
+      <c r="F79" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="G79" s="19" t="s">
+      <c r="G79" s="18" t="s">
         <v>65</v>
       </c>
       <c r="H79" s="7" t="s">
@@ -5803,10 +5811,10 @@
         <v>86</v>
       </c>
       <c r="S79" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" s="14" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="9" t="n">
         <v>2033</v>
       </c>
@@ -5822,10 +5830,10 @@
       <c r="E80" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F80" s="20" t="s">
+      <c r="F80" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="G80" s="21" t="s">
+      <c r="G80" s="20" t="s">
         <v>65</v>
       </c>
       <c r="H80" s="12" t="s">
@@ -5862,7 +5870,7 @@
         <v>91</v>
       </c>
       <c r="S80" s="14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5881,10 +5889,10 @@
       <c r="E81" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F81" s="18" t="s">
+      <c r="F81" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="G81" s="19" t="s">
+      <c r="G81" s="18" t="s">
         <v>167</v>
       </c>
       <c r="H81" s="7" t="s">
@@ -5921,7 +5929,7 @@
         <v>98</v>
       </c>
       <c r="S81" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5940,10 +5948,10 @@
       <c r="E82" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F82" s="18" t="s">
+      <c r="F82" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="G82" s="19" t="s">
+      <c r="G82" s="18" t="s">
         <v>167</v>
       </c>
       <c r="H82" s="7" t="s">
@@ -5980,7 +5988,7 @@
         <v>103</v>
       </c>
       <c r="S82" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5999,10 +6007,10 @@
       <c r="E83" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F83" s="18" t="s">
+      <c r="F83" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="G83" s="19" t="s">
+      <c r="G83" s="18" t="s">
         <v>167</v>
       </c>
       <c r="H83" s="7" t="s">
@@ -6039,7 +6047,7 @@
         <v>110</v>
       </c>
       <c r="S83" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6058,10 +6066,10 @@
       <c r="E84" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F84" s="18" t="s">
+      <c r="F84" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="G84" s="19" t="s">
+      <c r="G84" s="18" t="s">
         <v>169</v>
       </c>
       <c r="H84" s="7" t="s">
@@ -6098,7 +6106,7 @@
         <v>98</v>
       </c>
       <c r="S84" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6117,10 +6125,10 @@
       <c r="E85" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F85" s="18" t="s">
+      <c r="F85" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="G85" s="19" t="s">
+      <c r="G85" s="18" t="s">
         <v>169</v>
       </c>
       <c r="H85" s="7" t="s">
@@ -6157,7 +6165,7 @@
         <v>103</v>
       </c>
       <c r="S85" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6176,10 +6184,10 @@
       <c r="E86" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F86" s="18" t="s">
+      <c r="F86" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="G86" s="19" t="s">
+      <c r="G86" s="18" t="s">
         <v>169</v>
       </c>
       <c r="H86" s="7" t="s">
@@ -6216,7 +6224,7 @@
         <v>110</v>
       </c>
       <c r="S86" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6235,10 +6243,10 @@
       <c r="E87" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F87" s="18" t="s">
+      <c r="F87" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="G87" s="19" t="s">
+      <c r="G87" s="18" t="s">
         <v>171</v>
       </c>
       <c r="H87" s="7" t="s">
@@ -6275,7 +6283,7 @@
         <v>98</v>
       </c>
       <c r="S87" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6294,10 +6302,10 @@
       <c r="E88" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F88" s="18" t="s">
+      <c r="F88" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="G88" s="19" t="s">
+      <c r="G88" s="18" t="s">
         <v>171</v>
       </c>
       <c r="H88" s="7" t="s">
@@ -6334,7 +6342,7 @@
         <v>103</v>
       </c>
       <c r="S88" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6353,10 +6361,10 @@
       <c r="E89" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F89" s="18" t="s">
+      <c r="F89" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="G89" s="19" t="s">
+      <c r="G89" s="18" t="s">
         <v>171</v>
       </c>
       <c r="H89" s="7" t="s">
@@ -6393,7 +6401,7 @@
         <v>110</v>
       </c>
       <c r="S89" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6412,10 +6420,10 @@
       <c r="E90" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F90" s="18" t="s">
+      <c r="F90" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="G90" s="19" t="s">
+      <c r="G90" s="18" t="s">
         <v>173</v>
       </c>
       <c r="H90" s="7" t="s">
@@ -6452,7 +6460,7 @@
         <v>98</v>
       </c>
       <c r="S90" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6471,10 +6479,10 @@
       <c r="E91" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F91" s="18" t="s">
+      <c r="F91" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="G91" s="19" t="s">
+      <c r="G91" s="18" t="s">
         <v>173</v>
       </c>
       <c r="H91" s="7" t="s">
@@ -6511,7 +6519,7 @@
         <v>103</v>
       </c>
       <c r="S91" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6530,10 +6538,10 @@
       <c r="E92" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F92" s="18" t="s">
+      <c r="F92" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="G92" s="19" t="s">
+      <c r="G92" s="18" t="s">
         <v>173</v>
       </c>
       <c r="H92" s="7" t="s">
@@ -6570,7 +6578,7 @@
         <v>110</v>
       </c>
       <c r="S92" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6589,10 +6597,10 @@
       <c r="E93" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F93" s="18" t="s">
+      <c r="F93" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="G93" s="19" t="s">
+      <c r="G93" s="18" t="s">
         <v>175</v>
       </c>
       <c r="H93" s="7" t="s">
@@ -6629,7 +6637,7 @@
         <v>98</v>
       </c>
       <c r="S93" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6648,10 +6656,10 @@
       <c r="E94" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F94" s="18" t="s">
+      <c r="F94" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="G94" s="19" t="s">
+      <c r="G94" s="18" t="s">
         <v>175</v>
       </c>
       <c r="H94" s="7" t="s">
@@ -6688,7 +6696,7 @@
         <v>103</v>
       </c>
       <c r="S94" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6707,10 +6715,10 @@
       <c r="E95" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F95" s="18" t="s">
+      <c r="F95" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="G95" s="19" t="s">
+      <c r="G95" s="18" t="s">
         <v>175</v>
       </c>
       <c r="H95" s="7" t="s">
@@ -6747,7 +6755,7 @@
         <v>110</v>
       </c>
       <c r="S95" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6766,10 +6774,10 @@
       <c r="E96" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F96" s="18" t="s">
+      <c r="F96" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="G96" s="19" t="s">
+      <c r="G96" s="18" t="s">
         <v>177</v>
       </c>
       <c r="H96" s="7" t="s">
@@ -6806,7 +6814,7 @@
         <v>98</v>
       </c>
       <c r="S96" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6825,10 +6833,10 @@
       <c r="E97" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F97" s="18" t="s">
+      <c r="F97" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="G97" s="19" t="s">
+      <c r="G97" s="18" t="s">
         <v>177</v>
       </c>
       <c r="H97" s="7" t="s">
@@ -6865,7 +6873,7 @@
         <v>103</v>
       </c>
       <c r="S97" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6884,10 +6892,10 @@
       <c r="E98" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F98" s="18" t="s">
+      <c r="F98" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="G98" s="19" t="s">
+      <c r="G98" s="18" t="s">
         <v>177</v>
       </c>
       <c r="H98" s="7" t="s">
@@ -6924,7 +6932,7 @@
         <v>110</v>
       </c>
       <c r="S98" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6943,10 +6951,10 @@
       <c r="E99" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F99" s="18" t="s">
+      <c r="F99" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="G99" s="19" t="s">
+      <c r="G99" s="18" t="s">
         <v>179</v>
       </c>
       <c r="H99" s="7" t="s">
@@ -6983,7 +6991,7 @@
         <v>98</v>
       </c>
       <c r="S99" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7002,10 +7010,10 @@
       <c r="E100" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F100" s="18" t="s">
+      <c r="F100" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="G100" s="19" t="s">
+      <c r="G100" s="18" t="s">
         <v>179</v>
       </c>
       <c r="H100" s="7" t="s">
@@ -7042,7 +7050,7 @@
         <v>103</v>
       </c>
       <c r="S100" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7061,10 +7069,10 @@
       <c r="E101" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F101" s="18" t="s">
+      <c r="F101" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="G101" s="19" t="s">
+      <c r="G101" s="18" t="s">
         <v>179</v>
       </c>
       <c r="H101" s="7" t="s">
@@ -7101,7 +7109,7 @@
         <v>110</v>
       </c>
       <c r="S101" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7120,10 +7128,10 @@
       <c r="E102" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F102" s="18" t="s">
+      <c r="F102" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="G102" s="19" t="s">
+      <c r="G102" s="18" t="s">
         <v>181</v>
       </c>
       <c r="H102" s="7" t="s">
@@ -7160,7 +7168,7 @@
         <v>98</v>
       </c>
       <c r="S102" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7179,10 +7187,10 @@
       <c r="E103" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F103" s="18" t="s">
+      <c r="F103" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="G103" s="19" t="s">
+      <c r="G103" s="18" t="s">
         <v>181</v>
       </c>
       <c r="H103" s="7" t="s">
@@ -7219,7 +7227,7 @@
         <v>103</v>
       </c>
       <c r="S103" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7238,10 +7246,10 @@
       <c r="E104" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F104" s="18" t="s">
+      <c r="F104" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="G104" s="19" t="s">
+      <c r="G104" s="18" t="s">
         <v>181</v>
       </c>
       <c r="H104" s="7" t="s">
@@ -7278,7 +7286,7 @@
         <v>110</v>
       </c>
       <c r="S104" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7297,10 +7305,10 @@
       <c r="E105" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F105" s="18" t="s">
+      <c r="F105" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="G105" s="19" t="s">
+      <c r="G105" s="18" t="s">
         <v>183</v>
       </c>
       <c r="H105" s="7" t="s">
@@ -7337,7 +7345,7 @@
         <v>98</v>
       </c>
       <c r="S105" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7356,10 +7364,10 @@
       <c r="E106" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F106" s="18" t="s">
+      <c r="F106" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="G106" s="19" t="s">
+      <c r="G106" s="18" t="s">
         <v>183</v>
       </c>
       <c r="H106" s="7" t="s">
@@ -7396,7 +7404,7 @@
         <v>103</v>
       </c>
       <c r="S106" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7415,10 +7423,10 @@
       <c r="E107" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F107" s="18" t="s">
+      <c r="F107" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="G107" s="19" t="s">
+      <c r="G107" s="18" t="s">
         <v>183</v>
       </c>
       <c r="H107" s="7" t="s">
@@ -7455,7 +7463,7 @@
         <v>110</v>
       </c>
       <c r="S107" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7474,10 +7482,10 @@
       <c r="E108" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F108" s="18" t="s">
+      <c r="F108" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="G108" s="19" t="s">
+      <c r="G108" s="18" t="s">
         <v>185</v>
       </c>
       <c r="H108" s="7" t="s">
@@ -7514,7 +7522,7 @@
         <v>98</v>
       </c>
       <c r="S108" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7533,10 +7541,10 @@
       <c r="E109" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F109" s="18" t="s">
+      <c r="F109" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="G109" s="19" t="s">
+      <c r="G109" s="18" t="s">
         <v>185</v>
       </c>
       <c r="H109" s="7" t="s">
@@ -7573,10 +7581,10 @@
         <v>103</v>
       </c>
       <c r="S109" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" s="15" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" s="14" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="14" t="n">
         <v>3033</v>
       </c>
@@ -7592,10 +7600,10 @@
       <c r="E110" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F110" s="20" t="s">
+      <c r="F110" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="G110" s="21" t="s">
+      <c r="G110" s="20" t="s">
         <v>185</v>
       </c>
       <c r="H110" s="12" t="s">
@@ -7632,7 +7640,7 @@
         <v>110</v>
       </c>
       <c r="S110" s="14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7651,10 +7659,10 @@
       <c r="E111" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F111" s="18" t="s">
+      <c r="F111" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="G111" s="19" t="s">
+      <c r="G111" s="18" t="s">
         <v>187</v>
       </c>
       <c r="H111" s="7" t="s">
@@ -7691,7 +7699,7 @@
         <v>98</v>
       </c>
       <c r="S111" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7710,10 +7718,10 @@
       <c r="E112" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F112" s="18" t="s">
+      <c r="F112" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="G112" s="19" t="s">
+      <c r="G112" s="18" t="s">
         <v>187</v>
       </c>
       <c r="H112" s="7" t="s">
@@ -7750,7 +7758,7 @@
         <v>103</v>
       </c>
       <c r="S112" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7769,10 +7777,10 @@
       <c r="E113" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F113" s="18" t="s">
+      <c r="F113" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="G113" s="19" t="s">
+      <c r="G113" s="18" t="s">
         <v>187</v>
       </c>
       <c r="H113" s="7" t="s">
@@ -7809,7 +7817,7 @@
         <v>110</v>
       </c>
       <c r="S113" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7828,10 +7836,10 @@
       <c r="E114" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F114" s="18" t="s">
+      <c r="F114" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="G114" s="19" t="s">
+      <c r="G114" s="18" t="s">
         <v>189</v>
       </c>
       <c r="H114" s="7" t="s">
@@ -7868,7 +7876,7 @@
         <v>98</v>
       </c>
       <c r="S114" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7887,10 +7895,10 @@
       <c r="E115" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F115" s="18" t="s">
+      <c r="F115" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="G115" s="19" t="s">
+      <c r="G115" s="18" t="s">
         <v>189</v>
       </c>
       <c r="H115" s="7" t="s">
@@ -7927,7 +7935,7 @@
         <v>103</v>
       </c>
       <c r="S115" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7946,10 +7954,10 @@
       <c r="E116" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F116" s="18" t="s">
+      <c r="F116" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="G116" s="19" t="s">
+      <c r="G116" s="18" t="s">
         <v>189</v>
       </c>
       <c r="H116" s="7" t="s">
@@ -7986,7 +7994,7 @@
         <v>110</v>
       </c>
       <c r="S116" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8005,10 +8013,10 @@
       <c r="E117" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F117" s="18" t="s">
+      <c r="F117" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="G117" s="19" t="s">
+      <c r="G117" s="18" t="s">
         <v>191</v>
       </c>
       <c r="H117" s="7" t="s">
@@ -8045,7 +8053,7 @@
         <v>98</v>
       </c>
       <c r="S117" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8064,10 +8072,10 @@
       <c r="E118" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F118" s="18" t="s">
+      <c r="F118" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="G118" s="19" t="s">
+      <c r="G118" s="18" t="s">
         <v>191</v>
       </c>
       <c r="H118" s="7" t="s">
@@ -8104,7 +8112,7 @@
         <v>103</v>
       </c>
       <c r="S118" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8123,10 +8131,10 @@
       <c r="E119" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F119" s="18" t="s">
+      <c r="F119" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="G119" s="19" t="s">
+      <c r="G119" s="18" t="s">
         <v>191</v>
       </c>
       <c r="H119" s="7" t="s">
@@ -8163,7 +8171,7 @@
         <v>110</v>
       </c>
       <c r="S119" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8182,10 +8190,10 @@
       <c r="E120" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F120" s="18" t="s">
+      <c r="F120" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="G120" s="19" t="s">
+      <c r="G120" s="18" t="s">
         <v>193</v>
       </c>
       <c r="H120" s="7" t="s">
@@ -8222,7 +8230,7 @@
         <v>98</v>
       </c>
       <c r="S120" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8241,10 +8249,10 @@
       <c r="E121" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F121" s="18" t="s">
+      <c r="F121" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="G121" s="19" t="s">
+      <c r="G121" s="18" t="s">
         <v>193</v>
       </c>
       <c r="H121" s="7" t="s">
@@ -8281,7 +8289,7 @@
         <v>103</v>
       </c>
       <c r="S121" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8300,10 +8308,10 @@
       <c r="E122" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F122" s="18" t="s">
+      <c r="F122" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="G122" s="19" t="s">
+      <c r="G122" s="18" t="s">
         <v>193</v>
       </c>
       <c r="H122" s="7" t="s">
@@ -8340,7 +8348,7 @@
         <v>110</v>
       </c>
       <c r="S122" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8359,10 +8367,10 @@
       <c r="E123" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F123" s="18" t="s">
+      <c r="F123" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="G123" s="19" t="s">
+      <c r="G123" s="18" t="s">
         <v>195</v>
       </c>
       <c r="H123" s="7" t="s">
@@ -8399,7 +8407,7 @@
         <v>98</v>
       </c>
       <c r="S123" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8418,10 +8426,10 @@
       <c r="E124" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F124" s="18" t="s">
+      <c r="F124" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="G124" s="19" t="s">
+      <c r="G124" s="18" t="s">
         <v>195</v>
       </c>
       <c r="H124" s="7" t="s">
@@ -8458,7 +8466,7 @@
         <v>103</v>
       </c>
       <c r="S124" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8477,10 +8485,10 @@
       <c r="E125" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F125" s="18" t="s">
+      <c r="F125" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="G125" s="19" t="s">
+      <c r="G125" s="18" t="s">
         <v>195</v>
       </c>
       <c r="H125" s="7" t="s">
@@ -8517,7 +8525,7 @@
         <v>110</v>
       </c>
       <c r="S125" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8536,10 +8544,10 @@
       <c r="E126" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F126" s="18" t="s">
+      <c r="F126" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="G126" s="19" t="s">
+      <c r="G126" s="18" t="s">
         <v>197</v>
       </c>
       <c r="H126" s="7" t="s">
@@ -8576,7 +8584,7 @@
         <v>98</v>
       </c>
       <c r="S126" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8595,10 +8603,10 @@
       <c r="E127" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F127" s="18" t="s">
+      <c r="F127" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="G127" s="19" t="s">
+      <c r="G127" s="18" t="s">
         <v>197</v>
       </c>
       <c r="H127" s="7" t="s">
@@ -8635,7 +8643,7 @@
         <v>103</v>
       </c>
       <c r="S127" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8654,10 +8662,10 @@
       <c r="E128" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F128" s="18" t="s">
+      <c r="F128" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="G128" s="19" t="s">
+      <c r="G128" s="18" t="s">
         <v>197</v>
       </c>
       <c r="H128" s="7" t="s">
@@ -8694,7 +8702,7 @@
         <v>110</v>
       </c>
       <c r="S128" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8713,10 +8721,10 @@
       <c r="E129" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F129" s="18" t="s">
+      <c r="F129" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="G129" s="19" t="s">
+      <c r="G129" s="18" t="s">
         <v>199</v>
       </c>
       <c r="H129" s="7" t="s">
@@ -8753,7 +8761,7 @@
         <v>98</v>
       </c>
       <c r="S129" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8772,10 +8780,10 @@
       <c r="E130" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F130" s="18" t="s">
+      <c r="F130" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="G130" s="19" t="s">
+      <c r="G130" s="18" t="s">
         <v>199</v>
       </c>
       <c r="H130" s="7" t="s">
@@ -8812,7 +8820,7 @@
         <v>103</v>
       </c>
       <c r="S130" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8831,10 +8839,10 @@
       <c r="E131" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F131" s="18" t="s">
+      <c r="F131" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="G131" s="19" t="s">
+      <c r="G131" s="18" t="s">
         <v>199</v>
       </c>
       <c r="H131" s="7" t="s">
@@ -8871,7 +8879,7 @@
         <v>110</v>
       </c>
       <c r="S131" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8890,10 +8898,10 @@
       <c r="E132" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F132" s="18" t="s">
+      <c r="F132" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="G132" s="19" t="s">
+      <c r="G132" s="18" t="s">
         <v>201</v>
       </c>
       <c r="H132" s="7" t="s">
@@ -8930,7 +8938,7 @@
         <v>98</v>
       </c>
       <c r="S132" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8949,10 +8957,10 @@
       <c r="E133" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F133" s="18" t="s">
+      <c r="F133" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="G133" s="19" t="s">
+      <c r="G133" s="18" t="s">
         <v>201</v>
       </c>
       <c r="H133" s="7" t="s">
@@ -8989,7 +8997,7 @@
         <v>103</v>
       </c>
       <c r="S133" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9008,10 +9016,10 @@
       <c r="E134" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F134" s="18" t="s">
+      <c r="F134" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="G134" s="19" t="s">
+      <c r="G134" s="18" t="s">
         <v>201</v>
       </c>
       <c r="H134" s="7" t="s">
@@ -9048,7 +9056,7 @@
         <v>110</v>
       </c>
       <c r="S134" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9067,10 +9075,10 @@
       <c r="E135" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F135" s="18" t="s">
+      <c r="F135" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="G135" s="19" t="s">
+      <c r="G135" s="18" t="s">
         <v>203</v>
       </c>
       <c r="H135" s="7" t="s">
@@ -9107,7 +9115,7 @@
         <v>98</v>
       </c>
       <c r="S135" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9126,10 +9134,10 @@
       <c r="E136" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F136" s="18" t="s">
+      <c r="F136" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="G136" s="19" t="s">
+      <c r="G136" s="18" t="s">
         <v>203</v>
       </c>
       <c r="H136" s="7" t="s">
@@ -9166,7 +9174,7 @@
         <v>103</v>
       </c>
       <c r="S136" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9185,10 +9193,10 @@
       <c r="E137" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F137" s="18" t="s">
+      <c r="F137" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="G137" s="19" t="s">
+      <c r="G137" s="18" t="s">
         <v>203</v>
       </c>
       <c r="H137" s="7" t="s">
@@ -9225,7 +9233,7 @@
         <v>110</v>
       </c>
       <c r="S137" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9244,10 +9252,10 @@
       <c r="E138" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F138" s="18" t="s">
+      <c r="F138" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="G138" s="19" t="s">
+      <c r="G138" s="18" t="s">
         <v>205</v>
       </c>
       <c r="H138" s="7" t="s">
@@ -9284,7 +9292,7 @@
         <v>98</v>
       </c>
       <c r="S138" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9303,10 +9311,10 @@
       <c r="E139" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F139" s="18" t="s">
+      <c r="F139" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="G139" s="19" t="s">
+      <c r="G139" s="18" t="s">
         <v>205</v>
       </c>
       <c r="H139" s="7" t="s">
@@ -9343,10 +9351,10 @@
         <v>103</v>
       </c>
       <c r="S139" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" s="15" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" s="14" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="14" t="n">
         <v>4033</v>
       </c>
@@ -9362,10 +9370,10 @@
       <c r="E140" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F140" s="20" t="s">
+      <c r="F140" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="G140" s="21" t="s">
+      <c r="G140" s="20" t="s">
         <v>205</v>
       </c>
       <c r="H140" s="12" t="s">
@@ -9402,7 +9410,7 @@
         <v>110</v>
       </c>
       <c r="S140" s="14" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9421,10 +9429,10 @@
       <c r="E141" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F141" s="18" t="s">
+      <c r="F141" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="G141" s="19" t="s">
+      <c r="G141" s="18" t="s">
         <v>207</v>
       </c>
       <c r="H141" s="7" t="s">
@@ -9461,7 +9469,7 @@
         <v>98</v>
       </c>
       <c r="S141" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9480,10 +9488,10 @@
       <c r="E142" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F142" s="18" t="s">
+      <c r="F142" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="G142" s="19" t="s">
+      <c r="G142" s="18" t="s">
         <v>207</v>
       </c>
       <c r="H142" s="7" t="s">
@@ -9520,7 +9528,7 @@
         <v>103</v>
       </c>
       <c r="S142" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9539,10 +9547,10 @@
       <c r="E143" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F143" s="18" t="s">
+      <c r="F143" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="G143" s="19" t="s">
+      <c r="G143" s="18" t="s">
         <v>207</v>
       </c>
       <c r="H143" s="7" t="s">
@@ -9579,7 +9587,7 @@
         <v>110</v>
       </c>
       <c r="S143" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9598,10 +9606,10 @@
       <c r="E144" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F144" s="18" t="s">
+      <c r="F144" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="G144" s="19" t="s">
+      <c r="G144" s="18" t="s">
         <v>209</v>
       </c>
       <c r="H144" s="7" t="s">
@@ -9638,7 +9646,7 @@
         <v>98</v>
       </c>
       <c r="S144" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9657,10 +9665,10 @@
       <c r="E145" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F145" s="18" t="s">
+      <c r="F145" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="G145" s="19" t="s">
+      <c r="G145" s="18" t="s">
         <v>209</v>
       </c>
       <c r="H145" s="7" t="s">
@@ -9697,7 +9705,7 @@
         <v>103</v>
       </c>
       <c r="S145" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9716,10 +9724,10 @@
       <c r="E146" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F146" s="18" t="s">
+      <c r="F146" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="G146" s="19" t="s">
+      <c r="G146" s="18" t="s">
         <v>209</v>
       </c>
       <c r="H146" s="7" t="s">
@@ -9756,7 +9764,7 @@
         <v>110</v>
       </c>
       <c r="S146" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9775,10 +9783,10 @@
       <c r="E147" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F147" s="18" t="s">
+      <c r="F147" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G147" s="19" t="s">
+      <c r="G147" s="18" t="s">
         <v>211</v>
       </c>
       <c r="H147" s="7" t="s">
@@ -9815,7 +9823,7 @@
         <v>98</v>
       </c>
       <c r="S147" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9834,10 +9842,10 @@
       <c r="E148" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F148" s="18" t="s">
+      <c r="F148" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G148" s="19" t="s">
+      <c r="G148" s="18" t="s">
         <v>211</v>
       </c>
       <c r="H148" s="7" t="s">
@@ -9874,7 +9882,7 @@
         <v>103</v>
       </c>
       <c r="S148" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9893,10 +9901,10 @@
       <c r="E149" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F149" s="18" t="s">
+      <c r="F149" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G149" s="19" t="s">
+      <c r="G149" s="18" t="s">
         <v>211</v>
       </c>
       <c r="H149" s="7" t="s">
@@ -9933,7 +9941,7 @@
         <v>110</v>
       </c>
       <c r="S149" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9952,10 +9960,10 @@
       <c r="E150" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F150" s="18" t="s">
+      <c r="F150" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="G150" s="19" t="s">
+      <c r="G150" s="18" t="s">
         <v>213</v>
       </c>
       <c r="H150" s="7" t="s">
@@ -9992,7 +10000,7 @@
         <v>98</v>
       </c>
       <c r="S150" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10011,10 +10019,10 @@
       <c r="E151" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F151" s="18" t="s">
+      <c r="F151" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="G151" s="19" t="s">
+      <c r="G151" s="18" t="s">
         <v>213</v>
       </c>
       <c r="H151" s="7" t="s">
@@ -10051,7 +10059,7 @@
         <v>103</v>
       </c>
       <c r="S151" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10070,10 +10078,10 @@
       <c r="E152" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F152" s="18" t="s">
+      <c r="F152" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="G152" s="19" t="s">
+      <c r="G152" s="18" t="s">
         <v>213</v>
       </c>
       <c r="H152" s="7" t="s">
@@ -10110,7 +10118,7 @@
         <v>110</v>
       </c>
       <c r="S152" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10129,10 +10137,10 @@
       <c r="E153" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F153" s="18" t="s">
+      <c r="F153" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="G153" s="19" t="s">
+      <c r="G153" s="18" t="s">
         <v>215</v>
       </c>
       <c r="H153" s="7" t="s">
@@ -10169,7 +10177,7 @@
         <v>98</v>
       </c>
       <c r="S153" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10188,10 +10196,10 @@
       <c r="E154" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F154" s="18" t="s">
+      <c r="F154" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="G154" s="19" t="s">
+      <c r="G154" s="18" t="s">
         <v>215</v>
       </c>
       <c r="H154" s="7" t="s">
@@ -10228,7 +10236,7 @@
         <v>103</v>
       </c>
       <c r="S154" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10247,10 +10255,10 @@
       <c r="E155" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F155" s="18" t="s">
+      <c r="F155" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="G155" s="19" t="s">
+      <c r="G155" s="18" t="s">
         <v>215</v>
       </c>
       <c r="H155" s="7" t="s">
@@ -10287,7 +10295,7 @@
         <v>110</v>
       </c>
       <c r="S155" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10306,10 +10314,10 @@
       <c r="E156" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F156" s="18" t="s">
+      <c r="F156" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="G156" s="18" t="s">
+      <c r="G156" s="17" t="s">
         <v>217</v>
       </c>
       <c r="H156" s="7" t="s">
@@ -10346,7 +10354,7 @@
         <v>98</v>
       </c>
       <c r="S156" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10365,10 +10373,10 @@
       <c r="E157" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F157" s="18" t="s">
+      <c r="F157" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="G157" s="18" t="s">
+      <c r="G157" s="17" t="s">
         <v>217</v>
       </c>
       <c r="H157" s="7" t="s">
@@ -10405,7 +10413,7 @@
         <v>103</v>
       </c>
       <c r="S157" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10424,10 +10432,10 @@
       <c r="E158" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F158" s="18" t="s">
+      <c r="F158" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="G158" s="18" t="s">
+      <c r="G158" s="17" t="s">
         <v>217</v>
       </c>
       <c r="H158" s="7" t="s">
@@ -10464,7 +10472,7 @@
         <v>110</v>
       </c>
       <c r="S158" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10483,10 +10491,10 @@
       <c r="E159" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F159" s="18" t="s">
+      <c r="F159" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="G159" s="18" t="s">
+      <c r="G159" s="17" t="s">
         <v>219</v>
       </c>
       <c r="H159" s="7" t="s">
@@ -10523,7 +10531,7 @@
         <v>98</v>
       </c>
       <c r="S159" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10542,10 +10550,10 @@
       <c r="E160" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F160" s="18" t="s">
+      <c r="F160" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="G160" s="18" t="s">
+      <c r="G160" s="17" t="s">
         <v>219</v>
       </c>
       <c r="H160" s="7" t="s">
@@ -10582,7 +10590,7 @@
         <v>103</v>
       </c>
       <c r="S160" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10601,10 +10609,10 @@
       <c r="E161" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F161" s="18" t="s">
+      <c r="F161" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="G161" s="18" t="s">
+      <c r="G161" s="17" t="s">
         <v>219</v>
       </c>
       <c r="H161" s="7" t="s">
@@ -10641,7 +10649,7 @@
         <v>110</v>
       </c>
       <c r="S161" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10660,10 +10668,10 @@
       <c r="E162" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F162" s="18" t="s">
+      <c r="F162" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="G162" s="18" t="s">
+      <c r="G162" s="17" t="s">
         <v>221</v>
       </c>
       <c r="H162" s="7" t="s">
@@ -10700,7 +10708,7 @@
         <v>98</v>
       </c>
       <c r="S162" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10719,10 +10727,10 @@
       <c r="E163" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F163" s="18" t="s">
+      <c r="F163" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="G163" s="18" t="s">
+      <c r="G163" s="17" t="s">
         <v>221</v>
       </c>
       <c r="H163" s="7" t="s">
@@ -10759,7 +10767,7 @@
         <v>103</v>
       </c>
       <c r="S163" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10778,10 +10786,10 @@
       <c r="E164" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F164" s="18" t="s">
+      <c r="F164" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="G164" s="18" t="s">
+      <c r="G164" s="17" t="s">
         <v>221</v>
       </c>
       <c r="H164" s="7" t="s">
@@ -10818,7 +10826,7 @@
         <v>110</v>
       </c>
       <c r="S164" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10837,10 +10845,10 @@
       <c r="E165" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F165" s="18" t="s">
+      <c r="F165" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="G165" s="18" t="s">
+      <c r="G165" s="17" t="s">
         <v>65</v>
       </c>
       <c r="H165" s="7" t="s">
@@ -10877,7 +10885,7 @@
         <v>98</v>
       </c>
       <c r="S165" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10896,10 +10904,10 @@
       <c r="E166" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F166" s="18" t="s">
+      <c r="F166" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="G166" s="18" t="s">
+      <c r="G166" s="17" t="s">
         <v>65</v>
       </c>
       <c r="H166" s="7" t="s">
@@ -10936,7 +10944,7 @@
         <v>103</v>
       </c>
       <c r="S166" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10955,10 +10963,10 @@
       <c r="E167" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F167" s="18" t="s">
+      <c r="F167" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="G167" s="18" t="s">
+      <c r="G167" s="17" t="s">
         <v>65</v>
       </c>
       <c r="H167" s="7" t="s">
@@ -10995,7 +11003,7 @@
         <v>110</v>
       </c>
       <c r="S167" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11014,10 +11022,10 @@
       <c r="E168" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F168" s="18" t="s">
+      <c r="F168" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="G168" s="18" t="s">
+      <c r="G168" s="17" t="s">
         <v>224</v>
       </c>
       <c r="H168" s="7" t="s">
@@ -11054,7 +11062,7 @@
         <v>98</v>
       </c>
       <c r="S168" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11073,10 +11081,10 @@
       <c r="E169" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F169" s="18" t="s">
+      <c r="F169" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="G169" s="18" t="s">
+      <c r="G169" s="17" t="s">
         <v>224</v>
       </c>
       <c r="H169" s="7" t="s">
@@ -11113,7 +11121,7 @@
         <v>103</v>
       </c>
       <c r="S169" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11132,10 +11140,10 @@
       <c r="E170" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F170" s="18" t="s">
+      <c r="F170" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="G170" s="18" t="s">
+      <c r="G170" s="17" t="s">
         <v>224</v>
       </c>
       <c r="H170" s="7" t="s">
@@ -11172,7 +11180,66 @@
         <v>110</v>
       </c>
       <c r="S170" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="1" t="n">
+        <v>6001</v>
+      </c>
+      <c r="B171" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C171" s="5" t="n">
+        <v>10056</v>
+      </c>
+      <c r="D171" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E171" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F171" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="G171" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="H171" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I171" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="J171" s="1" t="n">
+        <v>286352</v>
+      </c>
+      <c r="K171" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="L171" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M171" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N171" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="O171" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="P171" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q171" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="R171" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="S171" s="1" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat：some bgm sound fix
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Stage_关卡表.xlsx
+++ b/nevergiveup/Excel/Stage_关卡表.xlsx
@@ -1221,10 +1221,10 @@
   </sheetPr>
   <dimension ref="A1:V171"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="Q7" activeCellId="0" sqref="Q7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="bottomLeft" activeCell="W76" activeCellId="0" sqref="W76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.48828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2571,7 +2571,7 @@
         <v>404268</v>
       </c>
       <c r="V21" s="14" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2639,7 +2639,7 @@
         <v>404268</v>
       </c>
       <c r="V22" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2707,7 +2707,7 @@
         <v>404268</v>
       </c>
       <c r="V23" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2775,7 +2775,7 @@
         <v>404268</v>
       </c>
       <c r="V24" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2843,7 +2843,7 @@
         <v>404268</v>
       </c>
       <c r="V25" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2911,7 +2911,7 @@
         <v>404268</v>
       </c>
       <c r="V26" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2979,7 +2979,7 @@
         <v>404268</v>
       </c>
       <c r="V27" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3047,7 +3047,7 @@
         <v>404268</v>
       </c>
       <c r="V28" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3115,7 +3115,7 @@
         <v>404268</v>
       </c>
       <c r="V29" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3183,7 +3183,7 @@
         <v>404268</v>
       </c>
       <c r="V30" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3251,7 +3251,7 @@
         <v>404268</v>
       </c>
       <c r="V31" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3319,7 +3319,7 @@
         <v>404268</v>
       </c>
       <c r="V32" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3387,7 +3387,7 @@
         <v>404268</v>
       </c>
       <c r="V33" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3455,7 +3455,7 @@
         <v>404268</v>
       </c>
       <c r="V34" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3523,7 +3523,7 @@
         <v>404268</v>
       </c>
       <c r="V35" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3591,7 +3591,7 @@
         <v>404268</v>
       </c>
       <c r="V36" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3659,7 +3659,7 @@
         <v>404268</v>
       </c>
       <c r="V37" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3727,7 +3727,7 @@
         <v>404268</v>
       </c>
       <c r="V38" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3795,7 +3795,7 @@
         <v>404268</v>
       </c>
       <c r="V39" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3863,7 +3863,7 @@
         <v>404268</v>
       </c>
       <c r="V40" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3931,7 +3931,7 @@
         <v>404268</v>
       </c>
       <c r="V41" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3999,7 +3999,7 @@
         <v>404268</v>
       </c>
       <c r="V42" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4067,7 +4067,7 @@
         <v>404268</v>
       </c>
       <c r="V43" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4135,7 +4135,7 @@
         <v>404268</v>
       </c>
       <c r="V44" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4203,7 +4203,7 @@
         <v>404268</v>
       </c>
       <c r="V45" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4271,7 +4271,7 @@
         <v>404268</v>
       </c>
       <c r="V46" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4339,7 +4339,7 @@
         <v>404268</v>
       </c>
       <c r="V47" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4407,7 +4407,7 @@
         <v>404268</v>
       </c>
       <c r="V48" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4475,7 +4475,7 @@
         <v>404268</v>
       </c>
       <c r="V49" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="50" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4543,7 +4543,7 @@
         <v>404268</v>
       </c>
       <c r="V50" s="14" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4611,7 +4611,7 @@
         <v>404267</v>
       </c>
       <c r="V51" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4679,7 +4679,7 @@
         <v>404267</v>
       </c>
       <c r="V52" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4747,7 +4747,7 @@
         <v>404267</v>
       </c>
       <c r="V53" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4815,7 +4815,7 @@
         <v>404267</v>
       </c>
       <c r="V54" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4883,7 +4883,7 @@
         <v>404267</v>
       </c>
       <c r="V55" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4951,7 +4951,7 @@
         <v>404267</v>
       </c>
       <c r="V56" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5019,7 +5019,7 @@
         <v>404267</v>
       </c>
       <c r="V57" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5087,7 +5087,7 @@
         <v>404267</v>
       </c>
       <c r="V58" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5155,7 +5155,7 @@
         <v>404267</v>
       </c>
       <c r="V59" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5223,7 +5223,7 @@
         <v>404267</v>
       </c>
       <c r="V60" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5291,7 +5291,7 @@
         <v>404267</v>
       </c>
       <c r="V61" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5359,7 +5359,7 @@
         <v>404267</v>
       </c>
       <c r="V62" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5427,7 +5427,7 @@
         <v>404267</v>
       </c>
       <c r="V63" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5495,7 +5495,7 @@
         <v>404267</v>
       </c>
       <c r="V64" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5563,7 +5563,7 @@
         <v>404267</v>
       </c>
       <c r="V65" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5631,7 +5631,7 @@
         <v>404267</v>
       </c>
       <c r="V66" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5699,7 +5699,7 @@
         <v>404267</v>
       </c>
       <c r="V67" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5767,7 +5767,7 @@
         <v>404267</v>
       </c>
       <c r="V68" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5835,7 +5835,7 @@
         <v>404267</v>
       </c>
       <c r="V69" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5903,7 +5903,7 @@
         <v>404267</v>
       </c>
       <c r="V70" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5971,7 +5971,7 @@
         <v>404267</v>
       </c>
       <c r="V71" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6039,7 +6039,7 @@
         <v>404267</v>
       </c>
       <c r="V72" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6107,7 +6107,7 @@
         <v>404267</v>
       </c>
       <c r="V73" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6175,7 +6175,7 @@
         <v>404267</v>
       </c>
       <c r="V74" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6243,7 +6243,7 @@
         <v>404267</v>
       </c>
       <c r="V75" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6311,7 +6311,7 @@
         <v>404267</v>
       </c>
       <c r="V76" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6379,7 +6379,7 @@
         <v>404267</v>
       </c>
       <c r="V77" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6447,7 +6447,7 @@
         <v>404267</v>
       </c>
       <c r="V78" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6515,7 +6515,7 @@
         <v>404267</v>
       </c>
       <c r="V79" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="80" s="14" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6583,7 +6583,7 @@
         <v>404267</v>
       </c>
       <c r="V80" s="14" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat：change some monster excel
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Stage_关卡表.xlsx
+++ b/nevergiveup/Excel/Stage_关卡表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="245">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -431,6 +431,9 @@
   </si>
   <si>
     <t xml:space="preserve">0|0|-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1023|1||1|300||3|12</t>
   </si>
   <si>
     <t xml:space="preserve">1|50||3|10</t>
@@ -1221,10 +1224,10 @@
   </sheetPr>
   <dimension ref="A1:V171"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="W76" activeCellId="0" sqref="W76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="P21" activeCellId="0" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.48828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2553,13 +2556,13 @@
         <v>61</v>
       </c>
       <c r="P21" s="11" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="Q21" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="S21" s="14" t="n">
         <v>2</v>
@@ -2727,10 +2730,10 @@
         <v>53</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>58</v>
@@ -2760,10 +2763,10 @@
         <v>62</v>
       </c>
       <c r="Q24" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R24" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="S24" s="1" t="n">
         <v>2</v>
@@ -2795,10 +2798,10 @@
         <v>53</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>66</v>
@@ -2863,10 +2866,10 @@
         <v>53</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>74</v>
@@ -2931,10 +2934,10 @@
         <v>53</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>58</v>
@@ -2964,10 +2967,10 @@
         <v>62</v>
       </c>
       <c r="Q27" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="S27" s="1" t="n">
         <v>2</v>
@@ -2999,10 +3002,10 @@
         <v>53</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>66</v>
@@ -3067,10 +3070,10 @@
         <v>53</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>74</v>
@@ -3135,10 +3138,10 @@
         <v>53</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>58</v>
@@ -3168,10 +3171,10 @@
         <v>62</v>
       </c>
       <c r="Q30" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R30" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="S30" s="1" t="n">
         <v>2</v>
@@ -3203,10 +3206,10 @@
         <v>53</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>66</v>
@@ -3271,10 +3274,10 @@
         <v>53</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>74</v>
@@ -3339,10 +3342,10 @@
         <v>53</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>58</v>
@@ -3372,10 +3375,10 @@
         <v>62</v>
       </c>
       <c r="Q33" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R33" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="S33" s="1" t="n">
         <v>2</v>
@@ -3407,10 +3410,10 @@
         <v>53</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>66</v>
@@ -3475,10 +3478,10 @@
         <v>53</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>74</v>
@@ -3543,10 +3546,10 @@
         <v>53</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>58</v>
@@ -3576,10 +3579,10 @@
         <v>62</v>
       </c>
       <c r="Q36" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R36" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="S36" s="1" t="n">
         <v>2</v>
@@ -3611,10 +3614,10 @@
         <v>53</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>66</v>
@@ -3679,10 +3682,10 @@
         <v>53</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>74</v>
@@ -3747,10 +3750,10 @@
         <v>53</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H39" s="7" t="s">
         <v>58</v>
@@ -3780,10 +3783,10 @@
         <v>62</v>
       </c>
       <c r="Q39" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R39" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="S39" s="1" t="n">
         <v>2</v>
@@ -3815,10 +3818,10 @@
         <v>53</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>66</v>
@@ -3883,10 +3886,10 @@
         <v>53</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>74</v>
@@ -3951,10 +3954,10 @@
         <v>53</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H42" s="7" t="s">
         <v>58</v>
@@ -3984,10 +3987,10 @@
         <v>62</v>
       </c>
       <c r="Q42" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R42" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="S42" s="1" t="n">
         <v>2</v>
@@ -4019,10 +4022,10 @@
         <v>53</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>66</v>
@@ -4087,10 +4090,10 @@
         <v>53</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H44" s="7" t="s">
         <v>74</v>
@@ -4155,10 +4158,10 @@
         <v>53</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>58</v>
@@ -4188,10 +4191,10 @@
         <v>62</v>
       </c>
       <c r="Q45" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R45" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="S45" s="1" t="n">
         <v>2</v>
@@ -4223,10 +4226,10 @@
         <v>53</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>66</v>
@@ -4291,10 +4294,10 @@
         <v>53</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>74</v>
@@ -4359,10 +4362,10 @@
         <v>53</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H48" s="7" t="s">
         <v>58</v>
@@ -4392,10 +4395,10 @@
         <v>62</v>
       </c>
       <c r="Q48" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R48" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="S48" s="1" t="n">
         <v>2</v>
@@ -4427,10 +4430,10 @@
         <v>53</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>66</v>
@@ -4495,10 +4498,10 @@
         <v>53</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H50" s="12" t="s">
         <v>74</v>
@@ -4563,10 +4566,10 @@
         <v>53</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H51" s="7" t="s">
         <v>83</v>
@@ -4605,7 +4608,7 @@
         <v>3</v>
       </c>
       <c r="T51" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U51" s="1" t="n">
         <v>404267</v>
@@ -4631,10 +4634,10 @@
         <v>53</v>
       </c>
       <c r="F52" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H52" s="7" t="s">
         <v>90</v>
@@ -4673,7 +4676,7 @@
         <v>3</v>
       </c>
       <c r="T52" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U52" s="1" t="n">
         <v>404267</v>
@@ -4699,10 +4702,10 @@
         <v>53</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>95</v>
@@ -4741,7 +4744,7 @@
         <v>3</v>
       </c>
       <c r="T53" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U53" s="1" t="n">
         <v>404267</v>
@@ -4767,10 +4770,10 @@
         <v>53</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G54" s="18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>83</v>
@@ -4809,7 +4812,7 @@
         <v>3</v>
       </c>
       <c r="T54" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U54" s="1" t="n">
         <v>404267</v>
@@ -4835,10 +4838,10 @@
         <v>53</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G55" s="18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>90</v>
@@ -4877,7 +4880,7 @@
         <v>3</v>
       </c>
       <c r="T55" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U55" s="1" t="n">
         <v>404267</v>
@@ -4903,10 +4906,10 @@
         <v>53</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G56" s="18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>95</v>
@@ -4945,7 +4948,7 @@
         <v>3</v>
       </c>
       <c r="T56" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U56" s="1" t="n">
         <v>404267</v>
@@ -4971,10 +4974,10 @@
         <v>53</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G57" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>83</v>
@@ -5013,7 +5016,7 @@
         <v>3</v>
       </c>
       <c r="T57" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U57" s="1" t="n">
         <v>404267</v>
@@ -5039,10 +5042,10 @@
         <v>53</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G58" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H58" s="7" t="s">
         <v>90</v>
@@ -5081,7 +5084,7 @@
         <v>3</v>
       </c>
       <c r="T58" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U58" s="1" t="n">
         <v>404267</v>
@@ -5107,10 +5110,10 @@
         <v>53</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G59" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H59" s="7" t="s">
         <v>95</v>
@@ -5149,7 +5152,7 @@
         <v>3</v>
       </c>
       <c r="T59" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U59" s="1" t="n">
         <v>404267</v>
@@ -5175,10 +5178,10 @@
         <v>53</v>
       </c>
       <c r="F60" s="17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G60" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>83</v>
@@ -5217,7 +5220,7 @@
         <v>3</v>
       </c>
       <c r="T60" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U60" s="1" t="n">
         <v>404267</v>
@@ -5243,10 +5246,10 @@
         <v>53</v>
       </c>
       <c r="F61" s="17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G61" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>90</v>
@@ -5285,7 +5288,7 @@
         <v>3</v>
       </c>
       <c r="T61" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U61" s="1" t="n">
         <v>404267</v>
@@ -5311,10 +5314,10 @@
         <v>53</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G62" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H62" s="7" t="s">
         <v>95</v>
@@ -5353,7 +5356,7 @@
         <v>3</v>
       </c>
       <c r="T62" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U62" s="1" t="n">
         <v>404267</v>
@@ -5379,10 +5382,10 @@
         <v>53</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H63" s="7" t="s">
         <v>83</v>
@@ -5421,7 +5424,7 @@
         <v>3</v>
       </c>
       <c r="T63" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U63" s="1" t="n">
         <v>404267</v>
@@ -5447,10 +5450,10 @@
         <v>53</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G64" s="18" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H64" s="7" t="s">
         <v>90</v>
@@ -5489,7 +5492,7 @@
         <v>3</v>
       </c>
       <c r="T64" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U64" s="1" t="n">
         <v>404267</v>
@@ -5515,10 +5518,10 @@
         <v>53</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H65" s="7" t="s">
         <v>95</v>
@@ -5557,7 +5560,7 @@
         <v>3</v>
       </c>
       <c r="T65" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U65" s="1" t="n">
         <v>404267</v>
@@ -5583,10 +5586,10 @@
         <v>53</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H66" s="7" t="s">
         <v>83</v>
@@ -5625,7 +5628,7 @@
         <v>3</v>
       </c>
       <c r="T66" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U66" s="1" t="n">
         <v>404267</v>
@@ -5651,10 +5654,10 @@
         <v>53</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G67" s="18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H67" s="7" t="s">
         <v>90</v>
@@ -5693,7 +5696,7 @@
         <v>3</v>
       </c>
       <c r="T67" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U67" s="1" t="n">
         <v>404267</v>
@@ -5719,10 +5722,10 @@
         <v>53</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G68" s="18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H68" s="7" t="s">
         <v>95</v>
@@ -5761,7 +5764,7 @@
         <v>3</v>
       </c>
       <c r="T68" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U68" s="1" t="n">
         <v>404267</v>
@@ -5787,10 +5790,10 @@
         <v>53</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G69" s="18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H69" s="7" t="s">
         <v>83</v>
@@ -5829,7 +5832,7 @@
         <v>3</v>
       </c>
       <c r="T69" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U69" s="1" t="n">
         <v>404267</v>
@@ -5855,10 +5858,10 @@
         <v>53</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G70" s="18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H70" s="7" t="s">
         <v>90</v>
@@ -5897,7 +5900,7 @@
         <v>3</v>
       </c>
       <c r="T70" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U70" s="1" t="n">
         <v>404267</v>
@@ -5923,10 +5926,10 @@
         <v>53</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G71" s="18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H71" s="7" t="s">
         <v>95</v>
@@ -5965,7 +5968,7 @@
         <v>3</v>
       </c>
       <c r="T71" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U71" s="1" t="n">
         <v>404267</v>
@@ -5991,10 +5994,10 @@
         <v>53</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G72" s="18" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H72" s="7" t="s">
         <v>83</v>
@@ -6033,7 +6036,7 @@
         <v>3</v>
       </c>
       <c r="T72" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U72" s="1" t="n">
         <v>404267</v>
@@ -6059,10 +6062,10 @@
         <v>53</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G73" s="18" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H73" s="7" t="s">
         <v>90</v>
@@ -6101,7 +6104,7 @@
         <v>3</v>
       </c>
       <c r="T73" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U73" s="1" t="n">
         <v>404267</v>
@@ -6127,10 +6130,10 @@
         <v>53</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G74" s="18" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H74" s="7" t="s">
         <v>95</v>
@@ -6169,7 +6172,7 @@
         <v>3</v>
       </c>
       <c r="T74" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U74" s="1" t="n">
         <v>404267</v>
@@ -6195,10 +6198,10 @@
         <v>53</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G75" s="18" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H75" s="7" t="s">
         <v>83</v>
@@ -6237,7 +6240,7 @@
         <v>3</v>
       </c>
       <c r="T75" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U75" s="1" t="n">
         <v>404267</v>
@@ -6263,10 +6266,10 @@
         <v>53</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G76" s="18" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H76" s="7" t="s">
         <v>90</v>
@@ -6305,7 +6308,7 @@
         <v>3</v>
       </c>
       <c r="T76" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U76" s="1" t="n">
         <v>404267</v>
@@ -6331,10 +6334,10 @@
         <v>53</v>
       </c>
       <c r="F77" s="17" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G77" s="18" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H77" s="7" t="s">
         <v>95</v>
@@ -6373,7 +6376,7 @@
         <v>3</v>
       </c>
       <c r="T77" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U77" s="1" t="n">
         <v>404267</v>
@@ -6399,7 +6402,7 @@
         <v>53</v>
       </c>
       <c r="F78" s="17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G78" s="18" t="s">
         <v>73</v>
@@ -6441,7 +6444,7 @@
         <v>3</v>
       </c>
       <c r="T78" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U78" s="1" t="n">
         <v>404267</v>
@@ -6467,7 +6470,7 @@
         <v>53</v>
       </c>
       <c r="F79" s="17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G79" s="18" t="s">
         <v>73</v>
@@ -6509,7 +6512,7 @@
         <v>3</v>
       </c>
       <c r="T79" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U79" s="1" t="n">
         <v>404267</v>
@@ -6535,7 +6538,7 @@
         <v>53</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G80" s="20" t="s">
         <v>73</v>
@@ -6577,7 +6580,7 @@
         <v>3</v>
       </c>
       <c r="T80" s="14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U80" s="14" t="n">
         <v>404267</v>
@@ -6603,10 +6606,10 @@
         <v>53</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G81" s="18" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H81" s="7" t="s">
         <v>102</v>
@@ -6645,7 +6648,7 @@
         <v>4</v>
       </c>
       <c r="T81" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U81" s="1" t="n">
         <v>404269</v>
@@ -6671,10 +6674,10 @@
         <v>53</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G82" s="18" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H82" s="7" t="s">
         <v>107</v>
@@ -6713,7 +6716,7 @@
         <v>4</v>
       </c>
       <c r="T82" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U82" s="1" t="n">
         <v>404269</v>
@@ -6739,10 +6742,10 @@
         <v>53</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G83" s="18" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H83" s="7" t="s">
         <v>112</v>
@@ -6781,7 +6784,7 @@
         <v>4</v>
       </c>
       <c r="T83" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U83" s="1" t="n">
         <v>404269</v>
@@ -6807,10 +6810,10 @@
         <v>53</v>
       </c>
       <c r="F84" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G84" s="18" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H84" s="7" t="s">
         <v>102</v>
@@ -6849,7 +6852,7 @@
         <v>4</v>
       </c>
       <c r="T84" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U84" s="1" t="n">
         <v>404269</v>
@@ -6875,10 +6878,10 @@
         <v>53</v>
       </c>
       <c r="F85" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G85" s="18" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H85" s="7" t="s">
         <v>107</v>
@@ -6917,7 +6920,7 @@
         <v>4</v>
       </c>
       <c r="T85" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U85" s="1" t="n">
         <v>404269</v>
@@ -6943,10 +6946,10 @@
         <v>53</v>
       </c>
       <c r="F86" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G86" s="18" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H86" s="7" t="s">
         <v>112</v>
@@ -6985,7 +6988,7 @@
         <v>4</v>
       </c>
       <c r="T86" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U86" s="1" t="n">
         <v>404269</v>
@@ -7011,10 +7014,10 @@
         <v>53</v>
       </c>
       <c r="F87" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G87" s="18" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H87" s="7" t="s">
         <v>102</v>
@@ -7053,7 +7056,7 @@
         <v>4</v>
       </c>
       <c r="T87" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U87" s="1" t="n">
         <v>404269</v>
@@ -7079,10 +7082,10 @@
         <v>53</v>
       </c>
       <c r="F88" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G88" s="18" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H88" s="7" t="s">
         <v>107</v>
@@ -7121,7 +7124,7 @@
         <v>4</v>
       </c>
       <c r="T88" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U88" s="1" t="n">
         <v>404269</v>
@@ -7147,10 +7150,10 @@
         <v>53</v>
       </c>
       <c r="F89" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G89" s="18" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H89" s="7" t="s">
         <v>112</v>
@@ -7189,7 +7192,7 @@
         <v>4</v>
       </c>
       <c r="T89" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U89" s="1" t="n">
         <v>404269</v>
@@ -7215,10 +7218,10 @@
         <v>53</v>
       </c>
       <c r="F90" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G90" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H90" s="7" t="s">
         <v>102</v>
@@ -7257,7 +7260,7 @@
         <v>4</v>
       </c>
       <c r="T90" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U90" s="1" t="n">
         <v>404269</v>
@@ -7283,10 +7286,10 @@
         <v>53</v>
       </c>
       <c r="F91" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G91" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H91" s="7" t="s">
         <v>107</v>
@@ -7325,7 +7328,7 @@
         <v>4</v>
       </c>
       <c r="T91" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U91" s="1" t="n">
         <v>404269</v>
@@ -7351,10 +7354,10 @@
         <v>53</v>
       </c>
       <c r="F92" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G92" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H92" s="7" t="s">
         <v>112</v>
@@ -7393,7 +7396,7 @@
         <v>4</v>
       </c>
       <c r="T92" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U92" s="1" t="n">
         <v>404269</v>
@@ -7419,10 +7422,10 @@
         <v>53</v>
       </c>
       <c r="F93" s="17" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G93" s="18" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H93" s="7" t="s">
         <v>102</v>
@@ -7461,7 +7464,7 @@
         <v>4</v>
       </c>
       <c r="T93" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U93" s="1" t="n">
         <v>404269</v>
@@ -7487,10 +7490,10 @@
         <v>53</v>
       </c>
       <c r="F94" s="17" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G94" s="18" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H94" s="7" t="s">
         <v>107</v>
@@ -7529,7 +7532,7 @@
         <v>4</v>
       </c>
       <c r="T94" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U94" s="1" t="n">
         <v>404269</v>
@@ -7555,10 +7558,10 @@
         <v>53</v>
       </c>
       <c r="F95" s="17" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G95" s="18" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H95" s="7" t="s">
         <v>112</v>
@@ -7597,7 +7600,7 @@
         <v>4</v>
       </c>
       <c r="T95" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U95" s="1" t="n">
         <v>404269</v>
@@ -7623,10 +7626,10 @@
         <v>53</v>
       </c>
       <c r="F96" s="17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G96" s="18" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H96" s="7" t="s">
         <v>102</v>
@@ -7665,7 +7668,7 @@
         <v>4</v>
       </c>
       <c r="T96" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U96" s="1" t="n">
         <v>404269</v>
@@ -7691,10 +7694,10 @@
         <v>53</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G97" s="18" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H97" s="7" t="s">
         <v>107</v>
@@ -7733,7 +7736,7 @@
         <v>4</v>
       </c>
       <c r="T97" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U97" s="1" t="n">
         <v>404269</v>
@@ -7759,10 +7762,10 @@
         <v>53</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G98" s="18" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H98" s="7" t="s">
         <v>112</v>
@@ -7801,7 +7804,7 @@
         <v>4</v>
       </c>
       <c r="T98" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U98" s="1" t="n">
         <v>404269</v>
@@ -7827,10 +7830,10 @@
         <v>53</v>
       </c>
       <c r="F99" s="17" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G99" s="18" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H99" s="7" t="s">
         <v>102</v>
@@ -7869,7 +7872,7 @@
         <v>4</v>
       </c>
       <c r="T99" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U99" s="1" t="n">
         <v>404269</v>
@@ -7895,10 +7898,10 @@
         <v>53</v>
       </c>
       <c r="F100" s="17" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G100" s="18" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H100" s="7" t="s">
         <v>107</v>
@@ -7937,7 +7940,7 @@
         <v>4</v>
       </c>
       <c r="T100" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U100" s="1" t="n">
         <v>404269</v>
@@ -7963,10 +7966,10 @@
         <v>53</v>
       </c>
       <c r="F101" s="17" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G101" s="18" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H101" s="7" t="s">
         <v>112</v>
@@ -8005,7 +8008,7 @@
         <v>4</v>
       </c>
       <c r="T101" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U101" s="1" t="n">
         <v>404269</v>
@@ -8031,10 +8034,10 @@
         <v>53</v>
       </c>
       <c r="F102" s="17" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G102" s="18" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H102" s="7" t="s">
         <v>102</v>
@@ -8073,7 +8076,7 @@
         <v>4</v>
       </c>
       <c r="T102" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U102" s="1" t="n">
         <v>404269</v>
@@ -8099,10 +8102,10 @@
         <v>53</v>
       </c>
       <c r="F103" s="17" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G103" s="18" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H103" s="7" t="s">
         <v>107</v>
@@ -8141,7 +8144,7 @@
         <v>4</v>
       </c>
       <c r="T103" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U103" s="1" t="n">
         <v>404269</v>
@@ -8167,10 +8170,10 @@
         <v>53</v>
       </c>
       <c r="F104" s="17" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G104" s="18" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H104" s="7" t="s">
         <v>112</v>
@@ -8209,7 +8212,7 @@
         <v>4</v>
       </c>
       <c r="T104" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U104" s="1" t="n">
         <v>404269</v>
@@ -8235,10 +8238,10 @@
         <v>53</v>
       </c>
       <c r="F105" s="17" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G105" s="18" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H105" s="7" t="s">
         <v>102</v>
@@ -8277,7 +8280,7 @@
         <v>4</v>
       </c>
       <c r="T105" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U105" s="1" t="n">
         <v>404269</v>
@@ -8303,10 +8306,10 @@
         <v>53</v>
       </c>
       <c r="F106" s="17" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G106" s="18" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H106" s="7" t="s">
         <v>107</v>
@@ -8345,7 +8348,7 @@
         <v>4</v>
       </c>
       <c r="T106" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U106" s="1" t="n">
         <v>404269</v>
@@ -8371,10 +8374,10 @@
         <v>53</v>
       </c>
       <c r="F107" s="17" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G107" s="18" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H107" s="7" t="s">
         <v>112</v>
@@ -8413,7 +8416,7 @@
         <v>4</v>
       </c>
       <c r="T107" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U107" s="1" t="n">
         <v>404269</v>
@@ -8439,10 +8442,10 @@
         <v>53</v>
       </c>
       <c r="F108" s="17" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G108" s="18" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H108" s="7" t="s">
         <v>102</v>
@@ -8481,7 +8484,7 @@
         <v>4</v>
       </c>
       <c r="T108" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U108" s="1" t="n">
         <v>404269</v>
@@ -8507,10 +8510,10 @@
         <v>53</v>
       </c>
       <c r="F109" s="17" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G109" s="18" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H109" s="7" t="s">
         <v>107</v>
@@ -8549,7 +8552,7 @@
         <v>4</v>
       </c>
       <c r="T109" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U109" s="1" t="n">
         <v>404269</v>
@@ -8575,10 +8578,10 @@
         <v>53</v>
       </c>
       <c r="F110" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G110" s="20" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H110" s="12" t="s">
         <v>112</v>
@@ -8617,7 +8620,7 @@
         <v>4</v>
       </c>
       <c r="T110" s="14" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U110" s="14" t="n">
         <v>404269</v>
@@ -8643,10 +8646,10 @@
         <v>53</v>
       </c>
       <c r="F111" s="17" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G111" s="18" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H111" s="7" t="s">
         <v>121</v>
@@ -8685,7 +8688,7 @@
         <v>5</v>
       </c>
       <c r="T111" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U111" s="1" t="n">
         <v>404266</v>
@@ -8711,10 +8714,10 @@
         <v>53</v>
       </c>
       <c r="F112" s="17" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G112" s="18" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H112" s="7" t="s">
         <v>123</v>
@@ -8753,7 +8756,7 @@
         <v>5</v>
       </c>
       <c r="T112" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U112" s="1" t="n">
         <v>404266</v>
@@ -8779,10 +8782,10 @@
         <v>53</v>
       </c>
       <c r="F113" s="17" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G113" s="18" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H113" s="7" t="s">
         <v>125</v>
@@ -8821,7 +8824,7 @@
         <v>5</v>
       </c>
       <c r="T113" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U113" s="1" t="n">
         <v>404266</v>
@@ -8847,10 +8850,10 @@
         <v>53</v>
       </c>
       <c r="F114" s="17" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G114" s="18" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H114" s="7" t="s">
         <v>121</v>
@@ -8889,7 +8892,7 @@
         <v>5</v>
       </c>
       <c r="T114" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U114" s="1" t="n">
         <v>404266</v>
@@ -8915,10 +8918,10 @@
         <v>53</v>
       </c>
       <c r="F115" s="17" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G115" s="18" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H115" s="7" t="s">
         <v>123</v>
@@ -8957,7 +8960,7 @@
         <v>5</v>
       </c>
       <c r="T115" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U115" s="1" t="n">
         <v>404266</v>
@@ -8983,10 +8986,10 @@
         <v>53</v>
       </c>
       <c r="F116" s="17" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G116" s="18" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H116" s="7" t="s">
         <v>125</v>
@@ -9025,7 +9028,7 @@
         <v>5</v>
       </c>
       <c r="T116" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U116" s="1" t="n">
         <v>404266</v>
@@ -9051,10 +9054,10 @@
         <v>53</v>
       </c>
       <c r="F117" s="17" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G117" s="18" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H117" s="7" t="s">
         <v>121</v>
@@ -9093,7 +9096,7 @@
         <v>5</v>
       </c>
       <c r="T117" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U117" s="1" t="n">
         <v>404266</v>
@@ -9119,10 +9122,10 @@
         <v>53</v>
       </c>
       <c r="F118" s="17" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G118" s="18" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H118" s="7" t="s">
         <v>123</v>
@@ -9161,7 +9164,7 @@
         <v>5</v>
       </c>
       <c r="T118" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U118" s="1" t="n">
         <v>404266</v>
@@ -9187,10 +9190,10 @@
         <v>53</v>
       </c>
       <c r="F119" s="17" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G119" s="18" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H119" s="7" t="s">
         <v>125</v>
@@ -9229,7 +9232,7 @@
         <v>5</v>
       </c>
       <c r="T119" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U119" s="1" t="n">
         <v>404266</v>
@@ -9255,10 +9258,10 @@
         <v>53</v>
       </c>
       <c r="F120" s="17" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G120" s="18" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H120" s="7" t="s">
         <v>121</v>
@@ -9297,7 +9300,7 @@
         <v>5</v>
       </c>
       <c r="T120" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U120" s="1" t="n">
         <v>404266</v>
@@ -9323,10 +9326,10 @@
         <v>53</v>
       </c>
       <c r="F121" s="17" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G121" s="18" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H121" s="7" t="s">
         <v>123</v>
@@ -9365,7 +9368,7 @@
         <v>5</v>
       </c>
       <c r="T121" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U121" s="1" t="n">
         <v>404266</v>
@@ -9391,10 +9394,10 @@
         <v>53</v>
       </c>
       <c r="F122" s="17" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G122" s="18" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H122" s="7" t="s">
         <v>125</v>
@@ -9433,7 +9436,7 @@
         <v>5</v>
       </c>
       <c r="T122" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U122" s="1" t="n">
         <v>404266</v>
@@ -9459,10 +9462,10 @@
         <v>53</v>
       </c>
       <c r="F123" s="17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G123" s="18" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H123" s="7" t="s">
         <v>121</v>
@@ -9501,7 +9504,7 @@
         <v>5</v>
       </c>
       <c r="T123" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U123" s="1" t="n">
         <v>404266</v>
@@ -9527,10 +9530,10 @@
         <v>53</v>
       </c>
       <c r="F124" s="17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G124" s="18" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H124" s="7" t="s">
         <v>123</v>
@@ -9569,7 +9572,7 @@
         <v>5</v>
       </c>
       <c r="T124" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U124" s="1" t="n">
         <v>404266</v>
@@ -9595,10 +9598,10 @@
         <v>53</v>
       </c>
       <c r="F125" s="17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G125" s="18" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H125" s="7" t="s">
         <v>125</v>
@@ -9637,7 +9640,7 @@
         <v>5</v>
       </c>
       <c r="T125" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U125" s="1" t="n">
         <v>404266</v>
@@ -9663,10 +9666,10 @@
         <v>53</v>
       </c>
       <c r="F126" s="17" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G126" s="18" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H126" s="7" t="s">
         <v>121</v>
@@ -9705,7 +9708,7 @@
         <v>5</v>
       </c>
       <c r="T126" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U126" s="1" t="n">
         <v>404266</v>
@@ -9731,10 +9734,10 @@
         <v>53</v>
       </c>
       <c r="F127" s="17" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G127" s="18" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H127" s="7" t="s">
         <v>123</v>
@@ -9773,7 +9776,7 @@
         <v>5</v>
       </c>
       <c r="T127" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U127" s="1" t="n">
         <v>404266</v>
@@ -9799,10 +9802,10 @@
         <v>53</v>
       </c>
       <c r="F128" s="17" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G128" s="18" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H128" s="7" t="s">
         <v>125</v>
@@ -9841,7 +9844,7 @@
         <v>5</v>
       </c>
       <c r="T128" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U128" s="1" t="n">
         <v>404266</v>
@@ -9867,10 +9870,10 @@
         <v>53</v>
       </c>
       <c r="F129" s="17" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G129" s="18" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H129" s="7" t="s">
         <v>121</v>
@@ -9909,7 +9912,7 @@
         <v>5</v>
       </c>
       <c r="T129" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U129" s="1" t="n">
         <v>404266</v>
@@ -9935,10 +9938,10 @@
         <v>53</v>
       </c>
       <c r="F130" s="17" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G130" s="18" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H130" s="7" t="s">
         <v>123</v>
@@ -9977,7 +9980,7 @@
         <v>5</v>
       </c>
       <c r="T130" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U130" s="1" t="n">
         <v>404266</v>
@@ -10003,10 +10006,10 @@
         <v>53</v>
       </c>
       <c r="F131" s="17" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G131" s="18" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H131" s="7" t="s">
         <v>125</v>
@@ -10045,7 +10048,7 @@
         <v>5</v>
       </c>
       <c r="T131" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U131" s="1" t="n">
         <v>404266</v>
@@ -10071,10 +10074,10 @@
         <v>53</v>
       </c>
       <c r="F132" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G132" s="18" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H132" s="7" t="s">
         <v>121</v>
@@ -10113,7 +10116,7 @@
         <v>5</v>
       </c>
       <c r="T132" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U132" s="1" t="n">
         <v>404266</v>
@@ -10139,10 +10142,10 @@
         <v>53</v>
       </c>
       <c r="F133" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G133" s="18" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H133" s="7" t="s">
         <v>123</v>
@@ -10181,7 +10184,7 @@
         <v>5</v>
       </c>
       <c r="T133" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U133" s="1" t="n">
         <v>404266</v>
@@ -10207,10 +10210,10 @@
         <v>53</v>
       </c>
       <c r="F134" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G134" s="18" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H134" s="7" t="s">
         <v>125</v>
@@ -10249,7 +10252,7 @@
         <v>5</v>
       </c>
       <c r="T134" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U134" s="1" t="n">
         <v>404266</v>
@@ -10275,10 +10278,10 @@
         <v>53</v>
       </c>
       <c r="F135" s="17" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G135" s="18" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H135" s="7" t="s">
         <v>121</v>
@@ -10317,7 +10320,7 @@
         <v>5</v>
       </c>
       <c r="T135" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U135" s="1" t="n">
         <v>404266</v>
@@ -10343,10 +10346,10 @@
         <v>53</v>
       </c>
       <c r="F136" s="17" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G136" s="18" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H136" s="7" t="s">
         <v>123</v>
@@ -10385,7 +10388,7 @@
         <v>5</v>
       </c>
       <c r="T136" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U136" s="1" t="n">
         <v>404266</v>
@@ -10411,10 +10414,10 @@
         <v>53</v>
       </c>
       <c r="F137" s="17" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G137" s="18" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H137" s="7" t="s">
         <v>125</v>
@@ -10453,7 +10456,7 @@
         <v>5</v>
       </c>
       <c r="T137" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U137" s="1" t="n">
         <v>404266</v>
@@ -10479,10 +10482,10 @@
         <v>53</v>
       </c>
       <c r="F138" s="17" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G138" s="18" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H138" s="7" t="s">
         <v>121</v>
@@ -10521,7 +10524,7 @@
         <v>5</v>
       </c>
       <c r="T138" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U138" s="1" t="n">
         <v>404266</v>
@@ -10547,10 +10550,10 @@
         <v>53</v>
       </c>
       <c r="F139" s="17" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G139" s="18" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H139" s="7" t="s">
         <v>123</v>
@@ -10589,7 +10592,7 @@
         <v>5</v>
       </c>
       <c r="T139" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U139" s="1" t="n">
         <v>404266</v>
@@ -10615,10 +10618,10 @@
         <v>53</v>
       </c>
       <c r="F140" s="19" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G140" s="20" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H140" s="12" t="s">
         <v>125</v>
@@ -10657,7 +10660,7 @@
         <v>5</v>
       </c>
       <c r="T140" s="14" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U140" s="14" t="n">
         <v>404266</v>
@@ -10683,10 +10686,10 @@
         <v>53</v>
       </c>
       <c r="F141" s="17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G141" s="18" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H141" s="7" t="s">
         <v>129</v>
@@ -10725,7 +10728,7 @@
         <v>6</v>
       </c>
       <c r="T141" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U141" s="1" t="n">
         <v>404264</v>
@@ -10751,10 +10754,10 @@
         <v>53</v>
       </c>
       <c r="F142" s="17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G142" s="18" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H142" s="7" t="s">
         <v>131</v>
@@ -10793,7 +10796,7 @@
         <v>6</v>
       </c>
       <c r="T142" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U142" s="1" t="n">
         <v>404264</v>
@@ -10819,10 +10822,10 @@
         <v>53</v>
       </c>
       <c r="F143" s="17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G143" s="18" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H143" s="7" t="s">
         <v>133</v>
@@ -10861,7 +10864,7 @@
         <v>6</v>
       </c>
       <c r="T143" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U143" s="1" t="n">
         <v>404264</v>
@@ -10887,10 +10890,10 @@
         <v>53</v>
       </c>
       <c r="F144" s="17" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G144" s="18" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H144" s="7" t="s">
         <v>129</v>
@@ -10929,7 +10932,7 @@
         <v>6</v>
       </c>
       <c r="T144" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U144" s="1" t="n">
         <v>404264</v>
@@ -10955,10 +10958,10 @@
         <v>53</v>
       </c>
       <c r="F145" s="17" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G145" s="18" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H145" s="7" t="s">
         <v>131</v>
@@ -10997,7 +11000,7 @@
         <v>6</v>
       </c>
       <c r="T145" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U145" s="1" t="n">
         <v>404264</v>
@@ -11023,10 +11026,10 @@
         <v>53</v>
       </c>
       <c r="F146" s="17" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G146" s="18" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H146" s="7" t="s">
         <v>133</v>
@@ -11065,7 +11068,7 @@
         <v>6</v>
       </c>
       <c r="T146" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U146" s="1" t="n">
         <v>404264</v>
@@ -11091,10 +11094,10 @@
         <v>53</v>
       </c>
       <c r="F147" s="17" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G147" s="18" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H147" s="7" t="s">
         <v>129</v>
@@ -11133,7 +11136,7 @@
         <v>6</v>
       </c>
       <c r="T147" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U147" s="1" t="n">
         <v>404264</v>
@@ -11159,10 +11162,10 @@
         <v>53</v>
       </c>
       <c r="F148" s="17" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G148" s="18" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H148" s="7" t="s">
         <v>131</v>
@@ -11201,7 +11204,7 @@
         <v>6</v>
       </c>
       <c r="T148" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U148" s="1" t="n">
         <v>404264</v>
@@ -11227,10 +11230,10 @@
         <v>53</v>
       </c>
       <c r="F149" s="17" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G149" s="18" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H149" s="7" t="s">
         <v>133</v>
@@ -11269,7 +11272,7 @@
         <v>6</v>
       </c>
       <c r="T149" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U149" s="1" t="n">
         <v>404264</v>
@@ -11295,10 +11298,10 @@
         <v>53</v>
       </c>
       <c r="F150" s="17" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G150" s="18" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H150" s="7" t="s">
         <v>129</v>
@@ -11337,7 +11340,7 @@
         <v>6</v>
       </c>
       <c r="T150" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U150" s="1" t="n">
         <v>404264</v>
@@ -11363,10 +11366,10 @@
         <v>53</v>
       </c>
       <c r="F151" s="17" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G151" s="18" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H151" s="7" t="s">
         <v>131</v>
@@ -11405,7 +11408,7 @@
         <v>6</v>
       </c>
       <c r="T151" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U151" s="1" t="n">
         <v>404264</v>
@@ -11431,10 +11434,10 @@
         <v>53</v>
       </c>
       <c r="F152" s="17" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G152" s="18" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H152" s="7" t="s">
         <v>133</v>
@@ -11473,7 +11476,7 @@
         <v>6</v>
       </c>
       <c r="T152" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U152" s="1" t="n">
         <v>404264</v>
@@ -11499,10 +11502,10 @@
         <v>53</v>
       </c>
       <c r="F153" s="17" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G153" s="18" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H153" s="7" t="s">
         <v>129</v>
@@ -11541,7 +11544,7 @@
         <v>6</v>
       </c>
       <c r="T153" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U153" s="1" t="n">
         <v>404264</v>
@@ -11567,10 +11570,10 @@
         <v>53</v>
       </c>
       <c r="F154" s="17" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G154" s="18" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H154" s="7" t="s">
         <v>131</v>
@@ -11609,7 +11612,7 @@
         <v>6</v>
       </c>
       <c r="T154" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U154" s="1" t="n">
         <v>404264</v>
@@ -11635,10 +11638,10 @@
         <v>53</v>
       </c>
       <c r="F155" s="17" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G155" s="18" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H155" s="7" t="s">
         <v>133</v>
@@ -11677,7 +11680,7 @@
         <v>6</v>
       </c>
       <c r="T155" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U155" s="1" t="n">
         <v>404264</v>
@@ -11703,10 +11706,10 @@
         <v>53</v>
       </c>
       <c r="F156" s="17" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G156" s="17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H156" s="7" t="s">
         <v>129</v>
@@ -11745,7 +11748,7 @@
         <v>6</v>
       </c>
       <c r="T156" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U156" s="1" t="n">
         <v>404264</v>
@@ -11771,10 +11774,10 @@
         <v>53</v>
       </c>
       <c r="F157" s="17" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G157" s="17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H157" s="7" t="s">
         <v>131</v>
@@ -11813,7 +11816,7 @@
         <v>6</v>
       </c>
       <c r="T157" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U157" s="1" t="n">
         <v>404264</v>
@@ -11839,10 +11842,10 @@
         <v>53</v>
       </c>
       <c r="F158" s="17" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G158" s="17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H158" s="7" t="s">
         <v>133</v>
@@ -11881,7 +11884,7 @@
         <v>6</v>
       </c>
       <c r="T158" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U158" s="1" t="n">
         <v>404264</v>
@@ -11907,10 +11910,10 @@
         <v>53</v>
       </c>
       <c r="F159" s="17" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G159" s="17" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H159" s="7" t="s">
         <v>129</v>
@@ -11949,7 +11952,7 @@
         <v>6</v>
       </c>
       <c r="T159" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U159" s="1" t="n">
         <v>404264</v>
@@ -11975,10 +11978,10 @@
         <v>53</v>
       </c>
       <c r="F160" s="17" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G160" s="17" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H160" s="7" t="s">
         <v>131</v>
@@ -12017,7 +12020,7 @@
         <v>6</v>
       </c>
       <c r="T160" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U160" s="1" t="n">
         <v>404264</v>
@@ -12043,10 +12046,10 @@
         <v>53</v>
       </c>
       <c r="F161" s="17" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G161" s="17" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H161" s="7" t="s">
         <v>133</v>
@@ -12085,7 +12088,7 @@
         <v>6</v>
       </c>
       <c r="T161" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U161" s="1" t="n">
         <v>404264</v>
@@ -12111,10 +12114,10 @@
         <v>53</v>
       </c>
       <c r="F162" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G162" s="17" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H162" s="7" t="s">
         <v>129</v>
@@ -12153,7 +12156,7 @@
         <v>6</v>
       </c>
       <c r="T162" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U162" s="1" t="n">
         <v>404264</v>
@@ -12179,10 +12182,10 @@
         <v>53</v>
       </c>
       <c r="F163" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G163" s="17" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H163" s="7" t="s">
         <v>131</v>
@@ -12221,7 +12224,7 @@
         <v>6</v>
       </c>
       <c r="T163" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U163" s="1" t="n">
         <v>404264</v>
@@ -12247,10 +12250,10 @@
         <v>53</v>
       </c>
       <c r="F164" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G164" s="17" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H164" s="7" t="s">
         <v>133</v>
@@ -12289,7 +12292,7 @@
         <v>6</v>
       </c>
       <c r="T164" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U164" s="1" t="n">
         <v>404264</v>
@@ -12315,7 +12318,7 @@
         <v>53</v>
       </c>
       <c r="F165" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G165" s="17" t="s">
         <v>73</v>
@@ -12357,7 +12360,7 @@
         <v>6</v>
       </c>
       <c r="T165" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U165" s="1" t="n">
         <v>404264</v>
@@ -12383,7 +12386,7 @@
         <v>53</v>
       </c>
       <c r="F166" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G166" s="17" t="s">
         <v>73</v>
@@ -12425,7 +12428,7 @@
         <v>6</v>
       </c>
       <c r="T166" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U166" s="1" t="n">
         <v>404264</v>
@@ -12451,7 +12454,7 @@
         <v>53</v>
       </c>
       <c r="F167" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G167" s="17" t="s">
         <v>73</v>
@@ -12493,7 +12496,7 @@
         <v>6</v>
       </c>
       <c r="T167" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U167" s="1" t="n">
         <v>404264</v>
@@ -12519,10 +12522,10 @@
         <v>53</v>
       </c>
       <c r="F168" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G168" s="17" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H168" s="7" t="s">
         <v>129</v>
@@ -12561,7 +12564,7 @@
         <v>6</v>
       </c>
       <c r="T168" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U168" s="1" t="n">
         <v>404264</v>
@@ -12587,10 +12590,10 @@
         <v>53</v>
       </c>
       <c r="F169" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G169" s="17" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H169" s="7" t="s">
         <v>131</v>
@@ -12629,7 +12632,7 @@
         <v>6</v>
       </c>
       <c r="T169" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U169" s="1" t="n">
         <v>404264</v>
@@ -12655,10 +12658,10 @@
         <v>53</v>
       </c>
       <c r="F170" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G170" s="17" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H170" s="7" t="s">
         <v>133</v>
@@ -12697,7 +12700,7 @@
         <v>6</v>
       </c>
       <c r="T170" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U170" s="1" t="n">
         <v>404264</v>
@@ -12717,22 +12720,22 @@
         <v>10056</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E171" s="6" t="s">
         <v>53</v>
       </c>
       <c r="F171" s="17" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G171" s="17" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H171" s="7" t="s">
         <v>133</v>
       </c>
       <c r="I171" s="8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="J171" s="1" t="n">
         <v>286352</v>
@@ -12765,7 +12768,7 @@
         <v>7</v>
       </c>
       <c r="T171" s="17" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="U171" s="1" t="n">
         <v>404264</v>

</xml_diff>

<commit_message>
feat：update stage and tower excel
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Stage_关卡表.xlsx
+++ b/nevergiveup/Excel/Stage_关卡表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="246">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -431,6 +431,9 @@
   </si>
   <si>
     <t xml:space="preserve">0|0|-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1023|1||1|200||3|12</t>
   </si>
   <si>
     <t xml:space="preserve">1023|1||1|300||3|12</t>
@@ -1224,10 +1227,10 @@
   </sheetPr>
   <dimension ref="A1:V171"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="P21" activeCellId="0" sqref="P21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="N31" activeCellId="0" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.48828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2550,19 +2553,19 @@
         <v>1</v>
       </c>
       <c r="N21" s="11" t="s">
-        <v>60</v>
+        <v>137</v>
       </c>
       <c r="O21" s="11" t="s">
         <v>61</v>
       </c>
       <c r="P21" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="Q21" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S21" s="14" t="n">
         <v>2</v>
@@ -2730,10 +2733,10 @@
         <v>53</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>58</v>
@@ -2763,10 +2766,10 @@
         <v>62</v>
       </c>
       <c r="Q24" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R24" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S24" s="1" t="n">
         <v>2</v>
@@ -2798,10 +2801,10 @@
         <v>53</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>66</v>
@@ -2866,10 +2869,10 @@
         <v>53</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>74</v>
@@ -2934,10 +2937,10 @@
         <v>53</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>58</v>
@@ -2967,10 +2970,10 @@
         <v>62</v>
       </c>
       <c r="Q27" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S27" s="1" t="n">
         <v>2</v>
@@ -3002,10 +3005,10 @@
         <v>53</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>66</v>
@@ -3070,10 +3073,10 @@
         <v>53</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>74</v>
@@ -3138,10 +3141,10 @@
         <v>53</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>58</v>
@@ -3171,10 +3174,10 @@
         <v>62</v>
       </c>
       <c r="Q30" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R30" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S30" s="1" t="n">
         <v>2</v>
@@ -3206,10 +3209,10 @@
         <v>53</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>66</v>
@@ -3274,10 +3277,10 @@
         <v>53</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>74</v>
@@ -3342,10 +3345,10 @@
         <v>53</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>58</v>
@@ -3375,10 +3378,10 @@
         <v>62</v>
       </c>
       <c r="Q33" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R33" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S33" s="1" t="n">
         <v>2</v>
@@ -3410,10 +3413,10 @@
         <v>53</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>66</v>
@@ -3478,10 +3481,10 @@
         <v>53</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>74</v>
@@ -3546,10 +3549,10 @@
         <v>53</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>58</v>
@@ -3579,10 +3582,10 @@
         <v>62</v>
       </c>
       <c r="Q36" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R36" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S36" s="1" t="n">
         <v>2</v>
@@ -3614,10 +3617,10 @@
         <v>53</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>66</v>
@@ -3682,10 +3685,10 @@
         <v>53</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>74</v>
@@ -3750,10 +3753,10 @@
         <v>53</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H39" s="7" t="s">
         <v>58</v>
@@ -3783,10 +3786,10 @@
         <v>62</v>
       </c>
       <c r="Q39" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R39" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S39" s="1" t="n">
         <v>2</v>
@@ -3818,10 +3821,10 @@
         <v>53</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>66</v>
@@ -3886,10 +3889,10 @@
         <v>53</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>74</v>
@@ -3954,10 +3957,10 @@
         <v>53</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H42" s="7" t="s">
         <v>58</v>
@@ -3987,10 +3990,10 @@
         <v>62</v>
       </c>
       <c r="Q42" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R42" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S42" s="1" t="n">
         <v>2</v>
@@ -4022,10 +4025,10 @@
         <v>53</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>66</v>
@@ -4090,10 +4093,10 @@
         <v>53</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H44" s="7" t="s">
         <v>74</v>
@@ -4158,10 +4161,10 @@
         <v>53</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>58</v>
@@ -4191,10 +4194,10 @@
         <v>62</v>
       </c>
       <c r="Q45" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R45" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S45" s="1" t="n">
         <v>2</v>
@@ -4226,10 +4229,10 @@
         <v>53</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>66</v>
@@ -4294,10 +4297,10 @@
         <v>53</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>74</v>
@@ -4362,10 +4365,10 @@
         <v>53</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H48" s="7" t="s">
         <v>58</v>
@@ -4395,10 +4398,10 @@
         <v>62</v>
       </c>
       <c r="Q48" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R48" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S48" s="1" t="n">
         <v>2</v>
@@ -4430,10 +4433,10 @@
         <v>53</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>66</v>
@@ -4498,10 +4501,10 @@
         <v>53</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H50" s="12" t="s">
         <v>74</v>
@@ -4566,10 +4569,10 @@
         <v>53</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H51" s="7" t="s">
         <v>83</v>
@@ -4608,7 +4611,7 @@
         <v>3</v>
       </c>
       <c r="T51" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U51" s="1" t="n">
         <v>404267</v>
@@ -4634,10 +4637,10 @@
         <v>53</v>
       </c>
       <c r="F52" s="17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H52" s="7" t="s">
         <v>90</v>
@@ -4676,7 +4679,7 @@
         <v>3</v>
       </c>
       <c r="T52" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U52" s="1" t="n">
         <v>404267</v>
@@ -4702,10 +4705,10 @@
         <v>53</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>95</v>
@@ -4744,7 +4747,7 @@
         <v>3</v>
       </c>
       <c r="T53" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U53" s="1" t="n">
         <v>404267</v>
@@ -4770,10 +4773,10 @@
         <v>53</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G54" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>83</v>
@@ -4812,7 +4815,7 @@
         <v>3</v>
       </c>
       <c r="T54" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U54" s="1" t="n">
         <v>404267</v>
@@ -4838,10 +4841,10 @@
         <v>53</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G55" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>90</v>
@@ -4880,7 +4883,7 @@
         <v>3</v>
       </c>
       <c r="T55" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U55" s="1" t="n">
         <v>404267</v>
@@ -4906,10 +4909,10 @@
         <v>53</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G56" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>95</v>
@@ -4948,7 +4951,7 @@
         <v>3</v>
       </c>
       <c r="T56" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U56" s="1" t="n">
         <v>404267</v>
@@ -4974,10 +4977,10 @@
         <v>53</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G57" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>83</v>
@@ -5016,7 +5019,7 @@
         <v>3</v>
       </c>
       <c r="T57" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U57" s="1" t="n">
         <v>404267</v>
@@ -5042,10 +5045,10 @@
         <v>53</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G58" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H58" s="7" t="s">
         <v>90</v>
@@ -5084,7 +5087,7 @@
         <v>3</v>
       </c>
       <c r="T58" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U58" s="1" t="n">
         <v>404267</v>
@@ -5110,10 +5113,10 @@
         <v>53</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G59" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H59" s="7" t="s">
         <v>95</v>
@@ -5152,7 +5155,7 @@
         <v>3</v>
       </c>
       <c r="T59" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U59" s="1" t="n">
         <v>404267</v>
@@ -5178,10 +5181,10 @@
         <v>53</v>
       </c>
       <c r="F60" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G60" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>83</v>
@@ -5220,7 +5223,7 @@
         <v>3</v>
       </c>
       <c r="T60" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U60" s="1" t="n">
         <v>404267</v>
@@ -5246,10 +5249,10 @@
         <v>53</v>
       </c>
       <c r="F61" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G61" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>90</v>
@@ -5288,7 +5291,7 @@
         <v>3</v>
       </c>
       <c r="T61" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U61" s="1" t="n">
         <v>404267</v>
@@ -5314,10 +5317,10 @@
         <v>53</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G62" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H62" s="7" t="s">
         <v>95</v>
@@ -5356,7 +5359,7 @@
         <v>3</v>
       </c>
       <c r="T62" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U62" s="1" t="n">
         <v>404267</v>
@@ -5382,10 +5385,10 @@
         <v>53</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H63" s="7" t="s">
         <v>83</v>
@@ -5424,7 +5427,7 @@
         <v>3</v>
       </c>
       <c r="T63" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U63" s="1" t="n">
         <v>404267</v>
@@ -5450,10 +5453,10 @@
         <v>53</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G64" s="18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H64" s="7" t="s">
         <v>90</v>
@@ -5492,7 +5495,7 @@
         <v>3</v>
       </c>
       <c r="T64" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U64" s="1" t="n">
         <v>404267</v>
@@ -5518,10 +5521,10 @@
         <v>53</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H65" s="7" t="s">
         <v>95</v>
@@ -5560,7 +5563,7 @@
         <v>3</v>
       </c>
       <c r="T65" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U65" s="1" t="n">
         <v>404267</v>
@@ -5586,10 +5589,10 @@
         <v>53</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H66" s="7" t="s">
         <v>83</v>
@@ -5628,7 +5631,7 @@
         <v>3</v>
       </c>
       <c r="T66" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U66" s="1" t="n">
         <v>404267</v>
@@ -5654,10 +5657,10 @@
         <v>53</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G67" s="18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H67" s="7" t="s">
         <v>90</v>
@@ -5696,7 +5699,7 @@
         <v>3</v>
       </c>
       <c r="T67" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U67" s="1" t="n">
         <v>404267</v>
@@ -5722,10 +5725,10 @@
         <v>53</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G68" s="18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H68" s="7" t="s">
         <v>95</v>
@@ -5764,7 +5767,7 @@
         <v>3</v>
       </c>
       <c r="T68" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U68" s="1" t="n">
         <v>404267</v>
@@ -5790,10 +5793,10 @@
         <v>53</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G69" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H69" s="7" t="s">
         <v>83</v>
@@ -5832,7 +5835,7 @@
         <v>3</v>
       </c>
       <c r="T69" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U69" s="1" t="n">
         <v>404267</v>
@@ -5858,10 +5861,10 @@
         <v>53</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G70" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H70" s="7" t="s">
         <v>90</v>
@@ -5900,7 +5903,7 @@
         <v>3</v>
       </c>
       <c r="T70" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U70" s="1" t="n">
         <v>404267</v>
@@ -5926,10 +5929,10 @@
         <v>53</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G71" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H71" s="7" t="s">
         <v>95</v>
@@ -5968,7 +5971,7 @@
         <v>3</v>
       </c>
       <c r="T71" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U71" s="1" t="n">
         <v>404267</v>
@@ -5994,10 +5997,10 @@
         <v>53</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G72" s="18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H72" s="7" t="s">
         <v>83</v>
@@ -6036,7 +6039,7 @@
         <v>3</v>
       </c>
       <c r="T72" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U72" s="1" t="n">
         <v>404267</v>
@@ -6062,10 +6065,10 @@
         <v>53</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G73" s="18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H73" s="7" t="s">
         <v>90</v>
@@ -6104,7 +6107,7 @@
         <v>3</v>
       </c>
       <c r="T73" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U73" s="1" t="n">
         <v>404267</v>
@@ -6130,10 +6133,10 @@
         <v>53</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G74" s="18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H74" s="7" t="s">
         <v>95</v>
@@ -6172,7 +6175,7 @@
         <v>3</v>
       </c>
       <c r="T74" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U74" s="1" t="n">
         <v>404267</v>
@@ -6198,10 +6201,10 @@
         <v>53</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G75" s="18" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H75" s="7" t="s">
         <v>83</v>
@@ -6240,7 +6243,7 @@
         <v>3</v>
       </c>
       <c r="T75" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U75" s="1" t="n">
         <v>404267</v>
@@ -6266,10 +6269,10 @@
         <v>53</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G76" s="18" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H76" s="7" t="s">
         <v>90</v>
@@ -6308,7 +6311,7 @@
         <v>3</v>
       </c>
       <c r="T76" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U76" s="1" t="n">
         <v>404267</v>
@@ -6334,10 +6337,10 @@
         <v>53</v>
       </c>
       <c r="F77" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G77" s="18" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H77" s="7" t="s">
         <v>95</v>
@@ -6376,7 +6379,7 @@
         <v>3</v>
       </c>
       <c r="T77" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U77" s="1" t="n">
         <v>404267</v>
@@ -6402,7 +6405,7 @@
         <v>53</v>
       </c>
       <c r="F78" s="17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G78" s="18" t="s">
         <v>73</v>
@@ -6444,7 +6447,7 @@
         <v>3</v>
       </c>
       <c r="T78" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U78" s="1" t="n">
         <v>404267</v>
@@ -6470,7 +6473,7 @@
         <v>53</v>
       </c>
       <c r="F79" s="17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G79" s="18" t="s">
         <v>73</v>
@@ -6512,7 +6515,7 @@
         <v>3</v>
       </c>
       <c r="T79" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U79" s="1" t="n">
         <v>404267</v>
@@ -6538,7 +6541,7 @@
         <v>53</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G80" s="20" t="s">
         <v>73</v>
@@ -6580,7 +6583,7 @@
         <v>3</v>
       </c>
       <c r="T80" s="14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U80" s="14" t="n">
         <v>404267</v>
@@ -6606,10 +6609,10 @@
         <v>53</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G81" s="18" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H81" s="7" t="s">
         <v>102</v>
@@ -6648,7 +6651,7 @@
         <v>4</v>
       </c>
       <c r="T81" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U81" s="1" t="n">
         <v>404269</v>
@@ -6674,10 +6677,10 @@
         <v>53</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G82" s="18" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H82" s="7" t="s">
         <v>107</v>
@@ -6716,7 +6719,7 @@
         <v>4</v>
       </c>
       <c r="T82" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U82" s="1" t="n">
         <v>404269</v>
@@ -6742,10 +6745,10 @@
         <v>53</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G83" s="18" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H83" s="7" t="s">
         <v>112</v>
@@ -6784,7 +6787,7 @@
         <v>4</v>
       </c>
       <c r="T83" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U83" s="1" t="n">
         <v>404269</v>
@@ -6810,10 +6813,10 @@
         <v>53</v>
       </c>
       <c r="F84" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G84" s="18" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H84" s="7" t="s">
         <v>102</v>
@@ -6852,7 +6855,7 @@
         <v>4</v>
       </c>
       <c r="T84" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U84" s="1" t="n">
         <v>404269</v>
@@ -6878,10 +6881,10 @@
         <v>53</v>
       </c>
       <c r="F85" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G85" s="18" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H85" s="7" t="s">
         <v>107</v>
@@ -6920,7 +6923,7 @@
         <v>4</v>
       </c>
       <c r="T85" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U85" s="1" t="n">
         <v>404269</v>
@@ -6946,10 +6949,10 @@
         <v>53</v>
       </c>
       <c r="F86" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G86" s="18" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H86" s="7" t="s">
         <v>112</v>
@@ -6988,7 +6991,7 @@
         <v>4</v>
       </c>
       <c r="T86" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U86" s="1" t="n">
         <v>404269</v>
@@ -7014,10 +7017,10 @@
         <v>53</v>
       </c>
       <c r="F87" s="17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G87" s="18" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H87" s="7" t="s">
         <v>102</v>
@@ -7056,7 +7059,7 @@
         <v>4</v>
       </c>
       <c r="T87" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U87" s="1" t="n">
         <v>404269</v>
@@ -7082,10 +7085,10 @@
         <v>53</v>
       </c>
       <c r="F88" s="17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G88" s="18" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H88" s="7" t="s">
         <v>107</v>
@@ -7124,7 +7127,7 @@
         <v>4</v>
       </c>
       <c r="T88" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U88" s="1" t="n">
         <v>404269</v>
@@ -7150,10 +7153,10 @@
         <v>53</v>
       </c>
       <c r="F89" s="17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G89" s="18" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H89" s="7" t="s">
         <v>112</v>
@@ -7192,7 +7195,7 @@
         <v>4</v>
       </c>
       <c r="T89" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U89" s="1" t="n">
         <v>404269</v>
@@ -7218,10 +7221,10 @@
         <v>53</v>
       </c>
       <c r="F90" s="17" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G90" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H90" s="7" t="s">
         <v>102</v>
@@ -7260,7 +7263,7 @@
         <v>4</v>
       </c>
       <c r="T90" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U90" s="1" t="n">
         <v>404269</v>
@@ -7286,10 +7289,10 @@
         <v>53</v>
       </c>
       <c r="F91" s="17" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G91" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H91" s="7" t="s">
         <v>107</v>
@@ -7328,7 +7331,7 @@
         <v>4</v>
       </c>
       <c r="T91" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U91" s="1" t="n">
         <v>404269</v>
@@ -7354,10 +7357,10 @@
         <v>53</v>
       </c>
       <c r="F92" s="17" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G92" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H92" s="7" t="s">
         <v>112</v>
@@ -7396,7 +7399,7 @@
         <v>4</v>
       </c>
       <c r="T92" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U92" s="1" t="n">
         <v>404269</v>
@@ -7422,10 +7425,10 @@
         <v>53</v>
       </c>
       <c r="F93" s="17" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G93" s="18" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H93" s="7" t="s">
         <v>102</v>
@@ -7464,7 +7467,7 @@
         <v>4</v>
       </c>
       <c r="T93" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U93" s="1" t="n">
         <v>404269</v>
@@ -7490,10 +7493,10 @@
         <v>53</v>
       </c>
       <c r="F94" s="17" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G94" s="18" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H94" s="7" t="s">
         <v>107</v>
@@ -7532,7 +7535,7 @@
         <v>4</v>
       </c>
       <c r="T94" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U94" s="1" t="n">
         <v>404269</v>
@@ -7558,10 +7561,10 @@
         <v>53</v>
       </c>
       <c r="F95" s="17" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G95" s="18" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H95" s="7" t="s">
         <v>112</v>
@@ -7600,7 +7603,7 @@
         <v>4</v>
       </c>
       <c r="T95" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U95" s="1" t="n">
         <v>404269</v>
@@ -7626,10 +7629,10 @@
         <v>53</v>
       </c>
       <c r="F96" s="17" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G96" s="18" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H96" s="7" t="s">
         <v>102</v>
@@ -7668,7 +7671,7 @@
         <v>4</v>
       </c>
       <c r="T96" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U96" s="1" t="n">
         <v>404269</v>
@@ -7694,10 +7697,10 @@
         <v>53</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G97" s="18" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H97" s="7" t="s">
         <v>107</v>
@@ -7736,7 +7739,7 @@
         <v>4</v>
       </c>
       <c r="T97" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U97" s="1" t="n">
         <v>404269</v>
@@ -7762,10 +7765,10 @@
         <v>53</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G98" s="18" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H98" s="7" t="s">
         <v>112</v>
@@ -7804,7 +7807,7 @@
         <v>4</v>
       </c>
       <c r="T98" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U98" s="1" t="n">
         <v>404269</v>
@@ -7830,10 +7833,10 @@
         <v>53</v>
       </c>
       <c r="F99" s="17" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G99" s="18" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H99" s="7" t="s">
         <v>102</v>
@@ -7872,7 +7875,7 @@
         <v>4</v>
       </c>
       <c r="T99" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U99" s="1" t="n">
         <v>404269</v>
@@ -7898,10 +7901,10 @@
         <v>53</v>
       </c>
       <c r="F100" s="17" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G100" s="18" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H100" s="7" t="s">
         <v>107</v>
@@ -7940,7 +7943,7 @@
         <v>4</v>
       </c>
       <c r="T100" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U100" s="1" t="n">
         <v>404269</v>
@@ -7966,10 +7969,10 @@
         <v>53</v>
       </c>
       <c r="F101" s="17" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G101" s="18" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H101" s="7" t="s">
         <v>112</v>
@@ -8008,7 +8011,7 @@
         <v>4</v>
       </c>
       <c r="T101" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U101" s="1" t="n">
         <v>404269</v>
@@ -8034,10 +8037,10 @@
         <v>53</v>
       </c>
       <c r="F102" s="17" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G102" s="18" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H102" s="7" t="s">
         <v>102</v>
@@ -8076,7 +8079,7 @@
         <v>4</v>
       </c>
       <c r="T102" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U102" s="1" t="n">
         <v>404269</v>
@@ -8102,10 +8105,10 @@
         <v>53</v>
       </c>
       <c r="F103" s="17" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G103" s="18" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H103" s="7" t="s">
         <v>107</v>
@@ -8144,7 +8147,7 @@
         <v>4</v>
       </c>
       <c r="T103" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U103" s="1" t="n">
         <v>404269</v>
@@ -8170,10 +8173,10 @@
         <v>53</v>
       </c>
       <c r="F104" s="17" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G104" s="18" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H104" s="7" t="s">
         <v>112</v>
@@ -8212,7 +8215,7 @@
         <v>4</v>
       </c>
       <c r="T104" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U104" s="1" t="n">
         <v>404269</v>
@@ -8238,10 +8241,10 @@
         <v>53</v>
       </c>
       <c r="F105" s="17" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G105" s="18" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H105" s="7" t="s">
         <v>102</v>
@@ -8280,7 +8283,7 @@
         <v>4</v>
       </c>
       <c r="T105" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U105" s="1" t="n">
         <v>404269</v>
@@ -8306,10 +8309,10 @@
         <v>53</v>
       </c>
       <c r="F106" s="17" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G106" s="18" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H106" s="7" t="s">
         <v>107</v>
@@ -8348,7 +8351,7 @@
         <v>4</v>
       </c>
       <c r="T106" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U106" s="1" t="n">
         <v>404269</v>
@@ -8374,10 +8377,10 @@
         <v>53</v>
       </c>
       <c r="F107" s="17" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G107" s="18" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H107" s="7" t="s">
         <v>112</v>
@@ -8416,7 +8419,7 @@
         <v>4</v>
       </c>
       <c r="T107" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U107" s="1" t="n">
         <v>404269</v>
@@ -8442,10 +8445,10 @@
         <v>53</v>
       </c>
       <c r="F108" s="17" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G108" s="18" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H108" s="7" t="s">
         <v>102</v>
@@ -8484,7 +8487,7 @@
         <v>4</v>
       </c>
       <c r="T108" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U108" s="1" t="n">
         <v>404269</v>
@@ -8510,10 +8513,10 @@
         <v>53</v>
       </c>
       <c r="F109" s="17" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G109" s="18" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H109" s="7" t="s">
         <v>107</v>
@@ -8552,7 +8555,7 @@
         <v>4</v>
       </c>
       <c r="T109" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U109" s="1" t="n">
         <v>404269</v>
@@ -8578,10 +8581,10 @@
         <v>53</v>
       </c>
       <c r="F110" s="19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G110" s="20" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H110" s="12" t="s">
         <v>112</v>
@@ -8620,7 +8623,7 @@
         <v>4</v>
       </c>
       <c r="T110" s="14" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U110" s="14" t="n">
         <v>404269</v>
@@ -8646,10 +8649,10 @@
         <v>53</v>
       </c>
       <c r="F111" s="17" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G111" s="18" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H111" s="7" t="s">
         <v>121</v>
@@ -8688,7 +8691,7 @@
         <v>5</v>
       </c>
       <c r="T111" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U111" s="1" t="n">
         <v>404266</v>
@@ -8714,10 +8717,10 @@
         <v>53</v>
       </c>
       <c r="F112" s="17" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G112" s="18" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H112" s="7" t="s">
         <v>123</v>
@@ -8756,7 +8759,7 @@
         <v>5</v>
       </c>
       <c r="T112" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U112" s="1" t="n">
         <v>404266</v>
@@ -8782,10 +8785,10 @@
         <v>53</v>
       </c>
       <c r="F113" s="17" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G113" s="18" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H113" s="7" t="s">
         <v>125</v>
@@ -8824,7 +8827,7 @@
         <v>5</v>
       </c>
       <c r="T113" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U113" s="1" t="n">
         <v>404266</v>
@@ -8850,10 +8853,10 @@
         <v>53</v>
       </c>
       <c r="F114" s="17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G114" s="18" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H114" s="7" t="s">
         <v>121</v>
@@ -8892,7 +8895,7 @@
         <v>5</v>
       </c>
       <c r="T114" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U114" s="1" t="n">
         <v>404266</v>
@@ -8918,10 +8921,10 @@
         <v>53</v>
       </c>
       <c r="F115" s="17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G115" s="18" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H115" s="7" t="s">
         <v>123</v>
@@ -8960,7 +8963,7 @@
         <v>5</v>
       </c>
       <c r="T115" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U115" s="1" t="n">
         <v>404266</v>
@@ -8986,10 +8989,10 @@
         <v>53</v>
       </c>
       <c r="F116" s="17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G116" s="18" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H116" s="7" t="s">
         <v>125</v>
@@ -9028,7 +9031,7 @@
         <v>5</v>
       </c>
       <c r="T116" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U116" s="1" t="n">
         <v>404266</v>
@@ -9054,10 +9057,10 @@
         <v>53</v>
       </c>
       <c r="F117" s="17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G117" s="18" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H117" s="7" t="s">
         <v>121</v>
@@ -9096,7 +9099,7 @@
         <v>5</v>
       </c>
       <c r="T117" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U117" s="1" t="n">
         <v>404266</v>
@@ -9122,10 +9125,10 @@
         <v>53</v>
       </c>
       <c r="F118" s="17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G118" s="18" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H118" s="7" t="s">
         <v>123</v>
@@ -9164,7 +9167,7 @@
         <v>5</v>
       </c>
       <c r="T118" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U118" s="1" t="n">
         <v>404266</v>
@@ -9190,10 +9193,10 @@
         <v>53</v>
       </c>
       <c r="F119" s="17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G119" s="18" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H119" s="7" t="s">
         <v>125</v>
@@ -9232,7 +9235,7 @@
         <v>5</v>
       </c>
       <c r="T119" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U119" s="1" t="n">
         <v>404266</v>
@@ -9258,10 +9261,10 @@
         <v>53</v>
       </c>
       <c r="F120" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G120" s="18" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H120" s="7" t="s">
         <v>121</v>
@@ -9300,7 +9303,7 @@
         <v>5</v>
       </c>
       <c r="T120" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U120" s="1" t="n">
         <v>404266</v>
@@ -9326,10 +9329,10 @@
         <v>53</v>
       </c>
       <c r="F121" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G121" s="18" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H121" s="7" t="s">
         <v>123</v>
@@ -9368,7 +9371,7 @@
         <v>5</v>
       </c>
       <c r="T121" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U121" s="1" t="n">
         <v>404266</v>
@@ -9394,10 +9397,10 @@
         <v>53</v>
       </c>
       <c r="F122" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G122" s="18" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H122" s="7" t="s">
         <v>125</v>
@@ -9436,7 +9439,7 @@
         <v>5</v>
       </c>
       <c r="T122" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U122" s="1" t="n">
         <v>404266</v>
@@ -9462,10 +9465,10 @@
         <v>53</v>
       </c>
       <c r="F123" s="17" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G123" s="18" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H123" s="7" t="s">
         <v>121</v>
@@ -9504,7 +9507,7 @@
         <v>5</v>
       </c>
       <c r="T123" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U123" s="1" t="n">
         <v>404266</v>
@@ -9530,10 +9533,10 @@
         <v>53</v>
       </c>
       <c r="F124" s="17" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G124" s="18" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H124" s="7" t="s">
         <v>123</v>
@@ -9572,7 +9575,7 @@
         <v>5</v>
       </c>
       <c r="T124" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U124" s="1" t="n">
         <v>404266</v>
@@ -9598,10 +9601,10 @@
         <v>53</v>
       </c>
       <c r="F125" s="17" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G125" s="18" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H125" s="7" t="s">
         <v>125</v>
@@ -9640,7 +9643,7 @@
         <v>5</v>
       </c>
       <c r="T125" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U125" s="1" t="n">
         <v>404266</v>
@@ -9666,10 +9669,10 @@
         <v>53</v>
       </c>
       <c r="F126" s="17" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G126" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H126" s="7" t="s">
         <v>121</v>
@@ -9708,7 +9711,7 @@
         <v>5</v>
       </c>
       <c r="T126" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U126" s="1" t="n">
         <v>404266</v>
@@ -9734,10 +9737,10 @@
         <v>53</v>
       </c>
       <c r="F127" s="17" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G127" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H127" s="7" t="s">
         <v>123</v>
@@ -9776,7 +9779,7 @@
         <v>5</v>
       </c>
       <c r="T127" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U127" s="1" t="n">
         <v>404266</v>
@@ -9802,10 +9805,10 @@
         <v>53</v>
       </c>
       <c r="F128" s="17" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G128" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H128" s="7" t="s">
         <v>125</v>
@@ -9844,7 +9847,7 @@
         <v>5</v>
       </c>
       <c r="T128" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U128" s="1" t="n">
         <v>404266</v>
@@ -9870,10 +9873,10 @@
         <v>53</v>
       </c>
       <c r="F129" s="17" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G129" s="18" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H129" s="7" t="s">
         <v>121</v>
@@ -9912,7 +9915,7 @@
         <v>5</v>
       </c>
       <c r="T129" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U129" s="1" t="n">
         <v>404266</v>
@@ -9938,10 +9941,10 @@
         <v>53</v>
       </c>
       <c r="F130" s="17" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G130" s="18" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H130" s="7" t="s">
         <v>123</v>
@@ -9980,7 +9983,7 @@
         <v>5</v>
       </c>
       <c r="T130" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U130" s="1" t="n">
         <v>404266</v>
@@ -10006,10 +10009,10 @@
         <v>53</v>
       </c>
       <c r="F131" s="17" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G131" s="18" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H131" s="7" t="s">
         <v>125</v>
@@ -10048,7 +10051,7 @@
         <v>5</v>
       </c>
       <c r="T131" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U131" s="1" t="n">
         <v>404266</v>
@@ -10074,10 +10077,10 @@
         <v>53</v>
       </c>
       <c r="F132" s="17" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G132" s="18" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H132" s="7" t="s">
         <v>121</v>
@@ -10116,7 +10119,7 @@
         <v>5</v>
       </c>
       <c r="T132" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U132" s="1" t="n">
         <v>404266</v>
@@ -10142,10 +10145,10 @@
         <v>53</v>
       </c>
       <c r="F133" s="17" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G133" s="18" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H133" s="7" t="s">
         <v>123</v>
@@ -10184,7 +10187,7 @@
         <v>5</v>
       </c>
       <c r="T133" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U133" s="1" t="n">
         <v>404266</v>
@@ -10210,10 +10213,10 @@
         <v>53</v>
       </c>
       <c r="F134" s="17" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G134" s="18" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H134" s="7" t="s">
         <v>125</v>
@@ -10252,7 +10255,7 @@
         <v>5</v>
       </c>
       <c r="T134" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U134" s="1" t="n">
         <v>404266</v>
@@ -10278,10 +10281,10 @@
         <v>53</v>
       </c>
       <c r="F135" s="17" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G135" s="18" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H135" s="7" t="s">
         <v>121</v>
@@ -10320,7 +10323,7 @@
         <v>5</v>
       </c>
       <c r="T135" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U135" s="1" t="n">
         <v>404266</v>
@@ -10346,10 +10349,10 @@
         <v>53</v>
       </c>
       <c r="F136" s="17" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G136" s="18" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H136" s="7" t="s">
         <v>123</v>
@@ -10388,7 +10391,7 @@
         <v>5</v>
       </c>
       <c r="T136" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U136" s="1" t="n">
         <v>404266</v>
@@ -10414,10 +10417,10 @@
         <v>53</v>
       </c>
       <c r="F137" s="17" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G137" s="18" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H137" s="7" t="s">
         <v>125</v>
@@ -10456,7 +10459,7 @@
         <v>5</v>
       </c>
       <c r="T137" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U137" s="1" t="n">
         <v>404266</v>
@@ -10482,10 +10485,10 @@
         <v>53</v>
       </c>
       <c r="F138" s="17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G138" s="18" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H138" s="7" t="s">
         <v>121</v>
@@ -10524,7 +10527,7 @@
         <v>5</v>
       </c>
       <c r="T138" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U138" s="1" t="n">
         <v>404266</v>
@@ -10550,10 +10553,10 @@
         <v>53</v>
       </c>
       <c r="F139" s="17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G139" s="18" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H139" s="7" t="s">
         <v>123</v>
@@ -10592,7 +10595,7 @@
         <v>5</v>
       </c>
       <c r="T139" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U139" s="1" t="n">
         <v>404266</v>
@@ -10618,10 +10621,10 @@
         <v>53</v>
       </c>
       <c r="F140" s="19" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G140" s="20" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H140" s="12" t="s">
         <v>125</v>
@@ -10660,7 +10663,7 @@
         <v>5</v>
       </c>
       <c r="T140" s="14" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U140" s="14" t="n">
         <v>404266</v>
@@ -10686,10 +10689,10 @@
         <v>53</v>
       </c>
       <c r="F141" s="17" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G141" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H141" s="7" t="s">
         <v>129</v>
@@ -10728,7 +10731,7 @@
         <v>6</v>
       </c>
       <c r="T141" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U141" s="1" t="n">
         <v>404264</v>
@@ -10754,10 +10757,10 @@
         <v>53</v>
       </c>
       <c r="F142" s="17" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G142" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H142" s="7" t="s">
         <v>131</v>
@@ -10796,7 +10799,7 @@
         <v>6</v>
       </c>
       <c r="T142" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U142" s="1" t="n">
         <v>404264</v>
@@ -10822,10 +10825,10 @@
         <v>53</v>
       </c>
       <c r="F143" s="17" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G143" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H143" s="7" t="s">
         <v>133</v>
@@ -10864,7 +10867,7 @@
         <v>6</v>
       </c>
       <c r="T143" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U143" s="1" t="n">
         <v>404264</v>
@@ -10890,10 +10893,10 @@
         <v>53</v>
       </c>
       <c r="F144" s="17" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G144" s="18" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H144" s="7" t="s">
         <v>129</v>
@@ -10932,7 +10935,7 @@
         <v>6</v>
       </c>
       <c r="T144" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U144" s="1" t="n">
         <v>404264</v>
@@ -10958,10 +10961,10 @@
         <v>53</v>
       </c>
       <c r="F145" s="17" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G145" s="18" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H145" s="7" t="s">
         <v>131</v>
@@ -11000,7 +11003,7 @@
         <v>6</v>
       </c>
       <c r="T145" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U145" s="1" t="n">
         <v>404264</v>
@@ -11026,10 +11029,10 @@
         <v>53</v>
       </c>
       <c r="F146" s="17" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G146" s="18" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H146" s="7" t="s">
         <v>133</v>
@@ -11068,7 +11071,7 @@
         <v>6</v>
       </c>
       <c r="T146" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U146" s="1" t="n">
         <v>404264</v>
@@ -11094,10 +11097,10 @@
         <v>53</v>
       </c>
       <c r="F147" s="17" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G147" s="18" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H147" s="7" t="s">
         <v>129</v>
@@ -11136,7 +11139,7 @@
         <v>6</v>
       </c>
       <c r="T147" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U147" s="1" t="n">
         <v>404264</v>
@@ -11162,10 +11165,10 @@
         <v>53</v>
       </c>
       <c r="F148" s="17" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G148" s="18" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H148" s="7" t="s">
         <v>131</v>
@@ -11204,7 +11207,7 @@
         <v>6</v>
       </c>
       <c r="T148" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U148" s="1" t="n">
         <v>404264</v>
@@ -11230,10 +11233,10 @@
         <v>53</v>
       </c>
       <c r="F149" s="17" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G149" s="18" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H149" s="7" t="s">
         <v>133</v>
@@ -11272,7 +11275,7 @@
         <v>6</v>
       </c>
       <c r="T149" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U149" s="1" t="n">
         <v>404264</v>
@@ -11298,10 +11301,10 @@
         <v>53</v>
       </c>
       <c r="F150" s="17" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G150" s="18" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H150" s="7" t="s">
         <v>129</v>
@@ -11340,7 +11343,7 @@
         <v>6</v>
       </c>
       <c r="T150" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U150" s="1" t="n">
         <v>404264</v>
@@ -11366,10 +11369,10 @@
         <v>53</v>
       </c>
       <c r="F151" s="17" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G151" s="18" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H151" s="7" t="s">
         <v>131</v>
@@ -11408,7 +11411,7 @@
         <v>6</v>
       </c>
       <c r="T151" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U151" s="1" t="n">
         <v>404264</v>
@@ -11434,10 +11437,10 @@
         <v>53</v>
       </c>
       <c r="F152" s="17" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G152" s="18" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H152" s="7" t="s">
         <v>133</v>
@@ -11476,7 +11479,7 @@
         <v>6</v>
       </c>
       <c r="T152" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U152" s="1" t="n">
         <v>404264</v>
@@ -11502,10 +11505,10 @@
         <v>53</v>
       </c>
       <c r="F153" s="17" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G153" s="18" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H153" s="7" t="s">
         <v>129</v>
@@ -11544,7 +11547,7 @@
         <v>6</v>
       </c>
       <c r="T153" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U153" s="1" t="n">
         <v>404264</v>
@@ -11570,10 +11573,10 @@
         <v>53</v>
       </c>
       <c r="F154" s="17" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G154" s="18" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H154" s="7" t="s">
         <v>131</v>
@@ -11612,7 +11615,7 @@
         <v>6</v>
       </c>
       <c r="T154" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U154" s="1" t="n">
         <v>404264</v>
@@ -11638,10 +11641,10 @@
         <v>53</v>
       </c>
       <c r="F155" s="17" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G155" s="18" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H155" s="7" t="s">
         <v>133</v>
@@ -11680,7 +11683,7 @@
         <v>6</v>
       </c>
       <c r="T155" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U155" s="1" t="n">
         <v>404264</v>
@@ -11706,10 +11709,10 @@
         <v>53</v>
       </c>
       <c r="F156" s="17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G156" s="17" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H156" s="7" t="s">
         <v>129</v>
@@ -11748,7 +11751,7 @@
         <v>6</v>
       </c>
       <c r="T156" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U156" s="1" t="n">
         <v>404264</v>
@@ -11774,10 +11777,10 @@
         <v>53</v>
       </c>
       <c r="F157" s="17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G157" s="17" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H157" s="7" t="s">
         <v>131</v>
@@ -11816,7 +11819,7 @@
         <v>6</v>
       </c>
       <c r="T157" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U157" s="1" t="n">
         <v>404264</v>
@@ -11842,10 +11845,10 @@
         <v>53</v>
       </c>
       <c r="F158" s="17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G158" s="17" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H158" s="7" t="s">
         <v>133</v>
@@ -11884,7 +11887,7 @@
         <v>6</v>
       </c>
       <c r="T158" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U158" s="1" t="n">
         <v>404264</v>
@@ -11910,10 +11913,10 @@
         <v>53</v>
       </c>
       <c r="F159" s="17" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G159" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H159" s="7" t="s">
         <v>129</v>
@@ -11952,7 +11955,7 @@
         <v>6</v>
       </c>
       <c r="T159" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U159" s="1" t="n">
         <v>404264</v>
@@ -11978,10 +11981,10 @@
         <v>53</v>
       </c>
       <c r="F160" s="17" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G160" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H160" s="7" t="s">
         <v>131</v>
@@ -12020,7 +12023,7 @@
         <v>6</v>
       </c>
       <c r="T160" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U160" s="1" t="n">
         <v>404264</v>
@@ -12046,10 +12049,10 @@
         <v>53</v>
       </c>
       <c r="F161" s="17" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G161" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H161" s="7" t="s">
         <v>133</v>
@@ -12088,7 +12091,7 @@
         <v>6</v>
       </c>
       <c r="T161" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U161" s="1" t="n">
         <v>404264</v>
@@ -12114,10 +12117,10 @@
         <v>53</v>
       </c>
       <c r="F162" s="17" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G162" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H162" s="7" t="s">
         <v>129</v>
@@ -12156,7 +12159,7 @@
         <v>6</v>
       </c>
       <c r="T162" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U162" s="1" t="n">
         <v>404264</v>
@@ -12182,10 +12185,10 @@
         <v>53</v>
       </c>
       <c r="F163" s="17" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G163" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H163" s="7" t="s">
         <v>131</v>
@@ -12224,7 +12227,7 @@
         <v>6</v>
       </c>
       <c r="T163" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U163" s="1" t="n">
         <v>404264</v>
@@ -12250,10 +12253,10 @@
         <v>53</v>
       </c>
       <c r="F164" s="17" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G164" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H164" s="7" t="s">
         <v>133</v>
@@ -12292,7 +12295,7 @@
         <v>6</v>
       </c>
       <c r="T164" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U164" s="1" t="n">
         <v>404264</v>
@@ -12318,7 +12321,7 @@
         <v>53</v>
       </c>
       <c r="F165" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G165" s="17" t="s">
         <v>73</v>
@@ -12360,7 +12363,7 @@
         <v>6</v>
       </c>
       <c r="T165" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U165" s="1" t="n">
         <v>404264</v>
@@ -12386,7 +12389,7 @@
         <v>53</v>
       </c>
       <c r="F166" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G166" s="17" t="s">
         <v>73</v>
@@ -12428,7 +12431,7 @@
         <v>6</v>
       </c>
       <c r="T166" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U166" s="1" t="n">
         <v>404264</v>
@@ -12454,7 +12457,7 @@
         <v>53</v>
       </c>
       <c r="F167" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G167" s="17" t="s">
         <v>73</v>
@@ -12496,7 +12499,7 @@
         <v>6</v>
       </c>
       <c r="T167" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U167" s="1" t="n">
         <v>404264</v>
@@ -12522,10 +12525,10 @@
         <v>53</v>
       </c>
       <c r="F168" s="17" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G168" s="17" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H168" s="7" t="s">
         <v>129</v>
@@ -12564,7 +12567,7 @@
         <v>6</v>
       </c>
       <c r="T168" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U168" s="1" t="n">
         <v>404264</v>
@@ -12590,10 +12593,10 @@
         <v>53</v>
       </c>
       <c r="F169" s="17" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G169" s="17" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H169" s="7" t="s">
         <v>131</v>
@@ -12632,7 +12635,7 @@
         <v>6</v>
       </c>
       <c r="T169" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U169" s="1" t="n">
         <v>404264</v>
@@ -12658,10 +12661,10 @@
         <v>53</v>
       </c>
       <c r="F170" s="17" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G170" s="17" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H170" s="7" t="s">
         <v>133</v>
@@ -12700,7 +12703,7 @@
         <v>6</v>
       </c>
       <c r="T170" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U170" s="1" t="n">
         <v>404264</v>
@@ -12720,22 +12723,22 @@
         <v>10056</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E171" s="6" t="s">
         <v>53</v>
       </c>
       <c r="F171" s="17" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G171" s="17" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H171" s="7" t="s">
         <v>133</v>
       </c>
       <c r="I171" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="J171" s="1" t="n">
         <v>286352</v>
@@ -12768,7 +12771,7 @@
         <v>7</v>
       </c>
       <c r="T171" s="17" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="U171" s="1" t="n">
         <v>404264</v>

</xml_diff>

<commit_message>
feat：update level and stage excel change
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Stage_关卡表.xlsx
+++ b/nevergiveup/Excel/Stage_关卡表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="251">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -436,19 +436,34 @@
     <t xml:space="preserve">1023|1||1|200||3|12</t>
   </si>
   <si>
-    <t xml:space="preserve">1023|1||1|300||3|12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1|50||3|10</t>
+    <t xml:space="preserve">1|40||3|12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1|30||3|10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1|15||3|10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1|50||2|192||3|19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1|40||2|96||3|10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1|60||2|264||3|26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1|50||2|132||3|14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17878.6|101663.7|-35.78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0|0|10</t>
   </si>
   <si>
     <t xml:space="preserve">1|25||3|10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17878.6|101663.7|-35.78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0|0|10</t>
   </si>
   <si>
     <t xml:space="preserve">15525|106466.7|-35.78</t>
@@ -891,7 +906,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -949,6 +964,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1227,10 +1246,10 @@
   </sheetPr>
   <dimension ref="A1:V171"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="N31" activeCellId="0" sqref="N31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="N29" activeCellId="0" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.48828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2556,10 +2575,10 @@
         <v>137</v>
       </c>
       <c r="O21" s="11" t="s">
-        <v>61</v>
+        <v>138</v>
       </c>
       <c r="P21" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q21" s="11" t="s">
         <v>139</v>
@@ -2621,16 +2640,16 @@
         <v>2</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="O22" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P22" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q22" s="6" t="s">
-        <v>71</v>
+        <v>137</v>
+      </c>
+      <c r="O22" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="P22" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q22" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="R22" s="6" t="s">
         <v>72</v>
@@ -2689,16 +2708,16 @@
         <v>3</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O23" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P23" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q23" s="6" t="s">
-        <v>79</v>
+        <v>137</v>
+      </c>
+      <c r="O23" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="P23" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q23" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="R23" s="6" t="s">
         <v>80</v>
@@ -2733,10 +2752,10 @@
         <v>53</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>58</v>
@@ -2757,19 +2776,19 @@
         <v>1</v>
       </c>
       <c r="N24" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O24" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P24" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q24" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O24" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="P24" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q24" s="15" t="s">
         <v>139</v>
       </c>
       <c r="R24" s="6" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="S24" s="1" t="n">
         <v>2</v>
@@ -2801,10 +2820,10 @@
         <v>53</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>66</v>
@@ -2825,16 +2844,16 @@
         <v>2</v>
       </c>
       <c r="N25" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="O25" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P25" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q25" s="6" t="s">
-        <v>71</v>
+        <v>137</v>
+      </c>
+      <c r="O25" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="P25" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q25" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="R25" s="6" t="s">
         <v>72</v>
@@ -2869,10 +2888,10 @@
         <v>53</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>74</v>
@@ -2893,16 +2912,16 @@
         <v>3</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O26" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P26" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q26" s="6" t="s">
-        <v>79</v>
+        <v>137</v>
+      </c>
+      <c r="O26" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="P26" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q26" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="R26" s="6" t="s">
         <v>80</v>
@@ -2937,10 +2956,10 @@
         <v>53</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>58</v>
@@ -2961,19 +2980,19 @@
         <v>1</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P27" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q27" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O27" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="P27" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q27" s="15" t="s">
         <v>139</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="S27" s="1" t="n">
         <v>2</v>
@@ -3005,10 +3024,10 @@
         <v>53</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>66</v>
@@ -3029,16 +3048,16 @@
         <v>2</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="O28" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P28" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q28" s="6" t="s">
-        <v>71</v>
+        <v>137</v>
+      </c>
+      <c r="O28" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="P28" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q28" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="R28" s="6" t="s">
         <v>72</v>
@@ -3073,10 +3092,10 @@
         <v>53</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>74</v>
@@ -3097,16 +3116,16 @@
         <v>3</v>
       </c>
       <c r="N29" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O29" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P29" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q29" s="6" t="s">
-        <v>79</v>
+        <v>137</v>
+      </c>
+      <c r="O29" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="P29" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q29" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="R29" s="6" t="s">
         <v>80</v>
@@ -3141,10 +3160,10 @@
         <v>53</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>146</v>
+        <v>150</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>151</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>58</v>
@@ -3165,19 +3184,19 @@
         <v>1</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O30" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P30" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q30" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O30" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="P30" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q30" s="15" t="s">
         <v>139</v>
       </c>
       <c r="R30" s="6" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="S30" s="1" t="n">
         <v>2</v>
@@ -3209,10 +3228,10 @@
         <v>53</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>146</v>
+        <v>150</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>151</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>66</v>
@@ -3233,16 +3252,16 @@
         <v>2</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="O31" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P31" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q31" s="6" t="s">
-        <v>71</v>
+        <v>137</v>
+      </c>
+      <c r="O31" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="P31" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q31" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="R31" s="6" t="s">
         <v>72</v>
@@ -3277,10 +3296,10 @@
         <v>53</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>146</v>
+        <v>150</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>151</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>74</v>
@@ -3301,16 +3320,16 @@
         <v>3</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O32" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P32" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q32" s="6" t="s">
-        <v>79</v>
+        <v>137</v>
+      </c>
+      <c r="O32" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="P32" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q32" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="R32" s="6" t="s">
         <v>80</v>
@@ -3345,10 +3364,10 @@
         <v>53</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>148</v>
+        <v>152</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>153</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>58</v>
@@ -3369,19 +3388,19 @@
         <v>1</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O33" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P33" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q33" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O33" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="P33" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q33" s="15" t="s">
         <v>139</v>
       </c>
       <c r="R33" s="6" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="S33" s="1" t="n">
         <v>2</v>
@@ -3413,10 +3432,10 @@
         <v>53</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G34" s="15" t="s">
-        <v>148</v>
+        <v>152</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>153</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>66</v>
@@ -3437,16 +3456,16 @@
         <v>2</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="O34" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P34" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q34" s="6" t="s">
-        <v>71</v>
+        <v>137</v>
+      </c>
+      <c r="O34" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="P34" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q34" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="R34" s="6" t="s">
         <v>72</v>
@@ -3481,10 +3500,10 @@
         <v>53</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>148</v>
+        <v>152</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>153</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>74</v>
@@ -3505,16 +3524,16 @@
         <v>3</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O35" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P35" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q35" s="6" t="s">
-        <v>79</v>
+        <v>137</v>
+      </c>
+      <c r="O35" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="P35" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q35" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="R35" s="6" t="s">
         <v>80</v>
@@ -3549,10 +3568,10 @@
         <v>53</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>150</v>
+        <v>154</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>155</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>58</v>
@@ -3573,19 +3592,19 @@
         <v>1</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O36" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P36" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q36" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O36" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="P36" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q36" s="15" t="s">
         <v>139</v>
       </c>
       <c r="R36" s="6" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="S36" s="1" t="n">
         <v>2</v>
@@ -3617,10 +3636,10 @@
         <v>53</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>150</v>
+        <v>154</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>155</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>66</v>
@@ -3641,16 +3660,16 @@
         <v>2</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="O37" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P37" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q37" s="6" t="s">
-        <v>71</v>
+        <v>137</v>
+      </c>
+      <c r="O37" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="P37" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q37" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="R37" s="6" t="s">
         <v>72</v>
@@ -3685,10 +3704,10 @@
         <v>53</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>150</v>
+        <v>154</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>155</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>74</v>
@@ -3709,16 +3728,16 @@
         <v>3</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O38" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P38" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q38" s="6" t="s">
-        <v>79</v>
+        <v>137</v>
+      </c>
+      <c r="O38" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="P38" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q38" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="R38" s="6" t="s">
         <v>80</v>
@@ -3753,10 +3772,10 @@
         <v>53</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>152</v>
+        <v>156</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="H39" s="7" t="s">
         <v>58</v>
@@ -3777,19 +3796,19 @@
         <v>1</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O39" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P39" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q39" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O39" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="P39" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q39" s="15" t="s">
         <v>139</v>
       </c>
       <c r="R39" s="6" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="S39" s="1" t="n">
         <v>2</v>
@@ -3821,10 +3840,10 @@
         <v>53</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G40" s="15" t="s">
-        <v>152</v>
+        <v>156</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>66</v>
@@ -3845,16 +3864,16 @@
         <v>2</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="O40" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P40" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q40" s="6" t="s">
-        <v>71</v>
+        <v>137</v>
+      </c>
+      <c r="O40" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="P40" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q40" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="R40" s="6" t="s">
         <v>72</v>
@@ -3889,10 +3908,10 @@
         <v>53</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G41" s="15" t="s">
-        <v>152</v>
+        <v>156</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>74</v>
@@ -3913,16 +3932,16 @@
         <v>3</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O41" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P41" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q41" s="6" t="s">
-        <v>79</v>
+        <v>137</v>
+      </c>
+      <c r="O41" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="P41" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q41" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="R41" s="6" t="s">
         <v>80</v>
@@ -3957,10 +3976,10 @@
         <v>53</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G42" s="15" t="s">
-        <v>154</v>
+        <v>158</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>159</v>
       </c>
       <c r="H42" s="7" t="s">
         <v>58</v>
@@ -3981,19 +4000,19 @@
         <v>1</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O42" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P42" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q42" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O42" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="P42" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q42" s="15" t="s">
         <v>139</v>
       </c>
       <c r="R42" s="6" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="S42" s="1" t="n">
         <v>2</v>
@@ -4025,10 +4044,10 @@
         <v>53</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G43" s="15" t="s">
-        <v>154</v>
+        <v>158</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>159</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>66</v>
@@ -4049,16 +4068,16 @@
         <v>2</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="O43" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P43" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q43" s="6" t="s">
-        <v>71</v>
+        <v>137</v>
+      </c>
+      <c r="O43" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="P43" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q43" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="R43" s="6" t="s">
         <v>72</v>
@@ -4093,10 +4112,10 @@
         <v>53</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G44" s="15" t="s">
-        <v>154</v>
+        <v>158</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>159</v>
       </c>
       <c r="H44" s="7" t="s">
         <v>74</v>
@@ -4117,16 +4136,16 @@
         <v>3</v>
       </c>
       <c r="N44" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O44" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P44" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q44" s="6" t="s">
-        <v>79</v>
+        <v>137</v>
+      </c>
+      <c r="O44" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="P44" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q44" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="R44" s="6" t="s">
         <v>80</v>
@@ -4161,10 +4180,10 @@
         <v>53</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G45" s="15" t="s">
-        <v>156</v>
+        <v>160</v>
+      </c>
+      <c r="G45" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>58</v>
@@ -4185,19 +4204,19 @@
         <v>1</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O45" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P45" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q45" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O45" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="P45" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q45" s="15" t="s">
         <v>139</v>
       </c>
       <c r="R45" s="6" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="S45" s="1" t="n">
         <v>2</v>
@@ -4229,10 +4248,10 @@
         <v>53</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G46" s="15" t="s">
-        <v>156</v>
+        <v>160</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>66</v>
@@ -4253,16 +4272,16 @@
         <v>2</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="O46" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P46" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q46" s="6" t="s">
-        <v>71</v>
+        <v>137</v>
+      </c>
+      <c r="O46" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="P46" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q46" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="R46" s="6" t="s">
         <v>72</v>
@@ -4297,10 +4316,10 @@
         <v>53</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G47" s="15" t="s">
-        <v>156</v>
+        <v>160</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>74</v>
@@ -4321,16 +4340,16 @@
         <v>3</v>
       </c>
       <c r="N47" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O47" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P47" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q47" s="6" t="s">
-        <v>79</v>
+        <v>137</v>
+      </c>
+      <c r="O47" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="P47" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q47" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="R47" s="6" t="s">
         <v>80</v>
@@ -4365,10 +4384,10 @@
         <v>53</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G48" s="15" t="s">
-        <v>158</v>
+        <v>162</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="H48" s="7" t="s">
         <v>58</v>
@@ -4389,19 +4408,19 @@
         <v>1</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O48" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P48" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q48" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O48" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="P48" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q48" s="15" t="s">
         <v>139</v>
       </c>
       <c r="R48" s="6" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="S48" s="1" t="n">
         <v>2</v>
@@ -4433,10 +4452,10 @@
         <v>53</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G49" s="15" t="s">
-        <v>158</v>
+        <v>162</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>66</v>
@@ -4457,16 +4476,16 @@
         <v>2</v>
       </c>
       <c r="N49" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="O49" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P49" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q49" s="6" t="s">
-        <v>71</v>
+        <v>137</v>
+      </c>
+      <c r="O49" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="P49" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q49" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="R49" s="6" t="s">
         <v>72</v>
@@ -4501,10 +4520,10 @@
         <v>53</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G50" s="16" t="s">
-        <v>158</v>
+        <v>162</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>163</v>
       </c>
       <c r="H50" s="12" t="s">
         <v>74</v>
@@ -4525,16 +4544,16 @@
         <v>3</v>
       </c>
       <c r="N50" s="11" t="s">
-        <v>76</v>
+        <v>137</v>
       </c>
       <c r="O50" s="11" t="s">
-        <v>77</v>
+        <v>143</v>
       </c>
       <c r="P50" s="11" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="Q50" s="11" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
       <c r="R50" s="11" t="s">
         <v>80</v>
@@ -4568,11 +4587,11 @@
       <c r="E51" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F51" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="G51" s="18" t="s">
-        <v>160</v>
+      <c r="F51" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="G51" s="19" t="s">
+        <v>165</v>
       </c>
       <c r="H51" s="7" t="s">
         <v>83</v>
@@ -4611,7 +4630,7 @@
         <v>3</v>
       </c>
       <c r="T51" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U51" s="1" t="n">
         <v>404267</v>
@@ -4636,11 +4655,11 @@
       <c r="E52" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F52" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="G52" s="18" t="s">
-        <v>160</v>
+      <c r="F52" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="G52" s="19" t="s">
+        <v>165</v>
       </c>
       <c r="H52" s="7" t="s">
         <v>90</v>
@@ -4679,7 +4698,7 @@
         <v>3</v>
       </c>
       <c r="T52" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U52" s="1" t="n">
         <v>404267</v>
@@ -4704,11 +4723,11 @@
       <c r="E53" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F53" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="G53" s="18" t="s">
-        <v>160</v>
+      <c r="F53" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="G53" s="19" t="s">
+        <v>165</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>95</v>
@@ -4747,7 +4766,7 @@
         <v>3</v>
       </c>
       <c r="T53" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U53" s="1" t="n">
         <v>404267</v>
@@ -4772,11 +4791,11 @@
       <c r="E54" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F54" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="G54" s="18" t="s">
-        <v>163</v>
+      <c r="F54" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="G54" s="19" t="s">
+        <v>168</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>83</v>
@@ -4815,7 +4834,7 @@
         <v>3</v>
       </c>
       <c r="T54" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U54" s="1" t="n">
         <v>404267</v>
@@ -4840,11 +4859,11 @@
       <c r="E55" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F55" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="G55" s="18" t="s">
-        <v>163</v>
+      <c r="F55" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="G55" s="19" t="s">
+        <v>168</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>90</v>
@@ -4883,7 +4902,7 @@
         <v>3</v>
       </c>
       <c r="T55" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U55" s="1" t="n">
         <v>404267</v>
@@ -4908,11 +4927,11 @@
       <c r="E56" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F56" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="G56" s="18" t="s">
-        <v>163</v>
+      <c r="F56" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="G56" s="19" t="s">
+        <v>168</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>95</v>
@@ -4951,7 +4970,7 @@
         <v>3</v>
       </c>
       <c r="T56" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U56" s="1" t="n">
         <v>404267</v>
@@ -4976,11 +4995,11 @@
       <c r="E57" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F57" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="G57" s="18" t="s">
-        <v>165</v>
+      <c r="F57" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="G57" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>83</v>
@@ -5019,7 +5038,7 @@
         <v>3</v>
       </c>
       <c r="T57" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U57" s="1" t="n">
         <v>404267</v>
@@ -5044,11 +5063,11 @@
       <c r="E58" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F58" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="G58" s="18" t="s">
-        <v>165</v>
+      <c r="F58" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="G58" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="H58" s="7" t="s">
         <v>90</v>
@@ -5087,7 +5106,7 @@
         <v>3</v>
       </c>
       <c r="T58" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U58" s="1" t="n">
         <v>404267</v>
@@ -5112,11 +5131,11 @@
       <c r="E59" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F59" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="G59" s="18" t="s">
-        <v>165</v>
+      <c r="F59" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="G59" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="H59" s="7" t="s">
         <v>95</v>
@@ -5155,7 +5174,7 @@
         <v>3</v>
       </c>
       <c r="T59" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U59" s="1" t="n">
         <v>404267</v>
@@ -5180,11 +5199,11 @@
       <c r="E60" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F60" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G60" s="18" t="s">
-        <v>167</v>
+      <c r="F60" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="G60" s="19" t="s">
+        <v>172</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>83</v>
@@ -5223,7 +5242,7 @@
         <v>3</v>
       </c>
       <c r="T60" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U60" s="1" t="n">
         <v>404267</v>
@@ -5248,11 +5267,11 @@
       <c r="E61" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F61" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G61" s="18" t="s">
-        <v>167</v>
+      <c r="F61" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="G61" s="19" t="s">
+        <v>172</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>90</v>
@@ -5291,7 +5310,7 @@
         <v>3</v>
       </c>
       <c r="T61" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U61" s="1" t="n">
         <v>404267</v>
@@ -5316,11 +5335,11 @@
       <c r="E62" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F62" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G62" s="18" t="s">
-        <v>167</v>
+      <c r="F62" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="G62" s="19" t="s">
+        <v>172</v>
       </c>
       <c r="H62" s="7" t="s">
         <v>95</v>
@@ -5359,7 +5378,7 @@
         <v>3</v>
       </c>
       <c r="T62" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U62" s="1" t="n">
         <v>404267</v>
@@ -5384,11 +5403,11 @@
       <c r="E63" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F63" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="G63" s="18" t="s">
-        <v>169</v>
+      <c r="F63" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="G63" s="19" t="s">
+        <v>174</v>
       </c>
       <c r="H63" s="7" t="s">
         <v>83</v>
@@ -5427,7 +5446,7 @@
         <v>3</v>
       </c>
       <c r="T63" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U63" s="1" t="n">
         <v>404267</v>
@@ -5452,11 +5471,11 @@
       <c r="E64" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F64" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="G64" s="18" t="s">
-        <v>169</v>
+      <c r="F64" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="G64" s="19" t="s">
+        <v>174</v>
       </c>
       <c r="H64" s="7" t="s">
         <v>90</v>
@@ -5495,7 +5514,7 @@
         <v>3</v>
       </c>
       <c r="T64" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U64" s="1" t="n">
         <v>404267</v>
@@ -5520,11 +5539,11 @@
       <c r="E65" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F65" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="G65" s="18" t="s">
-        <v>169</v>
+      <c r="F65" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="G65" s="19" t="s">
+        <v>174</v>
       </c>
       <c r="H65" s="7" t="s">
         <v>95</v>
@@ -5563,7 +5582,7 @@
         <v>3</v>
       </c>
       <c r="T65" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U65" s="1" t="n">
         <v>404267</v>
@@ -5588,11 +5607,11 @@
       <c r="E66" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F66" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="G66" s="18" t="s">
-        <v>171</v>
+      <c r="F66" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="G66" s="19" t="s">
+        <v>176</v>
       </c>
       <c r="H66" s="7" t="s">
         <v>83</v>
@@ -5631,7 +5650,7 @@
         <v>3</v>
       </c>
       <c r="T66" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U66" s="1" t="n">
         <v>404267</v>
@@ -5656,11 +5675,11 @@
       <c r="E67" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F67" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="G67" s="18" t="s">
-        <v>171</v>
+      <c r="F67" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="G67" s="19" t="s">
+        <v>176</v>
       </c>
       <c r="H67" s="7" t="s">
         <v>90</v>
@@ -5699,7 +5718,7 @@
         <v>3</v>
       </c>
       <c r="T67" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U67" s="1" t="n">
         <v>404267</v>
@@ -5724,11 +5743,11 @@
       <c r="E68" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F68" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="G68" s="18" t="s">
-        <v>171</v>
+      <c r="F68" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="G68" s="19" t="s">
+        <v>176</v>
       </c>
       <c r="H68" s="7" t="s">
         <v>95</v>
@@ -5767,7 +5786,7 @@
         <v>3</v>
       </c>
       <c r="T68" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U68" s="1" t="n">
         <v>404267</v>
@@ -5792,11 +5811,11 @@
       <c r="E69" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F69" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="G69" s="18" t="s">
-        <v>173</v>
+      <c r="F69" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="G69" s="19" t="s">
+        <v>178</v>
       </c>
       <c r="H69" s="7" t="s">
         <v>83</v>
@@ -5835,7 +5854,7 @@
         <v>3</v>
       </c>
       <c r="T69" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U69" s="1" t="n">
         <v>404267</v>
@@ -5860,11 +5879,11 @@
       <c r="E70" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F70" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="G70" s="18" t="s">
-        <v>173</v>
+      <c r="F70" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="G70" s="19" t="s">
+        <v>178</v>
       </c>
       <c r="H70" s="7" t="s">
         <v>90</v>
@@ -5903,7 +5922,7 @@
         <v>3</v>
       </c>
       <c r="T70" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U70" s="1" t="n">
         <v>404267</v>
@@ -5928,11 +5947,11 @@
       <c r="E71" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F71" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="G71" s="18" t="s">
-        <v>173</v>
+      <c r="F71" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="G71" s="19" t="s">
+        <v>178</v>
       </c>
       <c r="H71" s="7" t="s">
         <v>95</v>
@@ -5971,7 +5990,7 @@
         <v>3</v>
       </c>
       <c r="T71" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U71" s="1" t="n">
         <v>404267</v>
@@ -5996,11 +6015,11 @@
       <c r="E72" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F72" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G72" s="18" t="s">
-        <v>175</v>
+      <c r="F72" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="G72" s="19" t="s">
+        <v>180</v>
       </c>
       <c r="H72" s="7" t="s">
         <v>83</v>
@@ -6039,7 +6058,7 @@
         <v>3</v>
       </c>
       <c r="T72" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U72" s="1" t="n">
         <v>404267</v>
@@ -6064,11 +6083,11 @@
       <c r="E73" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F73" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G73" s="18" t="s">
-        <v>175</v>
+      <c r="F73" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="G73" s="19" t="s">
+        <v>180</v>
       </c>
       <c r="H73" s="7" t="s">
         <v>90</v>
@@ -6107,7 +6126,7 @@
         <v>3</v>
       </c>
       <c r="T73" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U73" s="1" t="n">
         <v>404267</v>
@@ -6132,11 +6151,11 @@
       <c r="E74" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F74" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G74" s="18" t="s">
-        <v>175</v>
+      <c r="F74" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="G74" s="19" t="s">
+        <v>180</v>
       </c>
       <c r="H74" s="7" t="s">
         <v>95</v>
@@ -6175,7 +6194,7 @@
         <v>3</v>
       </c>
       <c r="T74" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U74" s="1" t="n">
         <v>404267</v>
@@ -6200,11 +6219,11 @@
       <c r="E75" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F75" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G75" s="18" t="s">
-        <v>177</v>
+      <c r="F75" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="G75" s="19" t="s">
+        <v>182</v>
       </c>
       <c r="H75" s="7" t="s">
         <v>83</v>
@@ -6243,7 +6262,7 @@
         <v>3</v>
       </c>
       <c r="T75" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U75" s="1" t="n">
         <v>404267</v>
@@ -6268,11 +6287,11 @@
       <c r="E76" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F76" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G76" s="18" t="s">
-        <v>177</v>
+      <c r="F76" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="G76" s="19" t="s">
+        <v>182</v>
       </c>
       <c r="H76" s="7" t="s">
         <v>90</v>
@@ -6311,7 +6330,7 @@
         <v>3</v>
       </c>
       <c r="T76" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U76" s="1" t="n">
         <v>404267</v>
@@ -6336,11 +6355,11 @@
       <c r="E77" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F77" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G77" s="18" t="s">
-        <v>177</v>
+      <c r="F77" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="G77" s="19" t="s">
+        <v>182</v>
       </c>
       <c r="H77" s="7" t="s">
         <v>95</v>
@@ -6379,7 +6398,7 @@
         <v>3</v>
       </c>
       <c r="T77" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U77" s="1" t="n">
         <v>404267</v>
@@ -6404,10 +6423,10 @@
       <c r="E78" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F78" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G78" s="18" t="s">
+      <c r="F78" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="G78" s="19" t="s">
         <v>73</v>
       </c>
       <c r="H78" s="7" t="s">
@@ -6447,7 +6466,7 @@
         <v>3</v>
       </c>
       <c r="T78" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U78" s="1" t="n">
         <v>404267</v>
@@ -6472,10 +6491,10 @@
       <c r="E79" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F79" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G79" s="18" t="s">
+      <c r="F79" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="G79" s="19" t="s">
         <v>73</v>
       </c>
       <c r="H79" s="7" t="s">
@@ -6515,7 +6534,7 @@
         <v>3</v>
       </c>
       <c r="T79" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U79" s="1" t="n">
         <v>404267</v>
@@ -6540,10 +6559,10 @@
       <c r="E80" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F80" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="G80" s="20" t="s">
+      <c r="F80" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="G80" s="21" t="s">
         <v>73</v>
       </c>
       <c r="H80" s="12" t="s">
@@ -6583,7 +6602,7 @@
         <v>3</v>
       </c>
       <c r="T80" s="14" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U80" s="14" t="n">
         <v>404267</v>
@@ -6608,11 +6627,11 @@
       <c r="E81" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F81" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="G81" s="18" t="s">
-        <v>180</v>
+      <c r="F81" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="G81" s="19" t="s">
+        <v>185</v>
       </c>
       <c r="H81" s="7" t="s">
         <v>102</v>
@@ -6651,7 +6670,7 @@
         <v>4</v>
       </c>
       <c r="T81" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U81" s="1" t="n">
         <v>404269</v>
@@ -6676,11 +6695,11 @@
       <c r="E82" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F82" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="G82" s="18" t="s">
-        <v>180</v>
+      <c r="F82" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="G82" s="19" t="s">
+        <v>185</v>
       </c>
       <c r="H82" s="7" t="s">
         <v>107</v>
@@ -6719,7 +6738,7 @@
         <v>4</v>
       </c>
       <c r="T82" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U82" s="1" t="n">
         <v>404269</v>
@@ -6744,11 +6763,11 @@
       <c r="E83" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F83" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="G83" s="18" t="s">
-        <v>180</v>
+      <c r="F83" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="G83" s="19" t="s">
+        <v>185</v>
       </c>
       <c r="H83" s="7" t="s">
         <v>112</v>
@@ -6787,7 +6806,7 @@
         <v>4</v>
       </c>
       <c r="T83" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U83" s="1" t="n">
         <v>404269</v>
@@ -6812,11 +6831,11 @@
       <c r="E84" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F84" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="G84" s="18" t="s">
-        <v>183</v>
+      <c r="F84" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G84" s="19" t="s">
+        <v>188</v>
       </c>
       <c r="H84" s="7" t="s">
         <v>102</v>
@@ -6855,7 +6874,7 @@
         <v>4</v>
       </c>
       <c r="T84" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U84" s="1" t="n">
         <v>404269</v>
@@ -6880,11 +6899,11 @@
       <c r="E85" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F85" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="G85" s="18" t="s">
-        <v>183</v>
+      <c r="F85" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G85" s="19" t="s">
+        <v>188</v>
       </c>
       <c r="H85" s="7" t="s">
         <v>107</v>
@@ -6923,7 +6942,7 @@
         <v>4</v>
       </c>
       <c r="T85" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U85" s="1" t="n">
         <v>404269</v>
@@ -6948,11 +6967,11 @@
       <c r="E86" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F86" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="G86" s="18" t="s">
-        <v>183</v>
+      <c r="F86" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G86" s="19" t="s">
+        <v>188</v>
       </c>
       <c r="H86" s="7" t="s">
         <v>112</v>
@@ -6991,7 +7010,7 @@
         <v>4</v>
       </c>
       <c r="T86" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U86" s="1" t="n">
         <v>404269</v>
@@ -7016,11 +7035,11 @@
       <c r="E87" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F87" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="G87" s="18" t="s">
-        <v>185</v>
+      <c r="F87" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="G87" s="19" t="s">
+        <v>190</v>
       </c>
       <c r="H87" s="7" t="s">
         <v>102</v>
@@ -7059,7 +7078,7 @@
         <v>4</v>
       </c>
       <c r="T87" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U87" s="1" t="n">
         <v>404269</v>
@@ -7084,11 +7103,11 @@
       <c r="E88" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F88" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="G88" s="18" t="s">
-        <v>185</v>
+      <c r="F88" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="G88" s="19" t="s">
+        <v>190</v>
       </c>
       <c r="H88" s="7" t="s">
         <v>107</v>
@@ -7127,7 +7146,7 @@
         <v>4</v>
       </c>
       <c r="T88" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U88" s="1" t="n">
         <v>404269</v>
@@ -7152,11 +7171,11 @@
       <c r="E89" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F89" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="G89" s="18" t="s">
-        <v>185</v>
+      <c r="F89" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="G89" s="19" t="s">
+        <v>190</v>
       </c>
       <c r="H89" s="7" t="s">
         <v>112</v>
@@ -7195,7 +7214,7 @@
         <v>4</v>
       </c>
       <c r="T89" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U89" s="1" t="n">
         <v>404269</v>
@@ -7220,11 +7239,11 @@
       <c r="E90" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F90" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="G90" s="18" t="s">
-        <v>187</v>
+      <c r="F90" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="G90" s="19" t="s">
+        <v>192</v>
       </c>
       <c r="H90" s="7" t="s">
         <v>102</v>
@@ -7263,7 +7282,7 @@
         <v>4</v>
       </c>
       <c r="T90" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U90" s="1" t="n">
         <v>404269</v>
@@ -7288,11 +7307,11 @@
       <c r="E91" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F91" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="G91" s="18" t="s">
-        <v>187</v>
+      <c r="F91" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="G91" s="19" t="s">
+        <v>192</v>
       </c>
       <c r="H91" s="7" t="s">
         <v>107</v>
@@ -7331,7 +7350,7 @@
         <v>4</v>
       </c>
       <c r="T91" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U91" s="1" t="n">
         <v>404269</v>
@@ -7356,11 +7375,11 @@
       <c r="E92" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F92" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="G92" s="18" t="s">
-        <v>187</v>
+      <c r="F92" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="G92" s="19" t="s">
+        <v>192</v>
       </c>
       <c r="H92" s="7" t="s">
         <v>112</v>
@@ -7399,7 +7418,7 @@
         <v>4</v>
       </c>
       <c r="T92" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U92" s="1" t="n">
         <v>404269</v>
@@ -7424,11 +7443,11 @@
       <c r="E93" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F93" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="G93" s="18" t="s">
-        <v>189</v>
+      <c r="F93" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="G93" s="19" t="s">
+        <v>194</v>
       </c>
       <c r="H93" s="7" t="s">
         <v>102</v>
@@ -7467,7 +7486,7 @@
         <v>4</v>
       </c>
       <c r="T93" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U93" s="1" t="n">
         <v>404269</v>
@@ -7492,11 +7511,11 @@
       <c r="E94" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F94" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="G94" s="18" t="s">
-        <v>189</v>
+      <c r="F94" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="G94" s="19" t="s">
+        <v>194</v>
       </c>
       <c r="H94" s="7" t="s">
         <v>107</v>
@@ -7535,7 +7554,7 @@
         <v>4</v>
       </c>
       <c r="T94" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U94" s="1" t="n">
         <v>404269</v>
@@ -7560,11 +7579,11 @@
       <c r="E95" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F95" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="G95" s="18" t="s">
-        <v>189</v>
+      <c r="F95" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="G95" s="19" t="s">
+        <v>194</v>
       </c>
       <c r="H95" s="7" t="s">
         <v>112</v>
@@ -7603,7 +7622,7 @@
         <v>4</v>
       </c>
       <c r="T95" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U95" s="1" t="n">
         <v>404269</v>
@@ -7628,11 +7647,11 @@
       <c r="E96" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F96" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="G96" s="18" t="s">
-        <v>191</v>
+      <c r="F96" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="G96" s="19" t="s">
+        <v>196</v>
       </c>
       <c r="H96" s="7" t="s">
         <v>102</v>
@@ -7671,7 +7690,7 @@
         <v>4</v>
       </c>
       <c r="T96" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U96" s="1" t="n">
         <v>404269</v>
@@ -7696,11 +7715,11 @@
       <c r="E97" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F97" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="G97" s="18" t="s">
-        <v>191</v>
+      <c r="F97" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="G97" s="19" t="s">
+        <v>196</v>
       </c>
       <c r="H97" s="7" t="s">
         <v>107</v>
@@ -7739,7 +7758,7 @@
         <v>4</v>
       </c>
       <c r="T97" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U97" s="1" t="n">
         <v>404269</v>
@@ -7764,11 +7783,11 @@
       <c r="E98" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F98" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="G98" s="18" t="s">
-        <v>191</v>
+      <c r="F98" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="G98" s="19" t="s">
+        <v>196</v>
       </c>
       <c r="H98" s="7" t="s">
         <v>112</v>
@@ -7807,7 +7826,7 @@
         <v>4</v>
       </c>
       <c r="T98" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U98" s="1" t="n">
         <v>404269</v>
@@ -7832,11 +7851,11 @@
       <c r="E99" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F99" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="G99" s="18" t="s">
-        <v>193</v>
+      <c r="F99" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="G99" s="19" t="s">
+        <v>198</v>
       </c>
       <c r="H99" s="7" t="s">
         <v>102</v>
@@ -7875,7 +7894,7 @@
         <v>4</v>
       </c>
       <c r="T99" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U99" s="1" t="n">
         <v>404269</v>
@@ -7900,11 +7919,11 @@
       <c r="E100" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F100" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="G100" s="18" t="s">
-        <v>193</v>
+      <c r="F100" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="G100" s="19" t="s">
+        <v>198</v>
       </c>
       <c r="H100" s="7" t="s">
         <v>107</v>
@@ -7943,7 +7962,7 @@
         <v>4</v>
       </c>
       <c r="T100" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U100" s="1" t="n">
         <v>404269</v>
@@ -7968,11 +7987,11 @@
       <c r="E101" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F101" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="G101" s="18" t="s">
-        <v>193</v>
+      <c r="F101" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="G101" s="19" t="s">
+        <v>198</v>
       </c>
       <c r="H101" s="7" t="s">
         <v>112</v>
@@ -8011,7 +8030,7 @@
         <v>4</v>
       </c>
       <c r="T101" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U101" s="1" t="n">
         <v>404269</v>
@@ -8036,11 +8055,11 @@
       <c r="E102" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F102" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="G102" s="18" t="s">
-        <v>195</v>
+      <c r="F102" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="G102" s="19" t="s">
+        <v>200</v>
       </c>
       <c r="H102" s="7" t="s">
         <v>102</v>
@@ -8079,7 +8098,7 @@
         <v>4</v>
       </c>
       <c r="T102" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U102" s="1" t="n">
         <v>404269</v>
@@ -8104,11 +8123,11 @@
       <c r="E103" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F103" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="G103" s="18" t="s">
-        <v>195</v>
+      <c r="F103" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="G103" s="19" t="s">
+        <v>200</v>
       </c>
       <c r="H103" s="7" t="s">
         <v>107</v>
@@ -8147,7 +8166,7 @@
         <v>4</v>
       </c>
       <c r="T103" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U103" s="1" t="n">
         <v>404269</v>
@@ -8172,11 +8191,11 @@
       <c r="E104" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F104" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="G104" s="18" t="s">
-        <v>195</v>
+      <c r="F104" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="G104" s="19" t="s">
+        <v>200</v>
       </c>
       <c r="H104" s="7" t="s">
         <v>112</v>
@@ -8215,7 +8234,7 @@
         <v>4</v>
       </c>
       <c r="T104" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U104" s="1" t="n">
         <v>404269</v>
@@ -8240,11 +8259,11 @@
       <c r="E105" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F105" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="G105" s="18" t="s">
-        <v>197</v>
+      <c r="F105" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="G105" s="19" t="s">
+        <v>202</v>
       </c>
       <c r="H105" s="7" t="s">
         <v>102</v>
@@ -8283,7 +8302,7 @@
         <v>4</v>
       </c>
       <c r="T105" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U105" s="1" t="n">
         <v>404269</v>
@@ -8308,11 +8327,11 @@
       <c r="E106" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F106" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="G106" s="18" t="s">
-        <v>197</v>
+      <c r="F106" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="G106" s="19" t="s">
+        <v>202</v>
       </c>
       <c r="H106" s="7" t="s">
         <v>107</v>
@@ -8351,7 +8370,7 @@
         <v>4</v>
       </c>
       <c r="T106" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U106" s="1" t="n">
         <v>404269</v>
@@ -8376,11 +8395,11 @@
       <c r="E107" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F107" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="G107" s="18" t="s">
-        <v>197</v>
+      <c r="F107" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="G107" s="19" t="s">
+        <v>202</v>
       </c>
       <c r="H107" s="7" t="s">
         <v>112</v>
@@ -8419,7 +8438,7 @@
         <v>4</v>
       </c>
       <c r="T107" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U107" s="1" t="n">
         <v>404269</v>
@@ -8444,11 +8463,11 @@
       <c r="E108" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F108" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="G108" s="18" t="s">
-        <v>199</v>
+      <c r="F108" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="G108" s="19" t="s">
+        <v>204</v>
       </c>
       <c r="H108" s="7" t="s">
         <v>102</v>
@@ -8487,7 +8506,7 @@
         <v>4</v>
       </c>
       <c r="T108" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U108" s="1" t="n">
         <v>404269</v>
@@ -8512,11 +8531,11 @@
       <c r="E109" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F109" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="G109" s="18" t="s">
-        <v>199</v>
+      <c r="F109" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="G109" s="19" t="s">
+        <v>204</v>
       </c>
       <c r="H109" s="7" t="s">
         <v>107</v>
@@ -8555,7 +8574,7 @@
         <v>4</v>
       </c>
       <c r="T109" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U109" s="1" t="n">
         <v>404269</v>
@@ -8580,11 +8599,11 @@
       <c r="E110" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F110" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="G110" s="20" t="s">
-        <v>199</v>
+      <c r="F110" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="G110" s="21" t="s">
+        <v>204</v>
       </c>
       <c r="H110" s="12" t="s">
         <v>112</v>
@@ -8623,7 +8642,7 @@
         <v>4</v>
       </c>
       <c r="T110" s="14" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="U110" s="14" t="n">
         <v>404269</v>
@@ -8648,11 +8667,11 @@
       <c r="E111" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F111" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="G111" s="18" t="s">
-        <v>201</v>
+      <c r="F111" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="G111" s="19" t="s">
+        <v>206</v>
       </c>
       <c r="H111" s="7" t="s">
         <v>121</v>
@@ -8691,7 +8710,7 @@
         <v>5</v>
       </c>
       <c r="T111" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U111" s="1" t="n">
         <v>404266</v>
@@ -8716,11 +8735,11 @@
       <c r="E112" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F112" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="G112" s="18" t="s">
-        <v>201</v>
+      <c r="F112" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="G112" s="19" t="s">
+        <v>206</v>
       </c>
       <c r="H112" s="7" t="s">
         <v>123</v>
@@ -8759,7 +8778,7 @@
         <v>5</v>
       </c>
       <c r="T112" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U112" s="1" t="n">
         <v>404266</v>
@@ -8784,11 +8803,11 @@
       <c r="E113" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F113" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="G113" s="18" t="s">
-        <v>201</v>
+      <c r="F113" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="G113" s="19" t="s">
+        <v>206</v>
       </c>
       <c r="H113" s="7" t="s">
         <v>125</v>
@@ -8827,7 +8846,7 @@
         <v>5</v>
       </c>
       <c r="T113" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U113" s="1" t="n">
         <v>404266</v>
@@ -8852,11 +8871,11 @@
       <c r="E114" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F114" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="G114" s="18" t="s">
-        <v>204</v>
+      <c r="F114" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="G114" s="19" t="s">
+        <v>209</v>
       </c>
       <c r="H114" s="7" t="s">
         <v>121</v>
@@ -8895,7 +8914,7 @@
         <v>5</v>
       </c>
       <c r="T114" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U114" s="1" t="n">
         <v>404266</v>
@@ -8920,11 +8939,11 @@
       <c r="E115" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F115" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="G115" s="18" t="s">
-        <v>204</v>
+      <c r="F115" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="G115" s="19" t="s">
+        <v>209</v>
       </c>
       <c r="H115" s="7" t="s">
         <v>123</v>
@@ -8963,7 +8982,7 @@
         <v>5</v>
       </c>
       <c r="T115" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U115" s="1" t="n">
         <v>404266</v>
@@ -8988,11 +9007,11 @@
       <c r="E116" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F116" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="G116" s="18" t="s">
-        <v>204</v>
+      <c r="F116" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="G116" s="19" t="s">
+        <v>209</v>
       </c>
       <c r="H116" s="7" t="s">
         <v>125</v>
@@ -9031,7 +9050,7 @@
         <v>5</v>
       </c>
       <c r="T116" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U116" s="1" t="n">
         <v>404266</v>
@@ -9056,11 +9075,11 @@
       <c r="E117" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F117" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="G117" s="18" t="s">
-        <v>206</v>
+      <c r="F117" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="G117" s="19" t="s">
+        <v>211</v>
       </c>
       <c r="H117" s="7" t="s">
         <v>121</v>
@@ -9099,7 +9118,7 @@
         <v>5</v>
       </c>
       <c r="T117" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U117" s="1" t="n">
         <v>404266</v>
@@ -9124,11 +9143,11 @@
       <c r="E118" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F118" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="G118" s="18" t="s">
-        <v>206</v>
+      <c r="F118" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="G118" s="19" t="s">
+        <v>211</v>
       </c>
       <c r="H118" s="7" t="s">
         <v>123</v>
@@ -9167,7 +9186,7 @@
         <v>5</v>
       </c>
       <c r="T118" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U118" s="1" t="n">
         <v>404266</v>
@@ -9192,11 +9211,11 @@
       <c r="E119" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F119" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="G119" s="18" t="s">
-        <v>206</v>
+      <c r="F119" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="G119" s="19" t="s">
+        <v>211</v>
       </c>
       <c r="H119" s="7" t="s">
         <v>125</v>
@@ -9235,7 +9254,7 @@
         <v>5</v>
       </c>
       <c r="T119" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U119" s="1" t="n">
         <v>404266</v>
@@ -9260,11 +9279,11 @@
       <c r="E120" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F120" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="G120" s="18" t="s">
-        <v>208</v>
+      <c r="F120" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="G120" s="19" t="s">
+        <v>213</v>
       </c>
       <c r="H120" s="7" t="s">
         <v>121</v>
@@ -9303,7 +9322,7 @@
         <v>5</v>
       </c>
       <c r="T120" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U120" s="1" t="n">
         <v>404266</v>
@@ -9328,11 +9347,11 @@
       <c r="E121" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F121" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="G121" s="18" t="s">
-        <v>208</v>
+      <c r="F121" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="G121" s="19" t="s">
+        <v>213</v>
       </c>
       <c r="H121" s="7" t="s">
         <v>123</v>
@@ -9371,7 +9390,7 @@
         <v>5</v>
       </c>
       <c r="T121" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U121" s="1" t="n">
         <v>404266</v>
@@ -9396,11 +9415,11 @@
       <c r="E122" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F122" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="G122" s="18" t="s">
-        <v>208</v>
+      <c r="F122" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="G122" s="19" t="s">
+        <v>213</v>
       </c>
       <c r="H122" s="7" t="s">
         <v>125</v>
@@ -9439,7 +9458,7 @@
         <v>5</v>
       </c>
       <c r="T122" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U122" s="1" t="n">
         <v>404266</v>
@@ -9464,11 +9483,11 @@
       <c r="E123" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F123" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="G123" s="18" t="s">
-        <v>210</v>
+      <c r="F123" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="G123" s="19" t="s">
+        <v>215</v>
       </c>
       <c r="H123" s="7" t="s">
         <v>121</v>
@@ -9507,7 +9526,7 @@
         <v>5</v>
       </c>
       <c r="T123" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U123" s="1" t="n">
         <v>404266</v>
@@ -9532,11 +9551,11 @@
       <c r="E124" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F124" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="G124" s="18" t="s">
-        <v>210</v>
+      <c r="F124" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="G124" s="19" t="s">
+        <v>215</v>
       </c>
       <c r="H124" s="7" t="s">
         <v>123</v>
@@ -9575,7 +9594,7 @@
         <v>5</v>
       </c>
       <c r="T124" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U124" s="1" t="n">
         <v>404266</v>
@@ -9600,11 +9619,11 @@
       <c r="E125" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F125" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="G125" s="18" t="s">
-        <v>210</v>
+      <c r="F125" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="G125" s="19" t="s">
+        <v>215</v>
       </c>
       <c r="H125" s="7" t="s">
         <v>125</v>
@@ -9643,7 +9662,7 @@
         <v>5</v>
       </c>
       <c r="T125" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U125" s="1" t="n">
         <v>404266</v>
@@ -9668,11 +9687,11 @@
       <c r="E126" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F126" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="G126" s="18" t="s">
-        <v>212</v>
+      <c r="F126" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="G126" s="19" t="s">
+        <v>217</v>
       </c>
       <c r="H126" s="7" t="s">
         <v>121</v>
@@ -9711,7 +9730,7 @@
         <v>5</v>
       </c>
       <c r="T126" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U126" s="1" t="n">
         <v>404266</v>
@@ -9736,11 +9755,11 @@
       <c r="E127" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F127" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="G127" s="18" t="s">
-        <v>212</v>
+      <c r="F127" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="G127" s="19" t="s">
+        <v>217</v>
       </c>
       <c r="H127" s="7" t="s">
         <v>123</v>
@@ -9779,7 +9798,7 @@
         <v>5</v>
       </c>
       <c r="T127" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U127" s="1" t="n">
         <v>404266</v>
@@ -9804,11 +9823,11 @@
       <c r="E128" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F128" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="G128" s="18" t="s">
-        <v>212</v>
+      <c r="F128" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="G128" s="19" t="s">
+        <v>217</v>
       </c>
       <c r="H128" s="7" t="s">
         <v>125</v>
@@ -9847,7 +9866,7 @@
         <v>5</v>
       </c>
       <c r="T128" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U128" s="1" t="n">
         <v>404266</v>
@@ -9872,11 +9891,11 @@
       <c r="E129" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F129" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="G129" s="18" t="s">
-        <v>214</v>
+      <c r="F129" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="G129" s="19" t="s">
+        <v>219</v>
       </c>
       <c r="H129" s="7" t="s">
         <v>121</v>
@@ -9915,7 +9934,7 @@
         <v>5</v>
       </c>
       <c r="T129" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U129" s="1" t="n">
         <v>404266</v>
@@ -9940,11 +9959,11 @@
       <c r="E130" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F130" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="G130" s="18" t="s">
-        <v>214</v>
+      <c r="F130" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="G130" s="19" t="s">
+        <v>219</v>
       </c>
       <c r="H130" s="7" t="s">
         <v>123</v>
@@ -9983,7 +10002,7 @@
         <v>5</v>
       </c>
       <c r="T130" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U130" s="1" t="n">
         <v>404266</v>
@@ -10008,11 +10027,11 @@
       <c r="E131" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F131" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="G131" s="18" t="s">
-        <v>214</v>
+      <c r="F131" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="G131" s="19" t="s">
+        <v>219</v>
       </c>
       <c r="H131" s="7" t="s">
         <v>125</v>
@@ -10051,7 +10070,7 @@
         <v>5</v>
       </c>
       <c r="T131" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U131" s="1" t="n">
         <v>404266</v>
@@ -10076,11 +10095,11 @@
       <c r="E132" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F132" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="G132" s="18" t="s">
-        <v>216</v>
+      <c r="F132" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="G132" s="19" t="s">
+        <v>221</v>
       </c>
       <c r="H132" s="7" t="s">
         <v>121</v>
@@ -10119,7 +10138,7 @@
         <v>5</v>
       </c>
       <c r="T132" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U132" s="1" t="n">
         <v>404266</v>
@@ -10144,11 +10163,11 @@
       <c r="E133" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F133" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="G133" s="18" t="s">
-        <v>216</v>
+      <c r="F133" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="G133" s="19" t="s">
+        <v>221</v>
       </c>
       <c r="H133" s="7" t="s">
         <v>123</v>
@@ -10187,7 +10206,7 @@
         <v>5</v>
       </c>
       <c r="T133" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U133" s="1" t="n">
         <v>404266</v>
@@ -10212,11 +10231,11 @@
       <c r="E134" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F134" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="G134" s="18" t="s">
-        <v>216</v>
+      <c r="F134" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="G134" s="19" t="s">
+        <v>221</v>
       </c>
       <c r="H134" s="7" t="s">
         <v>125</v>
@@ -10255,7 +10274,7 @@
         <v>5</v>
       </c>
       <c r="T134" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U134" s="1" t="n">
         <v>404266</v>
@@ -10280,11 +10299,11 @@
       <c r="E135" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F135" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="G135" s="18" t="s">
-        <v>218</v>
+      <c r="F135" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="G135" s="19" t="s">
+        <v>223</v>
       </c>
       <c r="H135" s="7" t="s">
         <v>121</v>
@@ -10323,7 +10342,7 @@
         <v>5</v>
       </c>
       <c r="T135" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U135" s="1" t="n">
         <v>404266</v>
@@ -10348,11 +10367,11 @@
       <c r="E136" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F136" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="G136" s="18" t="s">
-        <v>218</v>
+      <c r="F136" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="G136" s="19" t="s">
+        <v>223</v>
       </c>
       <c r="H136" s="7" t="s">
         <v>123</v>
@@ -10391,7 +10410,7 @@
         <v>5</v>
       </c>
       <c r="T136" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U136" s="1" t="n">
         <v>404266</v>
@@ -10416,11 +10435,11 @@
       <c r="E137" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F137" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="G137" s="18" t="s">
-        <v>218</v>
+      <c r="F137" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="G137" s="19" t="s">
+        <v>223</v>
       </c>
       <c r="H137" s="7" t="s">
         <v>125</v>
@@ -10459,7 +10478,7 @@
         <v>5</v>
       </c>
       <c r="T137" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U137" s="1" t="n">
         <v>404266</v>
@@ -10484,11 +10503,11 @@
       <c r="E138" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F138" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="G138" s="18" t="s">
-        <v>220</v>
+      <c r="F138" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="G138" s="19" t="s">
+        <v>225</v>
       </c>
       <c r="H138" s="7" t="s">
         <v>121</v>
@@ -10527,7 +10546,7 @@
         <v>5</v>
       </c>
       <c r="T138" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U138" s="1" t="n">
         <v>404266</v>
@@ -10552,11 +10571,11 @@
       <c r="E139" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F139" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="G139" s="18" t="s">
-        <v>220</v>
+      <c r="F139" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="G139" s="19" t="s">
+        <v>225</v>
       </c>
       <c r="H139" s="7" t="s">
         <v>123</v>
@@ -10595,7 +10614,7 @@
         <v>5</v>
       </c>
       <c r="T139" s="6" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U139" s="1" t="n">
         <v>404266</v>
@@ -10620,11 +10639,11 @@
       <c r="E140" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F140" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="G140" s="20" t="s">
-        <v>220</v>
+      <c r="F140" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="G140" s="21" t="s">
+        <v>225</v>
       </c>
       <c r="H140" s="12" t="s">
         <v>125</v>
@@ -10663,7 +10682,7 @@
         <v>5</v>
       </c>
       <c r="T140" s="14" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="U140" s="14" t="n">
         <v>404266</v>
@@ -10688,11 +10707,11 @@
       <c r="E141" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F141" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="G141" s="18" t="s">
-        <v>222</v>
+      <c r="F141" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="G141" s="19" t="s">
+        <v>227</v>
       </c>
       <c r="H141" s="7" t="s">
         <v>129</v>
@@ -10731,7 +10750,7 @@
         <v>6</v>
       </c>
       <c r="T141" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U141" s="1" t="n">
         <v>404264</v>
@@ -10756,11 +10775,11 @@
       <c r="E142" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F142" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="G142" s="18" t="s">
-        <v>222</v>
+      <c r="F142" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="G142" s="19" t="s">
+        <v>227</v>
       </c>
       <c r="H142" s="7" t="s">
         <v>131</v>
@@ -10799,7 +10818,7 @@
         <v>6</v>
       </c>
       <c r="T142" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U142" s="1" t="n">
         <v>404264</v>
@@ -10824,11 +10843,11 @@
       <c r="E143" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F143" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="G143" s="18" t="s">
-        <v>222</v>
+      <c r="F143" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="G143" s="19" t="s">
+        <v>227</v>
       </c>
       <c r="H143" s="7" t="s">
         <v>133</v>
@@ -10867,7 +10886,7 @@
         <v>6</v>
       </c>
       <c r="T143" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U143" s="1" t="n">
         <v>404264</v>
@@ -10892,11 +10911,11 @@
       <c r="E144" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F144" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="G144" s="18" t="s">
-        <v>225</v>
+      <c r="F144" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="G144" s="19" t="s">
+        <v>230</v>
       </c>
       <c r="H144" s="7" t="s">
         <v>129</v>
@@ -10935,7 +10954,7 @@
         <v>6</v>
       </c>
       <c r="T144" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U144" s="1" t="n">
         <v>404264</v>
@@ -10960,11 +10979,11 @@
       <c r="E145" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F145" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="G145" s="18" t="s">
-        <v>225</v>
+      <c r="F145" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="G145" s="19" t="s">
+        <v>230</v>
       </c>
       <c r="H145" s="7" t="s">
         <v>131</v>
@@ -11003,7 +11022,7 @@
         <v>6</v>
       </c>
       <c r="T145" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U145" s="1" t="n">
         <v>404264</v>
@@ -11028,11 +11047,11 @@
       <c r="E146" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F146" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="G146" s="18" t="s">
-        <v>225</v>
+      <c r="F146" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="G146" s="19" t="s">
+        <v>230</v>
       </c>
       <c r="H146" s="7" t="s">
         <v>133</v>
@@ -11071,7 +11090,7 @@
         <v>6</v>
       </c>
       <c r="T146" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U146" s="1" t="n">
         <v>404264</v>
@@ -11096,11 +11115,11 @@
       <c r="E147" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F147" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="G147" s="18" t="s">
-        <v>227</v>
+      <c r="F147" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="G147" s="19" t="s">
+        <v>232</v>
       </c>
       <c r="H147" s="7" t="s">
         <v>129</v>
@@ -11139,7 +11158,7 @@
         <v>6</v>
       </c>
       <c r="T147" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U147" s="1" t="n">
         <v>404264</v>
@@ -11164,11 +11183,11 @@
       <c r="E148" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F148" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="G148" s="18" t="s">
-        <v>227</v>
+      <c r="F148" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="G148" s="19" t="s">
+        <v>232</v>
       </c>
       <c r="H148" s="7" t="s">
         <v>131</v>
@@ -11207,7 +11226,7 @@
         <v>6</v>
       </c>
       <c r="T148" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U148" s="1" t="n">
         <v>404264</v>
@@ -11232,11 +11251,11 @@
       <c r="E149" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F149" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="G149" s="18" t="s">
-        <v>227</v>
+      <c r="F149" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="G149" s="19" t="s">
+        <v>232</v>
       </c>
       <c r="H149" s="7" t="s">
         <v>133</v>
@@ -11275,7 +11294,7 @@
         <v>6</v>
       </c>
       <c r="T149" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U149" s="1" t="n">
         <v>404264</v>
@@ -11300,11 +11319,11 @@
       <c r="E150" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F150" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="G150" s="18" t="s">
-        <v>229</v>
+      <c r="F150" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="G150" s="19" t="s">
+        <v>234</v>
       </c>
       <c r="H150" s="7" t="s">
         <v>129</v>
@@ -11343,7 +11362,7 @@
         <v>6</v>
       </c>
       <c r="T150" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U150" s="1" t="n">
         <v>404264</v>
@@ -11368,11 +11387,11 @@
       <c r="E151" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F151" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="G151" s="18" t="s">
-        <v>229</v>
+      <c r="F151" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="G151" s="19" t="s">
+        <v>234</v>
       </c>
       <c r="H151" s="7" t="s">
         <v>131</v>
@@ -11411,7 +11430,7 @@
         <v>6</v>
       </c>
       <c r="T151" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U151" s="1" t="n">
         <v>404264</v>
@@ -11436,11 +11455,11 @@
       <c r="E152" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F152" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="G152" s="18" t="s">
-        <v>229</v>
+      <c r="F152" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="G152" s="19" t="s">
+        <v>234</v>
       </c>
       <c r="H152" s="7" t="s">
         <v>133</v>
@@ -11479,7 +11498,7 @@
         <v>6</v>
       </c>
       <c r="T152" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U152" s="1" t="n">
         <v>404264</v>
@@ -11504,11 +11523,11 @@
       <c r="E153" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F153" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="G153" s="18" t="s">
-        <v>231</v>
+      <c r="F153" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="G153" s="19" t="s">
+        <v>236</v>
       </c>
       <c r="H153" s="7" t="s">
         <v>129</v>
@@ -11547,7 +11566,7 @@
         <v>6</v>
       </c>
       <c r="T153" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U153" s="1" t="n">
         <v>404264</v>
@@ -11572,11 +11591,11 @@
       <c r="E154" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F154" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="G154" s="18" t="s">
-        <v>231</v>
+      <c r="F154" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="G154" s="19" t="s">
+        <v>236</v>
       </c>
       <c r="H154" s="7" t="s">
         <v>131</v>
@@ -11615,7 +11634,7 @@
         <v>6</v>
       </c>
       <c r="T154" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U154" s="1" t="n">
         <v>404264</v>
@@ -11640,11 +11659,11 @@
       <c r="E155" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F155" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="G155" s="18" t="s">
-        <v>231</v>
+      <c r="F155" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="G155" s="19" t="s">
+        <v>236</v>
       </c>
       <c r="H155" s="7" t="s">
         <v>133</v>
@@ -11683,7 +11702,7 @@
         <v>6</v>
       </c>
       <c r="T155" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U155" s="1" t="n">
         <v>404264</v>
@@ -11708,11 +11727,11 @@
       <c r="E156" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F156" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="G156" s="17" t="s">
-        <v>233</v>
+      <c r="F156" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="G156" s="18" t="s">
+        <v>238</v>
       </c>
       <c r="H156" s="7" t="s">
         <v>129</v>
@@ -11751,7 +11770,7 @@
         <v>6</v>
       </c>
       <c r="T156" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U156" s="1" t="n">
         <v>404264</v>
@@ -11776,11 +11795,11 @@
       <c r="E157" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F157" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="G157" s="17" t="s">
-        <v>233</v>
+      <c r="F157" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="G157" s="18" t="s">
+        <v>238</v>
       </c>
       <c r="H157" s="7" t="s">
         <v>131</v>
@@ -11819,7 +11838,7 @@
         <v>6</v>
       </c>
       <c r="T157" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U157" s="1" t="n">
         <v>404264</v>
@@ -11844,11 +11863,11 @@
       <c r="E158" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F158" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="G158" s="17" t="s">
-        <v>233</v>
+      <c r="F158" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="G158" s="18" t="s">
+        <v>238</v>
       </c>
       <c r="H158" s="7" t="s">
         <v>133</v>
@@ -11887,7 +11906,7 @@
         <v>6</v>
       </c>
       <c r="T158" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U158" s="1" t="n">
         <v>404264</v>
@@ -11912,11 +11931,11 @@
       <c r="E159" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F159" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="G159" s="17" t="s">
-        <v>235</v>
+      <c r="F159" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G159" s="18" t="s">
+        <v>240</v>
       </c>
       <c r="H159" s="7" t="s">
         <v>129</v>
@@ -11955,7 +11974,7 @@
         <v>6</v>
       </c>
       <c r="T159" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U159" s="1" t="n">
         <v>404264</v>
@@ -11980,11 +11999,11 @@
       <c r="E160" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F160" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="G160" s="17" t="s">
-        <v>235</v>
+      <c r="F160" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G160" s="18" t="s">
+        <v>240</v>
       </c>
       <c r="H160" s="7" t="s">
         <v>131</v>
@@ -12023,7 +12042,7 @@
         <v>6</v>
       </c>
       <c r="T160" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U160" s="1" t="n">
         <v>404264</v>
@@ -12048,11 +12067,11 @@
       <c r="E161" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F161" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="G161" s="17" t="s">
-        <v>235</v>
+      <c r="F161" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G161" s="18" t="s">
+        <v>240</v>
       </c>
       <c r="H161" s="7" t="s">
         <v>133</v>
@@ -12091,7 +12110,7 @@
         <v>6</v>
       </c>
       <c r="T161" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U161" s="1" t="n">
         <v>404264</v>
@@ -12116,11 +12135,11 @@
       <c r="E162" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F162" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="G162" s="17" t="s">
-        <v>237</v>
+      <c r="F162" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="G162" s="18" t="s">
+        <v>242</v>
       </c>
       <c r="H162" s="7" t="s">
         <v>129</v>
@@ -12159,7 +12178,7 @@
         <v>6</v>
       </c>
       <c r="T162" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U162" s="1" t="n">
         <v>404264</v>
@@ -12184,11 +12203,11 @@
       <c r="E163" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F163" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="G163" s="17" t="s">
-        <v>237</v>
+      <c r="F163" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="G163" s="18" t="s">
+        <v>242</v>
       </c>
       <c r="H163" s="7" t="s">
         <v>131</v>
@@ -12227,7 +12246,7 @@
         <v>6</v>
       </c>
       <c r="T163" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U163" s="1" t="n">
         <v>404264</v>
@@ -12252,11 +12271,11 @@
       <c r="E164" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F164" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="G164" s="17" t="s">
-        <v>237</v>
+      <c r="F164" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="G164" s="18" t="s">
+        <v>242</v>
       </c>
       <c r="H164" s="7" t="s">
         <v>133</v>
@@ -12295,7 +12314,7 @@
         <v>6</v>
       </c>
       <c r="T164" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U164" s="1" t="n">
         <v>404264</v>
@@ -12320,10 +12339,10 @@
       <c r="E165" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F165" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="G165" s="17" t="s">
+      <c r="F165" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="G165" s="18" t="s">
         <v>73</v>
       </c>
       <c r="H165" s="7" t="s">
@@ -12363,7 +12382,7 @@
         <v>6</v>
       </c>
       <c r="T165" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U165" s="1" t="n">
         <v>404264</v>
@@ -12388,10 +12407,10 @@
       <c r="E166" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F166" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="G166" s="17" t="s">
+      <c r="F166" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="G166" s="18" t="s">
         <v>73</v>
       </c>
       <c r="H166" s="7" t="s">
@@ -12431,7 +12450,7 @@
         <v>6</v>
       </c>
       <c r="T166" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U166" s="1" t="n">
         <v>404264</v>
@@ -12456,10 +12475,10 @@
       <c r="E167" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F167" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="G167" s="17" t="s">
+      <c r="F167" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="G167" s="18" t="s">
         <v>73</v>
       </c>
       <c r="H167" s="7" t="s">
@@ -12499,7 +12518,7 @@
         <v>6</v>
       </c>
       <c r="T167" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U167" s="1" t="n">
         <v>404264</v>
@@ -12524,11 +12543,11 @@
       <c r="E168" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F168" s="17" t="s">
-        <v>239</v>
-      </c>
-      <c r="G168" s="17" t="s">
-        <v>240</v>
+      <c r="F168" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="G168" s="18" t="s">
+        <v>245</v>
       </c>
       <c r="H168" s="7" t="s">
         <v>129</v>
@@ -12567,7 +12586,7 @@
         <v>6</v>
       </c>
       <c r="T168" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U168" s="1" t="n">
         <v>404264</v>
@@ -12592,11 +12611,11 @@
       <c r="E169" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F169" s="17" t="s">
-        <v>239</v>
-      </c>
-      <c r="G169" s="17" t="s">
-        <v>240</v>
+      <c r="F169" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="G169" s="18" t="s">
+        <v>245</v>
       </c>
       <c r="H169" s="7" t="s">
         <v>131</v>
@@ -12635,7 +12654,7 @@
         <v>6</v>
       </c>
       <c r="T169" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U169" s="1" t="n">
         <v>404264</v>
@@ -12660,11 +12679,11 @@
       <c r="E170" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F170" s="17" t="s">
-        <v>239</v>
-      </c>
-      <c r="G170" s="17" t="s">
-        <v>240</v>
+      <c r="F170" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="G170" s="18" t="s">
+        <v>245</v>
       </c>
       <c r="H170" s="7" t="s">
         <v>133</v>
@@ -12703,7 +12722,7 @@
         <v>6</v>
       </c>
       <c r="T170" s="6" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="U170" s="1" t="n">
         <v>404264</v>
@@ -12723,22 +12742,22 @@
         <v>10056</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="E171" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F171" s="17" t="s">
-        <v>242</v>
-      </c>
-      <c r="G171" s="17" t="s">
-        <v>243</v>
+      <c r="F171" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="G171" s="18" t="s">
+        <v>248</v>
       </c>
       <c r="H171" s="7" t="s">
         <v>133</v>
       </c>
       <c r="I171" s="8" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="J171" s="1" t="n">
         <v>286352</v>
@@ -12770,8 +12789,8 @@
       <c r="S171" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="T171" s="17" t="s">
-        <v>245</v>
+      <c r="T171" s="18" t="s">
+        <v>250</v>
       </c>
       <c r="U171" s="1" t="n">
         <v>404264</v>

</xml_diff>

<commit_message>
feat：update stage excel and map5
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Stage_关卡表.xlsx
+++ b/nevergiveup/Excel/Stage_关卡表.xlsx
@@ -1251,10 +1251,10 @@
   </sheetPr>
   <dimension ref="A1:V171"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F88" activeCellId="0" sqref="F88"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.48828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat：update stage config change
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Stage_关卡表.xlsx
+++ b/nevergiveup/Excel/Stage_关卡表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2067" uniqueCount="256">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -782,6 +782,12 @@
   </si>
   <si>
     <t xml:space="preserve">300|300|300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3842.29|-18997.09|-73.57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4.83|0|29.75</t>
   </si>
 </sst>
 </file>
@@ -915,7 +921,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -998,6 +1004,10 @@
     </xf>
     <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1249,12 +1259,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V171"/>
+  <dimension ref="A1:V172"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="N110" activeCellId="0" sqref="N110"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D182" activeCellId="0" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.48828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12771,7 +12781,7 @@
         <v>25</v>
       </c>
       <c r="L171" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M171" s="4" t="n">
         <v>3</v>
@@ -12802,6 +12812,74 @@
       </c>
       <c r="V171" s="1" t="n">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="5" t="n">
+        <v>7001</v>
+      </c>
+      <c r="B172" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C172" s="5" t="n">
+        <v>10057</v>
+      </c>
+      <c r="D172" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E172" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F172" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="G172" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="H172" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I172" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J172" s="4" t="n">
+        <v>267079</v>
+      </c>
+      <c r="K172" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L172" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M172" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N172" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O172" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="P172" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q172" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="R172" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="S172" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="T172" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="U172" s="1" t="n">
+        <v>404268</v>
+      </c>
+      <c r="V172" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat：update npc and test level
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Stage_关卡表.xlsx
+++ b/nevergiveup/Excel/Stage_关卡表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2067" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2067" uniqueCount="257">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -784,10 +784,13 @@
     <t xml:space="preserve">300|300|300</t>
   </si>
   <si>
-    <t xml:space="preserve">3842.29|-18997.09|-73.57</t>
+    <t xml:space="preserve">3753.13|-18832.4|-158.57</t>
   </si>
   <si>
     <t xml:space="preserve">-4.83|0|29.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">训练关卡</t>
   </si>
 </sst>
 </file>
@@ -1261,10 +1264,10 @@
   </sheetPr>
   <dimension ref="A1:V172"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="M159" activeCellId="0" sqref="M159"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="M177" activeCellId="0" sqref="M177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.48828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12840,7 +12843,7 @@
         <v>58</v>
       </c>
       <c r="I172" s="8" t="s">
-        <v>59</v>
+        <v>256</v>
       </c>
       <c r="J172" s="4" t="n">
         <v>267079</v>

</xml_diff>

<commit_message>
feat：update stage excel and level change
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Stage_关卡表.xlsx
+++ b/nevergiveup/Excel/Stage_关卡表.xlsx
@@ -1264,10 +1264,10 @@
   </sheetPr>
   <dimension ref="A1:V172"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="M177" activeCellId="0" sqref="M177"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F170" activeCellId="0" sqref="F170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.48828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12822,7 +12822,7 @@
         <v>7001</v>
       </c>
       <c r="B172" s="5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C172" s="5" t="n">
         <v>10057</v>

</xml_diff>

<commit_message>
fix: change training reset position
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Stage_关卡表.xlsx
+++ b/nevergiveup/Excel/Stage_关卡表.xlsx
@@ -2043,10 +2043,10 @@
   <sheetPr/>
   <dimension ref="A1:V172"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D176" sqref="D176"/>
+      <selection pane="bottomLeft" activeCell="T172" sqref="T172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4916666666667" defaultRowHeight="14.5"/>
@@ -13654,8 +13654,8 @@
       <c r="S172" s="2">
         <v>2</v>
       </c>
-      <c r="T172" s="6" t="s">
-        <v>65</v>
+      <c r="T172" s="14" t="s">
+        <v>253</v>
       </c>
       <c r="U172" s="2">
         <v>404268</v>

</xml_diff>

<commit_message>
feat: update Stage config
更新关卡首通奖励和后续通关奖励一致
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Stage_关卡表.xlsx
+++ b/nevergiveup/Excel/Stage_关卡表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6862613F-6221-442F-AFA2-D79F2E96D647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABDF35B-FE8C-46D8-A45C-5FCE9C435117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1797" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2067" uniqueCount="291">
   <si>
     <t>int</t>
   </si>
@@ -787,118 +787,130 @@
     <t>-0.56|-0.35|157.70</t>
   </si>
   <si>
-    <t>1023|1</t>
+    <t>1|20||2|7||3|5</t>
+  </si>
+  <si>
+    <t>1|20||2|7||3|6</t>
+  </si>
+  <si>
+    <t>1|20||2|7||3|7</t>
+  </si>
+  <si>
+    <t>1|20||2|7||3|8</t>
+  </si>
+  <si>
+    <t>1|20||2|7||3|9</t>
+  </si>
+  <si>
+    <t>1|50||2|20||3|12</t>
+  </si>
+  <si>
+    <t>1|60||2|30||3|12</t>
+  </si>
+  <si>
+    <t>1|70||2|40||3|12</t>
+  </si>
+  <si>
+    <t>1|30||2|10||3|10</t>
+  </si>
+  <si>
+    <t>1|35||2|15||3|10</t>
+  </si>
+  <si>
+    <t>1|40||2|20||3|10</t>
+  </si>
+  <si>
+    <t>1|70||2|40||3|14</t>
+  </si>
+  <si>
+    <t>1|40||2|20||3|12</t>
+  </si>
+  <si>
+    <t>1|100||2|50||3|22</t>
+  </si>
+  <si>
+    <t>1|60||2|25||3|12</t>
+  </si>
+  <si>
+    <t>1|150||2|70||3|29</t>
+  </si>
+  <si>
+    <t>1|80||2|35||3|12</t>
+  </si>
+  <si>
+    <t>1|140||2|65||3|17</t>
+  </si>
+  <si>
+    <t>1|70||2|30||3|12</t>
+  </si>
+  <si>
+    <t>1|170||2|70||3|24</t>
+  </si>
+  <si>
+    <t>1|80||2|35||3|14</t>
+  </si>
+  <si>
+    <t>1|200||2|80||3|31</t>
+  </si>
+  <si>
+    <t>1|90||2|40||3|16</t>
+  </si>
+  <si>
+    <t>1|180||2|70||3|17</t>
+  </si>
+  <si>
+    <t>1|220||2|90||3|24</t>
+  </si>
+  <si>
+    <t>1|100||2|45||3|14</t>
+  </si>
+  <si>
+    <t>1|240||2|100||3|31</t>
+  </si>
+  <si>
+    <t>1|110||2|50||3|16</t>
+  </si>
+  <si>
+    <t>1|220||2|90||3|17</t>
+  </si>
+  <si>
+    <t>1|100||2|45||3|12</t>
+  </si>
+  <si>
+    <t>1|300||2|120||3|24</t>
+  </si>
+  <si>
+    <t>1|140||2|60||3|14</t>
+  </si>
+  <si>
+    <t>1|400||2|160||3|31</t>
+  </si>
+  <si>
+    <t>1|180||2|80||3|16</t>
+  </si>
+  <si>
+    <t>1|50||2|20||3|12</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>1005|1</t>
+    <t>1023|1||1|50||2|20||3|12</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>1017|1</t>
+    <t>1|60||2|30||3|12</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>1|20||2|7||3|5</t>
-  </si>
-  <si>
-    <t>1|20||2|7||3|6</t>
-  </si>
-  <si>
-    <t>1|20||2|7||3|7</t>
-  </si>
-  <si>
-    <t>1|20||2|7||3|8</t>
-  </si>
-  <si>
-    <t>1|20||2|7||3|9</t>
-  </si>
-  <si>
-    <t>1|50||2|20||3|12</t>
-  </si>
-  <si>
-    <t>1|60||2|30||3|12</t>
+    <t>1005|1||1|60||2|30||3|12</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>1|70||2|40||3|12</t>
-  </si>
-  <si>
-    <t>1|30||2|10||3|10</t>
-  </si>
-  <si>
-    <t>1|35||2|15||3|10</t>
-  </si>
-  <si>
-    <t>1|40||2|20||3|10</t>
-  </si>
-  <si>
-    <t>1|70||2|40||3|14</t>
-  </si>
-  <si>
-    <t>1|40||2|20||3|12</t>
-  </si>
-  <si>
-    <t>1|100||2|50||3|22</t>
-  </si>
-  <si>
-    <t>1|60||2|25||3|12</t>
-  </si>
-  <si>
-    <t>1|150||2|70||3|29</t>
-  </si>
-  <si>
-    <t>1|80||2|35||3|12</t>
-  </si>
-  <si>
-    <t>1|140||2|65||3|17</t>
-  </si>
-  <si>
-    <t>1|70||2|30||3|12</t>
-  </si>
-  <si>
-    <t>1|170||2|70||3|24</t>
-  </si>
-  <si>
-    <t>1|80||2|35||3|14</t>
-  </si>
-  <si>
-    <t>1|200||2|80||3|31</t>
-  </si>
-  <si>
-    <t>1|90||2|40||3|16</t>
-  </si>
-  <si>
-    <t>1|180||2|70||3|17</t>
-  </si>
-  <si>
-    <t>1|220||2|90||3|24</t>
-  </si>
-  <si>
-    <t>1|100||2|45||3|14</t>
-  </si>
-  <si>
-    <t>1|240||2|100||3|31</t>
-  </si>
-  <si>
-    <t>1|110||2|50||3|16</t>
-  </si>
-  <si>
-    <t>1|220||2|90||3|17</t>
-  </si>
-  <si>
-    <t>1|100||2|45||3|12</t>
-  </si>
-  <si>
-    <t>1|300||2|120||3|24</t>
-  </si>
-  <si>
-    <t>1|140||2|60||3|14</t>
-  </si>
-  <si>
-    <t>1|400||2|160||3|31</t>
-  </si>
-  <si>
-    <t>1|180||2|80||3|16</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1017|1||1|70||2|40||3|12</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1515,8 +1527,8 @@
   <dimension ref="A1:V172"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P160" sqref="P160"/>
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -2839,17 +2851,19 @@
         <v>1</v>
       </c>
       <c r="N21" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="O21" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="P21" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q21" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="R21" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="O21" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="R21" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="S21">
         <v>2</v>
@@ -2905,17 +2919,19 @@
         <v>1</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="O22" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="P22" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="P22" s="8"/>
       <c r="Q22" s="10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="R22" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S22">
         <v>2</v>
@@ -2971,17 +2987,19 @@
         <v>1</v>
       </c>
       <c r="N23" s="8" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="O23" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="P23" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="P23" s="8"/>
       <c r="Q23" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="R23" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S23">
         <v>2</v>
@@ -3037,17 +3055,19 @@
         <v>1</v>
       </c>
       <c r="N24" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="O24" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q24" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="R24" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="O24" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="R24" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="S24">
         <v>2</v>
@@ -3103,17 +3123,19 @@
         <v>1</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="O25" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="P25" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="P25" s="8"/>
       <c r="Q25" s="10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="R25" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S25">
         <v>2</v>
@@ -3169,17 +3191,19 @@
         <v>1</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="O26" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="P26" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="P26" s="8"/>
       <c r="Q26" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="R26" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S26">
         <v>2</v>
@@ -3235,17 +3259,19 @@
         <v>1</v>
       </c>
       <c r="N27" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="O27" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="P27" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q27" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="R27" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="O27" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="R27" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="S27">
         <v>2</v>
@@ -3301,17 +3327,19 @@
         <v>1</v>
       </c>
       <c r="N28" s="8" t="s">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="O28" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="P28" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="P28" s="8"/>
       <c r="Q28" s="10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="R28" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S28">
         <v>2</v>
@@ -3367,17 +3395,19 @@
         <v>1</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="O29" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="P29" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="P29" s="8"/>
       <c r="Q29" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="R29" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S29">
         <v>2</v>
@@ -3433,17 +3463,19 @@
         <v>1</v>
       </c>
       <c r="N30" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="O30" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="P30" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q30" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="R30" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="O30" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="R30" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="S30">
         <v>2</v>
@@ -3499,17 +3531,19 @@
         <v>1</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="O31" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="P31" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="P31" s="8"/>
       <c r="Q31" s="10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="R31" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S31">
         <v>2</v>
@@ -3565,17 +3599,19 @@
         <v>1</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="O32" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="P32" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="P32" s="8"/>
       <c r="Q32" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="R32" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S32">
         <v>2</v>
@@ -3631,17 +3667,19 @@
         <v>1</v>
       </c>
       <c r="N33" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="O33" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="P33" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q33" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="R33" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="O33" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="R33" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="S33">
         <v>2</v>
@@ -3697,17 +3735,19 @@
         <v>1</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="O34" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="P34" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="P34" s="8"/>
       <c r="Q34" s="10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="R34" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S34">
         <v>2</v>
@@ -3763,17 +3803,19 @@
         <v>1</v>
       </c>
       <c r="N35" s="8" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="O35" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="P35" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="P35" s="8"/>
       <c r="Q35" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="R35" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S35">
         <v>2</v>
@@ -3829,17 +3871,19 @@
         <v>1</v>
       </c>
       <c r="N36" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="O36" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="P36" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q36" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="R36" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="O36" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="R36" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="S36">
         <v>2</v>
@@ -3895,17 +3939,19 @@
         <v>1</v>
       </c>
       <c r="N37" s="8" t="s">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="O37" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="P37" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="P37" s="8"/>
       <c r="Q37" s="10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="R37" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S37">
         <v>2</v>
@@ -3961,17 +4007,19 @@
         <v>1</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="O38" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="P38" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="P38" s="8"/>
       <c r="Q38" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="R38" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S38">
         <v>2</v>
@@ -4027,17 +4075,19 @@
         <v>1</v>
       </c>
       <c r="N39" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="O39" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="P39" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q39" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="R39" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="O39" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="R39" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="S39">
         <v>2</v>
@@ -4093,17 +4143,19 @@
         <v>1</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="O40" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="P40" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="P40" s="8"/>
       <c r="Q40" s="10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="R40" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S40">
         <v>2</v>
@@ -4159,17 +4211,19 @@
         <v>1</v>
       </c>
       <c r="N41" s="8" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="O41" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="P41" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="P41" s="8"/>
       <c r="Q41" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="R41" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S41">
         <v>2</v>
@@ -4225,17 +4279,19 @@
         <v>1</v>
       </c>
       <c r="N42" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="O42" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q42" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="R42" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="O42" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="R42" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="S42">
         <v>2</v>
@@ -4291,17 +4347,19 @@
         <v>1</v>
       </c>
       <c r="N43" s="8" t="s">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="O43" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="P43" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="P43" s="8"/>
       <c r="Q43" s="10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="R43" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S43">
         <v>2</v>
@@ -4357,17 +4415,19 @@
         <v>1</v>
       </c>
       <c r="N44" s="8" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="O44" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="P44" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="P44" s="8"/>
       <c r="Q44" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="R44" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S44">
         <v>2</v>
@@ -4423,17 +4483,19 @@
         <v>1</v>
       </c>
       <c r="N45" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="O45" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q45" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="R45" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="O45" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="R45" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="S45">
         <v>2</v>
@@ -4489,17 +4551,19 @@
         <v>1</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="O46" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="P46" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="P46" s="8"/>
       <c r="Q46" s="10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="R46" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S46">
         <v>2</v>
@@ -4555,17 +4619,19 @@
         <v>1</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="O47" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="P47" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="P47" s="8"/>
       <c r="Q47" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="R47" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S47">
         <v>2</v>
@@ -4621,17 +4687,19 @@
         <v>1</v>
       </c>
       <c r="N48" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="O48" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="P48" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q48" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="R48" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="O48" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="P48" s="8"/>
-      <c r="Q48" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="R48" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="S48">
         <v>2</v>
@@ -4687,17 +4755,19 @@
         <v>1</v>
       </c>
       <c r="N49" s="8" t="s">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="O49" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="P49" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="P49" s="8"/>
       <c r="Q49" s="10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="R49" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S49">
         <v>2</v>
@@ -4753,17 +4823,19 @@
         <v>1</v>
       </c>
       <c r="N50" s="8" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="O50" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="P50" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="P50" s="8"/>
       <c r="Q50" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="R50" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S50">
         <v>2</v>
@@ -4818,16 +4890,20 @@
       <c r="M51" s="2">
         <v>1</v>
       </c>
-      <c r="N51" s="8"/>
+      <c r="N51" s="10" t="s">
+        <v>262</v>
+      </c>
       <c r="O51" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="P51" s="8"/>
+        <v>262</v>
+      </c>
+      <c r="P51" s="10" t="s">
+        <v>263</v>
+      </c>
       <c r="Q51" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="R51" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S51">
         <v>3</v>
@@ -4882,16 +4958,20 @@
       <c r="M52" s="2">
         <v>1</v>
       </c>
-      <c r="N52" s="8"/>
+      <c r="N52" s="10" t="s">
+        <v>264</v>
+      </c>
       <c r="O52" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="P52" s="8"/>
+        <v>264</v>
+      </c>
+      <c r="P52" s="10" t="s">
+        <v>265</v>
+      </c>
       <c r="Q52" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="R52" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S52">
         <v>3</v>
@@ -4946,16 +5026,20 @@
       <c r="M53" s="2">
         <v>1</v>
       </c>
-      <c r="N53" s="8"/>
+      <c r="N53" s="10" t="s">
+        <v>266</v>
+      </c>
       <c r="O53" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="P53" s="8"/>
+        <v>266</v>
+      </c>
+      <c r="P53" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q53" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R53" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S53">
         <v>3</v>
@@ -5010,16 +5094,20 @@
       <c r="M54" s="2">
         <v>1</v>
       </c>
-      <c r="N54" s="8"/>
+      <c r="N54" s="10" t="s">
+        <v>262</v>
+      </c>
       <c r="O54" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="P54" s="8"/>
+        <v>262</v>
+      </c>
+      <c r="P54" s="10" t="s">
+        <v>263</v>
+      </c>
       <c r="Q54" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="R54" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S54">
         <v>3</v>
@@ -5074,16 +5162,20 @@
       <c r="M55" s="2">
         <v>1</v>
       </c>
-      <c r="N55" s="8"/>
+      <c r="N55" s="10" t="s">
+        <v>264</v>
+      </c>
       <c r="O55" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="P55" s="8"/>
+        <v>264</v>
+      </c>
+      <c r="P55" s="10" t="s">
+        <v>265</v>
+      </c>
       <c r="Q55" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="R55" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S55">
         <v>3</v>
@@ -5138,16 +5230,20 @@
       <c r="M56" s="2">
         <v>1</v>
       </c>
-      <c r="N56" s="8"/>
+      <c r="N56" s="10" t="s">
+        <v>266</v>
+      </c>
       <c r="O56" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="P56" s="8"/>
+        <v>266</v>
+      </c>
+      <c r="P56" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q56" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R56" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S56">
         <v>3</v>
@@ -5202,16 +5298,20 @@
       <c r="M57" s="2">
         <v>1</v>
       </c>
-      <c r="N57" s="8"/>
+      <c r="N57" s="10" t="s">
+        <v>262</v>
+      </c>
       <c r="O57" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="P57" s="8"/>
+        <v>262</v>
+      </c>
+      <c r="P57" s="10" t="s">
+        <v>263</v>
+      </c>
       <c r="Q57" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="R57" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S57">
         <v>3</v>
@@ -5266,16 +5366,20 @@
       <c r="M58" s="2">
         <v>1</v>
       </c>
-      <c r="N58" s="8"/>
+      <c r="N58" s="10" t="s">
+        <v>264</v>
+      </c>
       <c r="O58" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="P58" s="8"/>
+        <v>264</v>
+      </c>
+      <c r="P58" s="10" t="s">
+        <v>265</v>
+      </c>
       <c r="Q58" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="R58" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S58">
         <v>3</v>
@@ -5330,16 +5434,20 @@
       <c r="M59" s="2">
         <v>1</v>
       </c>
-      <c r="N59" s="8"/>
+      <c r="N59" s="10" t="s">
+        <v>266</v>
+      </c>
       <c r="O59" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="P59" s="8"/>
+        <v>266</v>
+      </c>
+      <c r="P59" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q59" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R59" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S59">
         <v>3</v>
@@ -5394,16 +5502,20 @@
       <c r="M60" s="2">
         <v>1</v>
       </c>
-      <c r="N60" s="8"/>
+      <c r="N60" s="10" t="s">
+        <v>262</v>
+      </c>
       <c r="O60" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="P60" s="8"/>
+        <v>262</v>
+      </c>
+      <c r="P60" s="10" t="s">
+        <v>263</v>
+      </c>
       <c r="Q60" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="R60" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S60">
         <v>3</v>
@@ -5458,16 +5570,20 @@
       <c r="M61" s="2">
         <v>1</v>
       </c>
-      <c r="N61" s="8"/>
+      <c r="N61" s="10" t="s">
+        <v>264</v>
+      </c>
       <c r="O61" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="P61" s="8"/>
+        <v>264</v>
+      </c>
+      <c r="P61" s="10" t="s">
+        <v>265</v>
+      </c>
       <c r="Q61" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="R61" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S61">
         <v>3</v>
@@ -5522,16 +5638,20 @@
       <c r="M62" s="2">
         <v>1</v>
       </c>
-      <c r="N62" s="8"/>
+      <c r="N62" s="10" t="s">
+        <v>266</v>
+      </c>
       <c r="O62" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="P62" s="8"/>
+        <v>266</v>
+      </c>
+      <c r="P62" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q62" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R62" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S62">
         <v>3</v>
@@ -5586,16 +5706,20 @@
       <c r="M63" s="2">
         <v>1</v>
       </c>
-      <c r="N63" s="8"/>
+      <c r="N63" s="10" t="s">
+        <v>262</v>
+      </c>
       <c r="O63" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="P63" s="8"/>
+        <v>262</v>
+      </c>
+      <c r="P63" s="10" t="s">
+        <v>263</v>
+      </c>
       <c r="Q63" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="R63" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S63">
         <v>3</v>
@@ -5650,16 +5774,20 @@
       <c r="M64" s="2">
         <v>1</v>
       </c>
-      <c r="N64" s="8"/>
+      <c r="N64" s="10" t="s">
+        <v>264</v>
+      </c>
       <c r="O64" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="P64" s="8"/>
+        <v>264</v>
+      </c>
+      <c r="P64" s="10" t="s">
+        <v>265</v>
+      </c>
       <c r="Q64" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="R64" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S64">
         <v>3</v>
@@ -5714,16 +5842,20 @@
       <c r="M65" s="2">
         <v>1</v>
       </c>
-      <c r="N65" s="8"/>
+      <c r="N65" s="10" t="s">
+        <v>266</v>
+      </c>
       <c r="O65" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="P65" s="8"/>
+        <v>266</v>
+      </c>
+      <c r="P65" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q65" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R65" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S65">
         <v>3</v>
@@ -5778,16 +5910,20 @@
       <c r="M66" s="2">
         <v>1</v>
       </c>
-      <c r="N66" s="8"/>
+      <c r="N66" s="10" t="s">
+        <v>262</v>
+      </c>
       <c r="O66" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="P66" s="8"/>
+        <v>262</v>
+      </c>
+      <c r="P66" s="10" t="s">
+        <v>263</v>
+      </c>
       <c r="Q66" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="R66" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S66">
         <v>3</v>
@@ -5842,16 +5978,20 @@
       <c r="M67" s="2">
         <v>1</v>
       </c>
-      <c r="N67" s="8"/>
+      <c r="N67" s="10" t="s">
+        <v>264</v>
+      </c>
       <c r="O67" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="P67" s="8"/>
+        <v>264</v>
+      </c>
+      <c r="P67" s="10" t="s">
+        <v>265</v>
+      </c>
       <c r="Q67" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="R67" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S67">
         <v>3</v>
@@ -5906,16 +6046,20 @@
       <c r="M68" s="2">
         <v>1</v>
       </c>
-      <c r="N68" s="8"/>
+      <c r="N68" s="10" t="s">
+        <v>266</v>
+      </c>
       <c r="O68" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="P68" s="8"/>
+        <v>266</v>
+      </c>
+      <c r="P68" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q68" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R68" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S68">
         <v>3</v>
@@ -5970,16 +6114,20 @@
       <c r="M69" s="2">
         <v>1</v>
       </c>
-      <c r="N69" s="8"/>
+      <c r="N69" s="10" t="s">
+        <v>262</v>
+      </c>
       <c r="O69" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="P69" s="8"/>
+        <v>262</v>
+      </c>
+      <c r="P69" s="10" t="s">
+        <v>263</v>
+      </c>
       <c r="Q69" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="R69" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S69">
         <v>3</v>
@@ -6034,16 +6182,20 @@
       <c r="M70" s="2">
         <v>1</v>
       </c>
-      <c r="N70" s="8"/>
+      <c r="N70" s="10" t="s">
+        <v>264</v>
+      </c>
       <c r="O70" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="P70" s="8"/>
+        <v>264</v>
+      </c>
+      <c r="P70" s="10" t="s">
+        <v>265</v>
+      </c>
       <c r="Q70" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="R70" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S70">
         <v>3</v>
@@ -6098,16 +6250,20 @@
       <c r="M71" s="2">
         <v>1</v>
       </c>
-      <c r="N71" s="8"/>
+      <c r="N71" s="10" t="s">
+        <v>266</v>
+      </c>
       <c r="O71" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="P71" s="8"/>
+        <v>266</v>
+      </c>
+      <c r="P71" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q71" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R71" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S71">
         <v>3</v>
@@ -6162,16 +6318,20 @@
       <c r="M72" s="2">
         <v>1</v>
       </c>
-      <c r="N72" s="8"/>
+      <c r="N72" s="10" t="s">
+        <v>262</v>
+      </c>
       <c r="O72" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="P72" s="8"/>
+        <v>262</v>
+      </c>
+      <c r="P72" s="10" t="s">
+        <v>263</v>
+      </c>
       <c r="Q72" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="R72" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S72">
         <v>3</v>
@@ -6226,16 +6386,20 @@
       <c r="M73" s="2">
         <v>1</v>
       </c>
-      <c r="N73" s="8"/>
+      <c r="N73" s="10" t="s">
+        <v>264</v>
+      </c>
       <c r="O73" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="P73" s="8"/>
+        <v>264</v>
+      </c>
+      <c r="P73" s="10" t="s">
+        <v>265</v>
+      </c>
       <c r="Q73" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="R73" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S73">
         <v>3</v>
@@ -6290,16 +6454,20 @@
       <c r="M74" s="2">
         <v>1</v>
       </c>
-      <c r="N74" s="8"/>
+      <c r="N74" s="10" t="s">
+        <v>266</v>
+      </c>
       <c r="O74" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="P74" s="8"/>
+        <v>266</v>
+      </c>
+      <c r="P74" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q74" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R74" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S74">
         <v>3</v>
@@ -6354,16 +6522,20 @@
       <c r="M75" s="2">
         <v>1</v>
       </c>
-      <c r="N75" s="8"/>
+      <c r="N75" s="10" t="s">
+        <v>262</v>
+      </c>
       <c r="O75" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="P75" s="8"/>
+        <v>262</v>
+      </c>
+      <c r="P75" s="10" t="s">
+        <v>263</v>
+      </c>
       <c r="Q75" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="R75" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S75">
         <v>3</v>
@@ -6418,16 +6590,20 @@
       <c r="M76" s="2">
         <v>1</v>
       </c>
-      <c r="N76" s="8"/>
+      <c r="N76" s="10" t="s">
+        <v>264</v>
+      </c>
       <c r="O76" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="P76" s="8"/>
+        <v>264</v>
+      </c>
+      <c r="P76" s="10" t="s">
+        <v>265</v>
+      </c>
       <c r="Q76" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="R76" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S76">
         <v>3</v>
@@ -6482,16 +6658,20 @@
       <c r="M77" s="2">
         <v>1</v>
       </c>
-      <c r="N77" s="8"/>
+      <c r="N77" s="10" t="s">
+        <v>266</v>
+      </c>
       <c r="O77" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="P77" s="8"/>
+        <v>266</v>
+      </c>
+      <c r="P77" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q77" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R77" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S77">
         <v>3</v>
@@ -6546,16 +6726,20 @@
       <c r="M78" s="2">
         <v>1</v>
       </c>
-      <c r="N78" s="8"/>
+      <c r="N78" s="10" t="s">
+        <v>262</v>
+      </c>
       <c r="O78" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="P78" s="8"/>
+        <v>262</v>
+      </c>
+      <c r="P78" s="10" t="s">
+        <v>263</v>
+      </c>
       <c r="Q78" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="R78" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S78">
         <v>3</v>
@@ -6610,16 +6794,20 @@
       <c r="M79" s="2">
         <v>1</v>
       </c>
-      <c r="N79" s="8"/>
+      <c r="N79" s="10" t="s">
+        <v>264</v>
+      </c>
       <c r="O79" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="P79" s="8"/>
+        <v>264</v>
+      </c>
+      <c r="P79" s="10" t="s">
+        <v>265</v>
+      </c>
       <c r="Q79" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="R79" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S79">
         <v>3</v>
@@ -6674,16 +6862,20 @@
       <c r="M80" s="2">
         <v>1</v>
       </c>
-      <c r="N80" s="8"/>
+      <c r="N80" s="10" t="s">
+        <v>266</v>
+      </c>
       <c r="O80" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="P80" s="8"/>
+        <v>266</v>
+      </c>
+      <c r="P80" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q80" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R80" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S80">
         <v>3</v>
@@ -6738,16 +6930,20 @@
       <c r="M81" s="2">
         <v>1</v>
       </c>
-      <c r="N81" s="8"/>
+      <c r="N81" s="10" t="s">
+        <v>268</v>
+      </c>
       <c r="O81" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="P81" s="8"/>
+        <v>268</v>
+      </c>
+      <c r="P81" s="10" t="s">
+        <v>269</v>
+      </c>
       <c r="Q81" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="R81" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S81">
         <v>4</v>
@@ -6802,16 +6998,20 @@
       <c r="M82" s="2">
         <v>1</v>
       </c>
-      <c r="N82" s="8"/>
+      <c r="N82" s="10" t="s">
+        <v>270</v>
+      </c>
       <c r="O82" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="P82" s="8"/>
+        <v>270</v>
+      </c>
+      <c r="P82" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="Q82" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="R82" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S82">
         <v>4</v>
@@ -6866,16 +7066,20 @@
       <c r="M83" s="2">
         <v>1</v>
       </c>
-      <c r="N83" s="8"/>
+      <c r="N83" s="10" t="s">
+        <v>272</v>
+      </c>
       <c r="O83" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="P83" s="8"/>
+        <v>272</v>
+      </c>
+      <c r="P83" s="10" t="s">
+        <v>273</v>
+      </c>
       <c r="Q83" s="10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="R83" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S83">
         <v>4</v>
@@ -6930,16 +7134,20 @@
       <c r="M84" s="2">
         <v>1</v>
       </c>
-      <c r="N84" s="8"/>
+      <c r="N84" s="10" t="s">
+        <v>268</v>
+      </c>
       <c r="O84" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="P84" s="8"/>
+        <v>268</v>
+      </c>
+      <c r="P84" s="10" t="s">
+        <v>269</v>
+      </c>
       <c r="Q84" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="R84" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S84">
         <v>4</v>
@@ -6994,16 +7202,20 @@
       <c r="M85" s="2">
         <v>1</v>
       </c>
-      <c r="N85" s="8"/>
+      <c r="N85" s="10" t="s">
+        <v>270</v>
+      </c>
       <c r="O85" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="P85" s="8"/>
+        <v>270</v>
+      </c>
+      <c r="P85" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="Q85" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="R85" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S85">
         <v>4</v>
@@ -7058,16 +7270,20 @@
       <c r="M86" s="2">
         <v>1</v>
       </c>
-      <c r="N86" s="8"/>
+      <c r="N86" s="10" t="s">
+        <v>272</v>
+      </c>
       <c r="O86" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="P86" s="8"/>
+        <v>272</v>
+      </c>
+      <c r="P86" s="10" t="s">
+        <v>273</v>
+      </c>
       <c r="Q86" s="10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="R86" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S86">
         <v>4</v>
@@ -7122,16 +7338,20 @@
       <c r="M87" s="2">
         <v>1</v>
       </c>
-      <c r="N87" s="8"/>
+      <c r="N87" s="10" t="s">
+        <v>268</v>
+      </c>
       <c r="O87" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="P87" s="8"/>
+        <v>268</v>
+      </c>
+      <c r="P87" s="10" t="s">
+        <v>269</v>
+      </c>
       <c r="Q87" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="R87" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S87">
         <v>4</v>
@@ -7186,16 +7406,20 @@
       <c r="M88" s="2">
         <v>1</v>
       </c>
-      <c r="N88" s="8"/>
+      <c r="N88" s="10" t="s">
+        <v>270</v>
+      </c>
       <c r="O88" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="P88" s="8"/>
+        <v>270</v>
+      </c>
+      <c r="P88" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="Q88" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="R88" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S88">
         <v>4</v>
@@ -7250,16 +7474,20 @@
       <c r="M89" s="2">
         <v>1</v>
       </c>
-      <c r="N89" s="8"/>
+      <c r="N89" s="10" t="s">
+        <v>272</v>
+      </c>
       <c r="O89" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="P89" s="8"/>
+        <v>272</v>
+      </c>
+      <c r="P89" s="10" t="s">
+        <v>273</v>
+      </c>
       <c r="Q89" s="10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="R89" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S89">
         <v>4</v>
@@ -7314,16 +7542,20 @@
       <c r="M90" s="2">
         <v>1</v>
       </c>
-      <c r="N90" s="8"/>
+      <c r="N90" s="10" t="s">
+        <v>268</v>
+      </c>
       <c r="O90" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="P90" s="8"/>
+        <v>268</v>
+      </c>
+      <c r="P90" s="10" t="s">
+        <v>269</v>
+      </c>
       <c r="Q90" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="R90" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S90">
         <v>4</v>
@@ -7378,16 +7610,20 @@
       <c r="M91" s="2">
         <v>1</v>
       </c>
-      <c r="N91" s="8"/>
+      <c r="N91" s="10" t="s">
+        <v>270</v>
+      </c>
       <c r="O91" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="P91" s="8"/>
+        <v>270</v>
+      </c>
+      <c r="P91" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="Q91" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="R91" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S91">
         <v>4</v>
@@ -7442,16 +7678,20 @@
       <c r="M92" s="2">
         <v>1</v>
       </c>
-      <c r="N92" s="8"/>
+      <c r="N92" s="10" t="s">
+        <v>272</v>
+      </c>
       <c r="O92" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="P92" s="8"/>
+        <v>272</v>
+      </c>
+      <c r="P92" s="10" t="s">
+        <v>273</v>
+      </c>
       <c r="Q92" s="10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="R92" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S92">
         <v>4</v>
@@ -7506,16 +7746,20 @@
       <c r="M93" s="2">
         <v>1</v>
       </c>
-      <c r="N93" s="8"/>
+      <c r="N93" s="10" t="s">
+        <v>268</v>
+      </c>
       <c r="O93" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="P93" s="8"/>
+        <v>268</v>
+      </c>
+      <c r="P93" s="10" t="s">
+        <v>269</v>
+      </c>
       <c r="Q93" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="R93" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S93">
         <v>4</v>
@@ -7570,16 +7814,20 @@
       <c r="M94" s="2">
         <v>1</v>
       </c>
-      <c r="N94" s="8"/>
+      <c r="N94" s="10" t="s">
+        <v>270</v>
+      </c>
       <c r="O94" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="P94" s="8"/>
+        <v>270</v>
+      </c>
+      <c r="P94" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="Q94" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="R94" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S94">
         <v>4</v>
@@ -7634,16 +7882,20 @@
       <c r="M95" s="2">
         <v>1</v>
       </c>
-      <c r="N95" s="8"/>
+      <c r="N95" s="10" t="s">
+        <v>272</v>
+      </c>
       <c r="O95" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="P95" s="8"/>
+        <v>272</v>
+      </c>
+      <c r="P95" s="10" t="s">
+        <v>273</v>
+      </c>
       <c r="Q95" s="10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="R95" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S95">
         <v>4</v>
@@ -7698,16 +7950,20 @@
       <c r="M96" s="2">
         <v>1</v>
       </c>
-      <c r="N96" s="8"/>
+      <c r="N96" s="10" t="s">
+        <v>268</v>
+      </c>
       <c r="O96" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="P96" s="8"/>
+        <v>268</v>
+      </c>
+      <c r="P96" s="10" t="s">
+        <v>269</v>
+      </c>
       <c r="Q96" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="R96" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S96">
         <v>4</v>
@@ -7762,16 +8018,20 @@
       <c r="M97" s="2">
         <v>1</v>
       </c>
-      <c r="N97" s="8"/>
+      <c r="N97" s="10" t="s">
+        <v>270</v>
+      </c>
       <c r="O97" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="P97" s="8"/>
+        <v>270</v>
+      </c>
+      <c r="P97" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="Q97" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="R97" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S97">
         <v>4</v>
@@ -7826,16 +8086,20 @@
       <c r="M98" s="2">
         <v>1</v>
       </c>
-      <c r="N98" s="8"/>
+      <c r="N98" s="10" t="s">
+        <v>272</v>
+      </c>
       <c r="O98" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="P98" s="8"/>
+        <v>272</v>
+      </c>
+      <c r="P98" s="10" t="s">
+        <v>273</v>
+      </c>
       <c r="Q98" s="10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="R98" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S98">
         <v>4</v>
@@ -7890,16 +8154,20 @@
       <c r="M99" s="2">
         <v>1</v>
       </c>
-      <c r="N99" s="8"/>
+      <c r="N99" s="10" t="s">
+        <v>268</v>
+      </c>
       <c r="O99" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="P99" s="8"/>
+        <v>268</v>
+      </c>
+      <c r="P99" s="10" t="s">
+        <v>269</v>
+      </c>
       <c r="Q99" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="R99" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S99">
         <v>4</v>
@@ -7954,16 +8222,20 @@
       <c r="M100" s="2">
         <v>1</v>
       </c>
-      <c r="N100" s="8"/>
+      <c r="N100" s="10" t="s">
+        <v>270</v>
+      </c>
       <c r="O100" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="P100" s="8"/>
+        <v>270</v>
+      </c>
+      <c r="P100" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="Q100" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="R100" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S100">
         <v>4</v>
@@ -8018,16 +8290,20 @@
       <c r="M101" s="2">
         <v>1</v>
       </c>
-      <c r="N101" s="8"/>
+      <c r="N101" s="10" t="s">
+        <v>272</v>
+      </c>
       <c r="O101" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="P101" s="8"/>
+        <v>272</v>
+      </c>
+      <c r="P101" s="10" t="s">
+        <v>273</v>
+      </c>
       <c r="Q101" s="10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="R101" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S101">
         <v>4</v>
@@ -8082,16 +8358,20 @@
       <c r="M102" s="2">
         <v>1</v>
       </c>
-      <c r="N102" s="8"/>
+      <c r="N102" s="10" t="s">
+        <v>268</v>
+      </c>
       <c r="O102" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="P102" s="8"/>
+        <v>268</v>
+      </c>
+      <c r="P102" s="10" t="s">
+        <v>269</v>
+      </c>
       <c r="Q102" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="R102" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S102">
         <v>4</v>
@@ -8146,16 +8426,20 @@
       <c r="M103" s="2">
         <v>1</v>
       </c>
-      <c r="N103" s="8"/>
+      <c r="N103" s="10" t="s">
+        <v>270</v>
+      </c>
       <c r="O103" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="P103" s="8"/>
+        <v>270</v>
+      </c>
+      <c r="P103" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="Q103" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="R103" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S103">
         <v>4</v>
@@ -8210,16 +8494,20 @@
       <c r="M104" s="2">
         <v>1</v>
       </c>
-      <c r="N104" s="8"/>
+      <c r="N104" s="10" t="s">
+        <v>272</v>
+      </c>
       <c r="O104" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="P104" s="8"/>
+        <v>272</v>
+      </c>
+      <c r="P104" s="10" t="s">
+        <v>273</v>
+      </c>
       <c r="Q104" s="10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="R104" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S104">
         <v>4</v>
@@ -8274,16 +8562,20 @@
       <c r="M105" s="2">
         <v>1</v>
       </c>
-      <c r="N105" s="8"/>
+      <c r="N105" s="10" t="s">
+        <v>268</v>
+      </c>
       <c r="O105" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="P105" s="8"/>
+        <v>268</v>
+      </c>
+      <c r="P105" s="10" t="s">
+        <v>269</v>
+      </c>
       <c r="Q105" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="R105" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S105">
         <v>4</v>
@@ -8338,16 +8630,20 @@
       <c r="M106" s="2">
         <v>1</v>
       </c>
-      <c r="N106" s="8"/>
+      <c r="N106" s="10" t="s">
+        <v>270</v>
+      </c>
       <c r="O106" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="P106" s="8"/>
+        <v>270</v>
+      </c>
+      <c r="P106" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="Q106" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="R106" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S106">
         <v>4</v>
@@ -8402,16 +8698,20 @@
       <c r="M107" s="2">
         <v>1</v>
       </c>
-      <c r="N107" s="8"/>
+      <c r="N107" s="10" t="s">
+        <v>272</v>
+      </c>
       <c r="O107" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="P107" s="8"/>
+        <v>272</v>
+      </c>
+      <c r="P107" s="10" t="s">
+        <v>273</v>
+      </c>
       <c r="Q107" s="10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="R107" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S107">
         <v>4</v>
@@ -8466,16 +8766,20 @@
       <c r="M108" s="2">
         <v>1</v>
       </c>
-      <c r="N108" s="8"/>
+      <c r="N108" s="10" t="s">
+        <v>268</v>
+      </c>
       <c r="O108" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="P108" s="8"/>
+        <v>268</v>
+      </c>
+      <c r="P108" s="10" t="s">
+        <v>269</v>
+      </c>
       <c r="Q108" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="R108" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S108">
         <v>4</v>
@@ -8530,16 +8834,20 @@
       <c r="M109" s="2">
         <v>1</v>
       </c>
-      <c r="N109" s="8"/>
+      <c r="N109" s="10" t="s">
+        <v>270</v>
+      </c>
       <c r="O109" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="P109" s="8"/>
+        <v>270</v>
+      </c>
+      <c r="P109" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="Q109" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="R109" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S109">
         <v>4</v>
@@ -8594,16 +8902,20 @@
       <c r="M110" s="2">
         <v>1</v>
       </c>
-      <c r="N110" s="8"/>
+      <c r="N110" s="10" t="s">
+        <v>272</v>
+      </c>
       <c r="O110" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="P110" s="8"/>
+        <v>272</v>
+      </c>
+      <c r="P110" s="10" t="s">
+        <v>273</v>
+      </c>
       <c r="Q110" s="10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="R110" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S110">
         <v>4</v>
@@ -8658,16 +8970,20 @@
       <c r="M111" s="2">
         <v>1</v>
       </c>
-      <c r="N111" s="8"/>
+      <c r="N111" s="10" t="s">
+        <v>274</v>
+      </c>
       <c r="O111" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="P111" s="8"/>
+        <v>274</v>
+      </c>
+      <c r="P111" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q111" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R111" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S111">
         <v>5</v>
@@ -8722,16 +9038,20 @@
       <c r="M112" s="2">
         <v>1</v>
       </c>
-      <c r="N112" s="8"/>
+      <c r="N112" s="10" t="s">
+        <v>275</v>
+      </c>
       <c r="O112" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="P112" s="8"/>
+        <v>275</v>
+      </c>
+      <c r="P112" s="10" t="s">
+        <v>276</v>
+      </c>
       <c r="Q112" s="10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="R112" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S112">
         <v>5</v>
@@ -8786,16 +9106,20 @@
       <c r="M113" s="2">
         <v>1</v>
       </c>
-      <c r="N113" s="8"/>
+      <c r="N113" s="10" t="s">
+        <v>277</v>
+      </c>
       <c r="O113" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="P113" s="8"/>
+        <v>277</v>
+      </c>
+      <c r="P113" s="10" t="s">
+        <v>278</v>
+      </c>
       <c r="Q113" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="R113" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S113">
         <v>5</v>
@@ -8850,16 +9174,20 @@
       <c r="M114" s="2">
         <v>1</v>
       </c>
-      <c r="N114" s="8"/>
+      <c r="N114" s="10" t="s">
+        <v>274</v>
+      </c>
       <c r="O114" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="P114" s="8"/>
+        <v>274</v>
+      </c>
+      <c r="P114" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q114" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R114" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S114">
         <v>5</v>
@@ -8914,16 +9242,20 @@
       <c r="M115" s="2">
         <v>1</v>
       </c>
-      <c r="N115" s="8"/>
+      <c r="N115" s="10" t="s">
+        <v>275</v>
+      </c>
       <c r="O115" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="P115" s="8"/>
+        <v>275</v>
+      </c>
+      <c r="P115" s="10" t="s">
+        <v>276</v>
+      </c>
       <c r="Q115" s="10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="R115" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S115">
         <v>5</v>
@@ -8978,16 +9310,20 @@
       <c r="M116" s="2">
         <v>1</v>
       </c>
-      <c r="N116" s="8"/>
+      <c r="N116" s="10" t="s">
+        <v>277</v>
+      </c>
       <c r="O116" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="P116" s="8"/>
+        <v>277</v>
+      </c>
+      <c r="P116" s="10" t="s">
+        <v>278</v>
+      </c>
       <c r="Q116" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="R116" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S116">
         <v>5</v>
@@ -9042,16 +9378,20 @@
       <c r="M117" s="2">
         <v>1</v>
       </c>
-      <c r="N117" s="8"/>
+      <c r="N117" s="10" t="s">
+        <v>274</v>
+      </c>
       <c r="O117" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="P117" s="8"/>
+        <v>274</v>
+      </c>
+      <c r="P117" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q117" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R117" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S117">
         <v>5</v>
@@ -9106,16 +9446,20 @@
       <c r="M118" s="2">
         <v>1</v>
       </c>
-      <c r="N118" s="8"/>
+      <c r="N118" s="10" t="s">
+        <v>275</v>
+      </c>
       <c r="O118" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="P118" s="8"/>
+        <v>275</v>
+      </c>
+      <c r="P118" s="10" t="s">
+        <v>276</v>
+      </c>
       <c r="Q118" s="10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="R118" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S118">
         <v>5</v>
@@ -9170,16 +9514,20 @@
       <c r="M119" s="2">
         <v>1</v>
       </c>
-      <c r="N119" s="8"/>
+      <c r="N119" s="10" t="s">
+        <v>277</v>
+      </c>
       <c r="O119" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="P119" s="8"/>
+        <v>277</v>
+      </c>
+      <c r="P119" s="10" t="s">
+        <v>278</v>
+      </c>
       <c r="Q119" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="R119" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S119">
         <v>5</v>
@@ -9234,16 +9582,20 @@
       <c r="M120" s="2">
         <v>1</v>
       </c>
-      <c r="N120" s="8"/>
+      <c r="N120" s="10" t="s">
+        <v>274</v>
+      </c>
       <c r="O120" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="P120" s="8"/>
+        <v>274</v>
+      </c>
+      <c r="P120" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q120" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R120" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S120">
         <v>5</v>
@@ -9298,16 +9650,20 @@
       <c r="M121" s="2">
         <v>1</v>
       </c>
-      <c r="N121" s="8"/>
+      <c r="N121" s="10" t="s">
+        <v>275</v>
+      </c>
       <c r="O121" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="P121" s="8"/>
+        <v>275</v>
+      </c>
+      <c r="P121" s="10" t="s">
+        <v>276</v>
+      </c>
       <c r="Q121" s="10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="R121" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S121">
         <v>5</v>
@@ -9362,16 +9718,20 @@
       <c r="M122" s="2">
         <v>1</v>
       </c>
-      <c r="N122" s="8"/>
+      <c r="N122" s="10" t="s">
+        <v>277</v>
+      </c>
       <c r="O122" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="P122" s="8"/>
+        <v>277</v>
+      </c>
+      <c r="P122" s="10" t="s">
+        <v>278</v>
+      </c>
       <c r="Q122" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="R122" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S122">
         <v>5</v>
@@ -9426,16 +9786,20 @@
       <c r="M123" s="2">
         <v>1</v>
       </c>
-      <c r="N123" s="8"/>
+      <c r="N123" s="10" t="s">
+        <v>274</v>
+      </c>
       <c r="O123" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="P123" s="8"/>
+        <v>274</v>
+      </c>
+      <c r="P123" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q123" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R123" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S123">
         <v>5</v>
@@ -9490,16 +9854,20 @@
       <c r="M124" s="2">
         <v>1</v>
       </c>
-      <c r="N124" s="8"/>
+      <c r="N124" s="10" t="s">
+        <v>275</v>
+      </c>
       <c r="O124" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="P124" s="8"/>
+        <v>275</v>
+      </c>
+      <c r="P124" s="10" t="s">
+        <v>276</v>
+      </c>
       <c r="Q124" s="10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="R124" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S124">
         <v>5</v>
@@ -9554,16 +9922,20 @@
       <c r="M125" s="2">
         <v>1</v>
       </c>
-      <c r="N125" s="8"/>
+      <c r="N125" s="10" t="s">
+        <v>277</v>
+      </c>
       <c r="O125" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="P125" s="8"/>
+        <v>277</v>
+      </c>
+      <c r="P125" s="10" t="s">
+        <v>278</v>
+      </c>
       <c r="Q125" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="R125" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S125">
         <v>5</v>
@@ -9618,16 +9990,20 @@
       <c r="M126" s="2">
         <v>1</v>
       </c>
-      <c r="N126" s="8"/>
+      <c r="N126" s="10" t="s">
+        <v>274</v>
+      </c>
       <c r="O126" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="P126" s="8"/>
+        <v>274</v>
+      </c>
+      <c r="P126" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q126" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R126" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S126">
         <v>5</v>
@@ -9682,16 +10058,20 @@
       <c r="M127" s="2">
         <v>1</v>
       </c>
-      <c r="N127" s="8"/>
+      <c r="N127" s="10" t="s">
+        <v>275</v>
+      </c>
       <c r="O127" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="P127" s="8"/>
+        <v>275</v>
+      </c>
+      <c r="P127" s="10" t="s">
+        <v>276</v>
+      </c>
       <c r="Q127" s="10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="R127" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S127">
         <v>5</v>
@@ -9746,16 +10126,20 @@
       <c r="M128" s="2">
         <v>1</v>
       </c>
-      <c r="N128" s="8"/>
+      <c r="N128" s="10" t="s">
+        <v>277</v>
+      </c>
       <c r="O128" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="P128" s="8"/>
+        <v>277</v>
+      </c>
+      <c r="P128" s="10" t="s">
+        <v>278</v>
+      </c>
       <c r="Q128" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="R128" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S128">
         <v>5</v>
@@ -9810,16 +10194,20 @@
       <c r="M129" s="2">
         <v>1</v>
       </c>
-      <c r="N129" s="8"/>
+      <c r="N129" s="10" t="s">
+        <v>274</v>
+      </c>
       <c r="O129" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="P129" s="8"/>
+        <v>274</v>
+      </c>
+      <c r="P129" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q129" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R129" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S129">
         <v>5</v>
@@ -9874,16 +10262,20 @@
       <c r="M130" s="2">
         <v>1</v>
       </c>
-      <c r="N130" s="8"/>
+      <c r="N130" s="10" t="s">
+        <v>275</v>
+      </c>
       <c r="O130" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="P130" s="8"/>
+        <v>275</v>
+      </c>
+      <c r="P130" s="10" t="s">
+        <v>276</v>
+      </c>
       <c r="Q130" s="10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="R130" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S130">
         <v>5</v>
@@ -9938,16 +10330,20 @@
       <c r="M131" s="2">
         <v>1</v>
       </c>
-      <c r="N131" s="8"/>
+      <c r="N131" s="10" t="s">
+        <v>277</v>
+      </c>
       <c r="O131" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="P131" s="8"/>
+        <v>277</v>
+      </c>
+      <c r="P131" s="10" t="s">
+        <v>278</v>
+      </c>
       <c r="Q131" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="R131" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S131">
         <v>5</v>
@@ -10002,16 +10398,20 @@
       <c r="M132" s="2">
         <v>1</v>
       </c>
-      <c r="N132" s="8"/>
+      <c r="N132" s="10" t="s">
+        <v>274</v>
+      </c>
       <c r="O132" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="P132" s="8"/>
+        <v>274</v>
+      </c>
+      <c r="P132" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q132" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R132" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S132">
         <v>5</v>
@@ -10066,16 +10466,20 @@
       <c r="M133" s="2">
         <v>1</v>
       </c>
-      <c r="N133" s="8"/>
+      <c r="N133" s="10" t="s">
+        <v>275</v>
+      </c>
       <c r="O133" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="P133" s="8"/>
+        <v>275</v>
+      </c>
+      <c r="P133" s="10" t="s">
+        <v>276</v>
+      </c>
       <c r="Q133" s="10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="R133" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S133">
         <v>5</v>
@@ -10130,16 +10534,20 @@
       <c r="M134" s="2">
         <v>1</v>
       </c>
-      <c r="N134" s="8"/>
+      <c r="N134" s="10" t="s">
+        <v>277</v>
+      </c>
       <c r="O134" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="P134" s="8"/>
+        <v>277</v>
+      </c>
+      <c r="P134" s="10" t="s">
+        <v>278</v>
+      </c>
       <c r="Q134" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="R134" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S134">
         <v>5</v>
@@ -10194,16 +10602,20 @@
       <c r="M135" s="2">
         <v>1</v>
       </c>
-      <c r="N135" s="8"/>
+      <c r="N135" s="10" t="s">
+        <v>274</v>
+      </c>
       <c r="O135" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="P135" s="8"/>
+        <v>274</v>
+      </c>
+      <c r="P135" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q135" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R135" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S135">
         <v>5</v>
@@ -10258,16 +10670,20 @@
       <c r="M136" s="2">
         <v>1</v>
       </c>
-      <c r="N136" s="8"/>
+      <c r="N136" s="10" t="s">
+        <v>275</v>
+      </c>
       <c r="O136" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="P136" s="8"/>
+        <v>275</v>
+      </c>
+      <c r="P136" s="10" t="s">
+        <v>276</v>
+      </c>
       <c r="Q136" s="10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="R136" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S136">
         <v>5</v>
@@ -10322,16 +10738,20 @@
       <c r="M137" s="2">
         <v>1</v>
       </c>
-      <c r="N137" s="8"/>
+      <c r="N137" s="10" t="s">
+        <v>277</v>
+      </c>
       <c r="O137" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="P137" s="8"/>
+        <v>277</v>
+      </c>
+      <c r="P137" s="10" t="s">
+        <v>278</v>
+      </c>
       <c r="Q137" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="R137" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S137">
         <v>5</v>
@@ -10386,16 +10806,20 @@
       <c r="M138" s="2">
         <v>1</v>
       </c>
-      <c r="N138" s="8"/>
+      <c r="N138" s="10" t="s">
+        <v>274</v>
+      </c>
       <c r="O138" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="P138" s="8"/>
+        <v>274</v>
+      </c>
+      <c r="P138" s="10" t="s">
+        <v>267</v>
+      </c>
       <c r="Q138" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R138" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S138">
         <v>5</v>
@@ -10450,16 +10874,20 @@
       <c r="M139" s="2">
         <v>1</v>
       </c>
-      <c r="N139" s="8"/>
+      <c r="N139" s="10" t="s">
+        <v>275</v>
+      </c>
       <c r="O139" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="P139" s="8"/>
+        <v>275</v>
+      </c>
+      <c r="P139" s="10" t="s">
+        <v>276</v>
+      </c>
       <c r="Q139" s="10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="R139" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S139">
         <v>5</v>
@@ -10514,16 +10942,20 @@
       <c r="M140" s="2">
         <v>1</v>
       </c>
-      <c r="N140" s="8"/>
+      <c r="N140" s="10" t="s">
+        <v>277</v>
+      </c>
       <c r="O140" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="P140" s="8"/>
+        <v>277</v>
+      </c>
+      <c r="P140" s="10" t="s">
+        <v>278</v>
+      </c>
       <c r="Q140" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="R140" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S140">
         <v>5</v>
@@ -10578,16 +11010,20 @@
       <c r="M141" s="2">
         <v>1</v>
       </c>
-      <c r="N141" s="8"/>
+      <c r="N141" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="O141" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="P141" s="8"/>
+        <v>279</v>
+      </c>
+      <c r="P141" s="10" t="s">
+        <v>280</v>
+      </c>
       <c r="Q141" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="R141" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S141">
         <v>6</v>
@@ -10642,16 +11078,20 @@
       <c r="M142" s="2">
         <v>1</v>
       </c>
-      <c r="N142" s="8"/>
+      <c r="N142" s="10" t="s">
+        <v>281</v>
+      </c>
       <c r="O142" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="P142" s="8"/>
+        <v>281</v>
+      </c>
+      <c r="P142" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="Q142" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="R142" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S142">
         <v>6</v>
@@ -10706,16 +11146,20 @@
       <c r="M143" s="2">
         <v>1</v>
       </c>
-      <c r="N143" s="8"/>
+      <c r="N143" s="10" t="s">
+        <v>283</v>
+      </c>
       <c r="O143" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="P143" s="8"/>
+        <v>283</v>
+      </c>
+      <c r="P143" s="10" t="s">
+        <v>284</v>
+      </c>
       <c r="Q143" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="R143" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S143">
         <v>6</v>
@@ -10770,16 +11214,20 @@
       <c r="M144" s="2">
         <v>1</v>
       </c>
-      <c r="N144" s="8"/>
+      <c r="N144" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="O144" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="P144" s="8"/>
+        <v>279</v>
+      </c>
+      <c r="P144" s="10" t="s">
+        <v>280</v>
+      </c>
       <c r="Q144" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="R144" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S144">
         <v>6</v>
@@ -10834,16 +11282,20 @@
       <c r="M145" s="2">
         <v>1</v>
       </c>
-      <c r="N145" s="8"/>
+      <c r="N145" s="10" t="s">
+        <v>281</v>
+      </c>
       <c r="O145" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="P145" s="8"/>
+        <v>281</v>
+      </c>
+      <c r="P145" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="Q145" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="R145" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S145">
         <v>6</v>
@@ -10898,16 +11350,20 @@
       <c r="M146" s="2">
         <v>1</v>
       </c>
-      <c r="N146" s="8"/>
+      <c r="N146" s="10" t="s">
+        <v>283</v>
+      </c>
       <c r="O146" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="P146" s="8"/>
+        <v>283</v>
+      </c>
+      <c r="P146" s="10" t="s">
+        <v>284</v>
+      </c>
       <c r="Q146" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="R146" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S146">
         <v>6</v>
@@ -10962,16 +11418,20 @@
       <c r="M147" s="2">
         <v>1</v>
       </c>
-      <c r="N147" s="8"/>
+      <c r="N147" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="O147" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="P147" s="8"/>
+        <v>279</v>
+      </c>
+      <c r="P147" s="10" t="s">
+        <v>280</v>
+      </c>
       <c r="Q147" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="R147" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S147">
         <v>6</v>
@@ -11026,16 +11486,20 @@
       <c r="M148" s="2">
         <v>1</v>
       </c>
-      <c r="N148" s="8"/>
+      <c r="N148" s="10" t="s">
+        <v>281</v>
+      </c>
       <c r="O148" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="P148" s="8"/>
+        <v>281</v>
+      </c>
+      <c r="P148" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="Q148" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="R148" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S148">
         <v>6</v>
@@ -11090,16 +11554,20 @@
       <c r="M149" s="2">
         <v>1</v>
       </c>
-      <c r="N149" s="8"/>
+      <c r="N149" s="10" t="s">
+        <v>283</v>
+      </c>
       <c r="O149" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="P149" s="8"/>
+        <v>283</v>
+      </c>
+      <c r="P149" s="10" t="s">
+        <v>284</v>
+      </c>
       <c r="Q149" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="R149" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S149">
         <v>6</v>
@@ -11154,16 +11622,20 @@
       <c r="M150" s="2">
         <v>1</v>
       </c>
-      <c r="N150" s="8"/>
+      <c r="N150" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="O150" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="P150" s="8"/>
+        <v>279</v>
+      </c>
+      <c r="P150" s="10" t="s">
+        <v>280</v>
+      </c>
       <c r="Q150" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="R150" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S150">
         <v>6</v>
@@ -11218,16 +11690,20 @@
       <c r="M151" s="2">
         <v>1</v>
       </c>
-      <c r="N151" s="8"/>
+      <c r="N151" s="10" t="s">
+        <v>281</v>
+      </c>
       <c r="O151" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="P151" s="8"/>
+        <v>281</v>
+      </c>
+      <c r="P151" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="Q151" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="R151" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S151">
         <v>6</v>
@@ -11282,16 +11758,20 @@
       <c r="M152" s="2">
         <v>1</v>
       </c>
-      <c r="N152" s="8"/>
+      <c r="N152" s="10" t="s">
+        <v>283</v>
+      </c>
       <c r="O152" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="P152" s="8"/>
+        <v>283</v>
+      </c>
+      <c r="P152" s="10" t="s">
+        <v>284</v>
+      </c>
       <c r="Q152" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="R152" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S152">
         <v>6</v>
@@ -11346,16 +11826,20 @@
       <c r="M153" s="2">
         <v>1</v>
       </c>
-      <c r="N153" s="8"/>
+      <c r="N153" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="O153" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="P153" s="8"/>
+        <v>279</v>
+      </c>
+      <c r="P153" s="10" t="s">
+        <v>280</v>
+      </c>
       <c r="Q153" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="R153" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S153">
         <v>6</v>
@@ -11410,16 +11894,20 @@
       <c r="M154" s="2">
         <v>1</v>
       </c>
-      <c r="N154" s="8"/>
+      <c r="N154" s="10" t="s">
+        <v>281</v>
+      </c>
       <c r="O154" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="P154" s="8"/>
+        <v>281</v>
+      </c>
+      <c r="P154" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="Q154" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="R154" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S154">
         <v>6</v>
@@ -11474,16 +11962,20 @@
       <c r="M155" s="2">
         <v>1</v>
       </c>
-      <c r="N155" s="8"/>
+      <c r="N155" s="10" t="s">
+        <v>283</v>
+      </c>
       <c r="O155" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="P155" s="8"/>
+        <v>283</v>
+      </c>
+      <c r="P155" s="10" t="s">
+        <v>284</v>
+      </c>
       <c r="Q155" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="R155" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S155">
         <v>6</v>
@@ -11538,16 +12030,20 @@
       <c r="M156" s="2">
         <v>1</v>
       </c>
-      <c r="N156" s="8"/>
+      <c r="N156" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="O156" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="P156" s="8"/>
+        <v>279</v>
+      </c>
+      <c r="P156" s="10" t="s">
+        <v>280</v>
+      </c>
       <c r="Q156" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="R156" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S156">
         <v>6</v>
@@ -11602,16 +12098,20 @@
       <c r="M157" s="2">
         <v>1</v>
       </c>
-      <c r="N157" s="8"/>
+      <c r="N157" s="10" t="s">
+        <v>281</v>
+      </c>
       <c r="O157" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="P157" s="8"/>
+        <v>281</v>
+      </c>
+      <c r="P157" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="Q157" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="R157" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S157">
         <v>6</v>
@@ -11666,16 +12166,20 @@
       <c r="M158" s="2">
         <v>1</v>
       </c>
-      <c r="N158" s="8"/>
+      <c r="N158" s="10" t="s">
+        <v>283</v>
+      </c>
       <c r="O158" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="P158" s="8"/>
+        <v>283</v>
+      </c>
+      <c r="P158" s="10" t="s">
+        <v>284</v>
+      </c>
       <c r="Q158" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="R158" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S158">
         <v>6</v>
@@ -11730,16 +12234,20 @@
       <c r="M159" s="2">
         <v>1</v>
       </c>
-      <c r="N159" s="8"/>
+      <c r="N159" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="O159" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="P159" s="8"/>
+        <v>279</v>
+      </c>
+      <c r="P159" s="10" t="s">
+        <v>280</v>
+      </c>
       <c r="Q159" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="R159" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S159">
         <v>6</v>
@@ -11794,16 +12302,20 @@
       <c r="M160" s="2">
         <v>1</v>
       </c>
-      <c r="N160" s="8"/>
+      <c r="N160" s="10" t="s">
+        <v>281</v>
+      </c>
       <c r="O160" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="P160" s="8"/>
+        <v>281</v>
+      </c>
+      <c r="P160" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="Q160" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="R160" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S160">
         <v>6</v>
@@ -11858,16 +12370,20 @@
       <c r="M161" s="2">
         <v>1</v>
       </c>
-      <c r="N161" s="8"/>
+      <c r="N161" s="10" t="s">
+        <v>283</v>
+      </c>
       <c r="O161" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="P161" s="8"/>
+        <v>283</v>
+      </c>
+      <c r="P161" s="10" t="s">
+        <v>284</v>
+      </c>
       <c r="Q161" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="R161" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S161">
         <v>6</v>
@@ -11922,16 +12438,20 @@
       <c r="M162" s="2">
         <v>1</v>
       </c>
-      <c r="N162" s="8"/>
+      <c r="N162" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="O162" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="P162" s="8"/>
+        <v>279</v>
+      </c>
+      <c r="P162" s="10" t="s">
+        <v>280</v>
+      </c>
       <c r="Q162" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="R162" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S162">
         <v>6</v>
@@ -11986,16 +12506,20 @@
       <c r="M163" s="2">
         <v>1</v>
       </c>
-      <c r="N163" s="8"/>
+      <c r="N163" s="10" t="s">
+        <v>281</v>
+      </c>
       <c r="O163" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="P163" s="8"/>
+        <v>281</v>
+      </c>
+      <c r="P163" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="Q163" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="R163" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S163">
         <v>6</v>
@@ -12050,16 +12574,20 @@
       <c r="M164" s="2">
         <v>1</v>
       </c>
-      <c r="N164" s="8"/>
+      <c r="N164" s="10" t="s">
+        <v>283</v>
+      </c>
       <c r="O164" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="P164" s="8"/>
+        <v>283</v>
+      </c>
+      <c r="P164" s="10" t="s">
+        <v>284</v>
+      </c>
       <c r="Q164" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="R164" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S164">
         <v>6</v>
@@ -12114,16 +12642,20 @@
       <c r="M165" s="2">
         <v>1</v>
       </c>
-      <c r="N165" s="8"/>
+      <c r="N165" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="O165" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="P165" s="8"/>
+        <v>279</v>
+      </c>
+      <c r="P165" s="10" t="s">
+        <v>280</v>
+      </c>
       <c r="Q165" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="R165" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S165">
         <v>6</v>
@@ -12178,16 +12710,20 @@
       <c r="M166" s="2">
         <v>1</v>
       </c>
-      <c r="N166" s="8"/>
+      <c r="N166" s="10" t="s">
+        <v>281</v>
+      </c>
       <c r="O166" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="P166" s="8"/>
+        <v>281</v>
+      </c>
+      <c r="P166" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="Q166" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="R166" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S166">
         <v>6</v>
@@ -12242,16 +12778,20 @@
       <c r="M167" s="2">
         <v>1</v>
       </c>
-      <c r="N167" s="8"/>
+      <c r="N167" s="10" t="s">
+        <v>283</v>
+      </c>
       <c r="O167" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="P167" s="8"/>
+        <v>283</v>
+      </c>
+      <c r="P167" s="10" t="s">
+        <v>284</v>
+      </c>
       <c r="Q167" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="R167" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S167">
         <v>6</v>
@@ -12306,16 +12846,20 @@
       <c r="M168" s="2">
         <v>1</v>
       </c>
-      <c r="N168" s="8"/>
+      <c r="N168" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="O168" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="P168" s="8"/>
+        <v>279</v>
+      </c>
+      <c r="P168" s="10" t="s">
+        <v>280</v>
+      </c>
       <c r="Q168" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="R168" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S168">
         <v>6</v>
@@ -12370,16 +12914,20 @@
       <c r="M169" s="2">
         <v>1</v>
       </c>
-      <c r="N169" s="8"/>
+      <c r="N169" s="10" t="s">
+        <v>281</v>
+      </c>
       <c r="O169" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="P169" s="8"/>
+        <v>281</v>
+      </c>
+      <c r="P169" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="Q169" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="R169" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S169">
         <v>6</v>
@@ -12434,16 +12982,20 @@
       <c r="M170" s="2">
         <v>1</v>
       </c>
-      <c r="N170" s="8"/>
+      <c r="N170" s="10" t="s">
+        <v>283</v>
+      </c>
       <c r="O170" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="P170" s="8"/>
+        <v>283</v>
+      </c>
+      <c r="P170" s="10" t="s">
+        <v>284</v>
+      </c>
       <c r="Q170" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="R170" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S170">
         <v>6</v>

</xml_diff>